<commit_message>
Update automatico via Actualizar 05-15-2020 01-04-46
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="379" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{051DD93C-A4C7-4BBA-9033-0D9F4411AAC1}"/>
+  <xr:revisionPtr revIDLastSave="386" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DB023D28-3272-4287-BBCE-ECA5C6C39044}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="0" windowWidth="15372" windowHeight="12960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>rrodriguez:</t>
         </r>
@@ -55,7 +55,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Región
@@ -524,10 +524,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="39" x14ac:knownFonts="1">
     <font>
@@ -738,33 +738,39 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF1F3864"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -789,13 +795,13 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="40">
@@ -1139,7 +1145,7 @@
   </borders>
   <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1185,7 +1191,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1203,16 +1209,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="19" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="19" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="35" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="35" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1264,23 +1270,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="18" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="18" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="18" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="35" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="35" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1298,7 +1304,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="18" fillId="36" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="36" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1314,7 +1320,7 @@
     <xf numFmtId="0" fontId="26" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="43"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="29" fillId="38" borderId="0" xfId="44" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="39" borderId="0" xfId="44" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="44"/>
@@ -1331,6 +1337,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="43" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Énfasis1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1411,7 +1418,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -1430,7 +1437,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -1494,7 +1501,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1516,7 +1523,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1561,7 +1568,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -1580,7 +1587,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -1644,7 +1651,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1675,7 +1682,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2224,7 +2231,7 @@
     <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="bottomLeft" activeCell="G10" activeCellId="1" sqref="A10 G10"/>
+      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3873,8 +3880,8 @@
   </sheetPr>
   <dimension ref="A1:R504"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11515,7 +11522,7 @@
   </sheetPr>
   <dimension ref="A1:R504"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
@@ -22275,19 +22282,20 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.88671875" style="95" customWidth="1"/>
-    <col min="2" max="3" width="11.109375" style="95" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" style="95" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="95" customWidth="1"/>
     <col min="4" max="4" width="27.44140625" style="95" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="95" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" style="95" customWidth="1"/>
+    <col min="5" max="5" width="47.44140625" style="95" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="95.5546875" style="95" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5546875" style="95" customWidth="1"/>
     <col min="8" max="9" width="17.6640625" style="95" customWidth="1"/>
     <col min="10" max="10" width="11.5546875" style="95" customWidth="1"/>
@@ -22563,7 +22571,7 @@
       <c r="E5" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="F5" s="104" t="s">
+      <c r="F5" s="107" t="s">
         <v>115</v>
       </c>
       <c r="G5" s="103" t="s">
@@ -22618,7 +22626,7 @@
       <c r="E6" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="104" t="s">
+      <c r="F6" s="107" t="s">
         <v>117</v>
       </c>
       <c r="G6" s="103" t="s">
@@ -22673,7 +22681,7 @@
       <c r="E7" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="104" t="s">
+      <c r="F7" s="107" t="s">
         <v>60</v>
       </c>
       <c r="G7" s="103" t="s">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-16-2020 19-09-55
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="397" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3DF20DED-E645-4726-9821-26C371381A78}"/>
+  <xr:revisionPtr revIDLastSave="400" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F4E63D52-9C3B-4E39-9CC7-1F94BCCD883F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -1365,14 +1365,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="38" borderId="0" xfId="44" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="39" borderId="0" xfId="44" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="44" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="44" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="38" borderId="0" xfId="44" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="39" borderId="0" xfId="44" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Énfasis1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1423,7 +1427,10 @@
     <cellStyle name="Título 3" xfId="5" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1792,9 +1799,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Hoja1-style" pivot="0" count="3" xr9:uid="{0CF0D513-1B31-4541-AD45-09363BE32DD6}">
-      <tableStyleElement type="headerRow" dxfId="23"/>
-      <tableStyleElement type="firstRowStripe" dxfId="22"/>
-      <tableStyleElement type="secondRowStripe" dxfId="21"/>
+      <tableStyleElement type="headerRow" dxfId="24"/>
+      <tableStyleElement type="firstRowStripe" dxfId="23"/>
+      <tableStyleElement type="secondRowStripe" dxfId="22"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1912,13 +1919,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H501" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H501" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="A3:H501" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Café" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Azúcar" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Café" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Azúcar" dataDxfId="17"/>
     <tableColumn id="6" xr3:uid="{1A412D0D-9DDD-4532-ADAC-BC90F0ABB038}" name="Combustible Súper"/>
     <tableColumn id="7" xr3:uid="{6C9802FB-03D0-4F94-9942-ED195CC86D50}" name="Combustible Regular"/>
     <tableColumn id="8" xr3:uid="{EBFE959D-24EF-495E-9BE7-BDEC4C8061F8}" name="Combustible Diesel"/>
@@ -1929,18 +1936,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R44" totalsRowShown="0" headerRowDxfId="15" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R44" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R44" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="13">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{8FC1825F-E2AC-4830-AA41-5B12F2C15972}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Monto Inversión (millones de lempiras)" dataDxfId="11" dataCellStyle="Millares"/>
+    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Monto Inversión (millones de lempiras)" dataDxfId="12" dataCellStyle="Millares"/>
     <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Solicitudes Crédito"/>
-    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Monto Crédito (millones de lempiras)" dataDxfId="10" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Monto Crédito (millones de lempiras)" dataDxfId="11" dataCellStyle="Millares"/>
     <tableColumn id="8" xr3:uid="{1A570E63-F800-45DF-9E5A-B8961BEFE222}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{7E984A16-0976-4747-9D31-12709D8A9C2E}" name="Ingesos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1949,10 +1956,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H501" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H501" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A3:H501" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
     <tableColumn id="3" xr3:uid="{47070387-916A-43EA-9250-BD5CD00DE202}" name="Precio Café"/>
     <tableColumn id="4" xr3:uid="{017F8C94-7948-49FE-B245-F576C80EC85B}" name="Precio Azúcar"/>
@@ -1966,18 +1973,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R44" totalsRowShown="0" headerRowDxfId="7" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R44" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R44" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="5">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{B7D1225A-C849-430C-8F2C-569D3B5E64AD}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="3" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="2" dataCellStyle="Millares [0]"/>
-    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="1" dataCellStyle="Millares [0]"/>
+    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="4" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="3" dataCellStyle="Millares [0]"/>
+    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="2" dataCellStyle="Millares [0]"/>
     <tableColumn id="8" xr3:uid="{552CA574-1C46-4E0F-8C54-8DBCDA6B12C1}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{C793523A-103E-4CA7-94B8-3E3D9A633FDB}" name="Ingresos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1986,7 +1993,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="0">
   <autoFilter ref="A1:U36" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -2009,7 +2016,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3866,26 +3873,26 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="106" t="s">
+      <c r="A78" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="107"/>
-      <c r="C78" s="107"/>
-      <c r="D78" s="107"/>
-      <c r="E78" s="107"/>
-      <c r="F78" s="107"/>
-      <c r="G78" s="107"/>
+      <c r="B78" s="105"/>
+      <c r="C78" s="105"/>
+      <c r="D78" s="105"/>
+      <c r="E78" s="105"/>
+      <c r="F78" s="105"/>
+      <c r="G78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="106" t="s">
+      <c r="A79" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="B79" s="107"/>
-      <c r="C79" s="107"/>
-      <c r="D79" s="107"/>
-      <c r="E79" s="107"/>
-      <c r="F79" s="107"/>
-      <c r="G79" s="107"/>
+      <c r="B79" s="105"/>
+      <c r="C79" s="105"/>
+      <c r="D79" s="105"/>
+      <c r="E79" s="105"/>
+      <c r="F79" s="105"/>
+      <c r="G79" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -11575,7 +11582,7 @@
   </sheetPr>
   <dimension ref="A1:R504"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A433" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E2" activeCellId="2" sqref="E3 H2 E2"/>
     </sheetView>
   </sheetViews>
@@ -25041,16 +25048,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB840748-361D-4458-B100-AAECA785CA65}">
   <dimension ref="A1:Y972"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" style="92" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="92" customWidth="1"/>
     <col min="2" max="2" width="31.77734375" style="92" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.109375" style="92" customWidth="1"/>
     <col min="4" max="4" width="27.44140625" style="92" customWidth="1"/>
@@ -25070,68 +25077,68 @@
     <col min="27" max="16384" width="14" style="92"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+    <row r="1" spans="1:25" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="106" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="D1" s="106" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="102" t="s">
+      <c r="E1" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="F1" s="107" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="107" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="H1" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="102" t="s">
+      <c r="I1" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="102" t="s">
+      <c r="J1" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="102" t="s">
+      <c r="K1" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="102" t="s">
+      <c r="L1" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="M1" s="102" t="s">
+      <c r="M1" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="102" t="s">
+      <c r="N1" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="102" t="s">
+      <c r="O1" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="P1" s="102" t="s">
+      <c r="P1" s="106" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" s="102" t="s">
+      <c r="Q1" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="R1" s="102" t="s">
+      <c r="R1" s="106" t="s">
         <v>83</v>
       </c>
-      <c r="S1" s="102" t="s">
+      <c r="S1" s="106" t="s">
         <v>84</v>
       </c>
-      <c r="T1" s="102" t="s">
+      <c r="T1" s="106" t="s">
         <v>85</v>
       </c>
-      <c r="U1" s="102" t="s">
+      <c r="U1" s="106" t="s">
         <v>86</v>
       </c>
       <c r="Y1" s="93" t="s">
@@ -25139,16 +25146,16 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="104">
+      <c r="A2" s="102">
         <v>5</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="103" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="105">
+      <c r="C2" s="103">
         <v>7</v>
       </c>
-      <c r="D2" s="105" t="s">
+      <c r="D2" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E2" s="94" t="s">
@@ -25163,7 +25170,7 @@
       <c r="H2" s="95" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="105" t="s">
+      <c r="I2" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J2" s="95" t="s">
@@ -25172,11 +25179,11 @@
       <c r="K2" s="95" t="s">
         <v>96</v>
       </c>
-      <c r="L2" s="105" t="s">
+      <c r="L2" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
       <c r="O2" s="96">
         <v>43964</v>
       </c>
@@ -25200,16 +25207,16 @@
       </c>
     </row>
     <row r="3" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="104">
+      <c r="A3" s="102">
         <v>5</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="103" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="105">
+      <c r="C3" s="103">
         <v>7</v>
       </c>
-      <c r="D3" s="105" t="s">
+      <c r="D3" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E3" s="94" t="s">
@@ -25224,7 +25231,7 @@
       <c r="H3" s="95" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="105" t="s">
+      <c r="I3" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J3" s="95" t="s">
@@ -25233,11 +25240,11 @@
       <c r="K3" s="95" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="105" t="s">
+      <c r="L3" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
       <c r="O3" s="96">
         <v>43964</v>
       </c>
@@ -25261,16 +25268,16 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="104">
+      <c r="A4" s="102">
         <v>5</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="103" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="105">
+      <c r="C4" s="103">
         <v>7</v>
       </c>
-      <c r="D4" s="105" t="s">
+      <c r="D4" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E4" s="94" t="s">
@@ -25285,7 +25292,7 @@
       <c r="H4" s="95" t="s">
         <v>94</v>
       </c>
-      <c r="I4" s="105" t="s">
+      <c r="I4" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J4" s="95" t="s">
@@ -25294,11 +25301,11 @@
       <c r="K4" s="95" t="s">
         <v>96</v>
       </c>
-      <c r="L4" s="105" t="s">
+      <c r="L4" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="103"/>
       <c r="O4" s="96">
         <v>43964</v>
       </c>
@@ -25322,16 +25329,16 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="104">
+      <c r="A5" s="102">
         <v>16</v>
       </c>
       <c r="B5" s="94" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="105">
+      <c r="C5" s="103">
         <v>7</v>
       </c>
-      <c r="D5" s="105" t="s">
+      <c r="D5" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E5" s="94" t="s">
@@ -25346,16 +25353,16 @@
       <c r="H5" s="95" t="s">
         <v>145</v>
       </c>
-      <c r="I5" s="105" t="s">
+      <c r="I5" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J5" s="95" t="s">
         <v>146</v>
       </c>
       <c r="K5" s="95"/>
-      <c r="L5" s="105"/>
-      <c r="M5" s="105"/>
-      <c r="N5" s="105"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="103"/>
       <c r="O5" s="96">
         <v>43964</v>
       </c>
@@ -25377,16 +25384,16 @@
       <c r="U5" s="97"/>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="104">
+      <c r="A6" s="102">
         <v>16</v>
       </c>
       <c r="B6" s="94" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="105">
+      <c r="C6" s="103">
         <v>7</v>
       </c>
-      <c r="D6" s="105" t="s">
+      <c r="D6" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E6" s="94" t="s">
@@ -25401,16 +25408,16 @@
       <c r="H6" s="95" t="s">
         <v>145</v>
       </c>
-      <c r="I6" s="105" t="s">
+      <c r="I6" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J6" s="95" t="s">
         <v>146</v>
       </c>
       <c r="K6" s="95"/>
-      <c r="L6" s="105"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="105"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="103"/>
       <c r="O6" s="96">
         <v>43964</v>
       </c>
@@ -25432,16 +25439,16 @@
       <c r="U6" s="97"/>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="104">
+      <c r="A7" s="102">
         <v>16</v>
       </c>
       <c r="B7" s="94" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="105">
+      <c r="C7" s="103">
         <v>7</v>
       </c>
-      <c r="D7" s="105" t="s">
+      <c r="D7" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E7" s="94" t="s">
@@ -25456,16 +25463,16 @@
       <c r="H7" s="95" t="s">
         <v>145</v>
       </c>
-      <c r="I7" s="105" t="s">
+      <c r="I7" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J7" s="95" t="s">
         <v>146</v>
       </c>
       <c r="K7" s="95"/>
-      <c r="L7" s="105"/>
-      <c r="M7" s="105"/>
-      <c r="N7" s="105"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
       <c r="O7" s="96">
         <v>43964</v>
       </c>
@@ -25487,16 +25494,16 @@
       <c r="U7" s="97"/>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="104">
+      <c r="A8" s="102">
         <v>16</v>
       </c>
       <c r="B8" s="94" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="105">
+      <c r="C8" s="103">
         <v>7</v>
       </c>
-      <c r="D8" s="105" t="s">
+      <c r="D8" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E8" s="94" t="s">
@@ -25511,16 +25518,16 @@
       <c r="H8" s="95" t="s">
         <v>145</v>
       </c>
-      <c r="I8" s="105" t="s">
+      <c r="I8" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J8" s="95" t="s">
         <v>146</v>
       </c>
       <c r="K8" s="95"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="105"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="103"/>
       <c r="O8" s="96">
         <v>43964</v>
       </c>
@@ -25542,16 +25549,16 @@
       <c r="U8" s="97"/>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="104">
+      <c r="A9" s="102">
         <v>5</v>
       </c>
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="103" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="105">
+      <c r="C9" s="103">
         <v>7</v>
       </c>
-      <c r="D9" s="105" t="s">
+      <c r="D9" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E9" s="94" t="s">
@@ -25566,7 +25573,7 @@
       <c r="H9" s="95" t="s">
         <v>94</v>
       </c>
-      <c r="I9" s="105" t="s">
+      <c r="I9" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J9" s="95" t="s">
@@ -25575,11 +25582,11 @@
       <c r="K9" s="95" t="s">
         <v>96</v>
       </c>
-      <c r="L9" s="105" t="s">
+      <c r="L9" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="M9" s="105"/>
-      <c r="N9" s="105"/>
+      <c r="M9" s="103"/>
+      <c r="N9" s="103"/>
       <c r="O9" s="96">
         <v>43964</v>
       </c>
@@ -25603,16 +25610,16 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="104">
+      <c r="A10" s="102">
         <v>5</v>
       </c>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="103" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="105">
+      <c r="C10" s="103">
         <v>7</v>
       </c>
-      <c r="D10" s="105" t="s">
+      <c r="D10" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E10" s="94" t="s">
@@ -25627,7 +25634,7 @@
       <c r="H10" s="95" t="s">
         <v>94</v>
       </c>
-      <c r="I10" s="105" t="s">
+      <c r="I10" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J10" s="95" t="s">
@@ -25636,11 +25643,11 @@
       <c r="K10" s="95" t="s">
         <v>96</v>
       </c>
-      <c r="L10" s="105" t="s">
+      <c r="L10" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="M10" s="105"/>
-      <c r="N10" s="105"/>
+      <c r="M10" s="103"/>
+      <c r="N10" s="103"/>
       <c r="O10" s="96">
         <v>43964</v>
       </c>
@@ -25664,16 +25671,16 @@
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="104">
+      <c r="A11" s="102">
         <v>17</v>
       </c>
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="103" t="s">
         <v>126</v>
       </c>
-      <c r="C11" s="105">
+      <c r="C11" s="103">
         <v>7</v>
       </c>
-      <c r="D11" s="105" t="s">
+      <c r="D11" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E11" s="94" t="s">
@@ -25686,7 +25693,7 @@
         <v>128</v>
       </c>
       <c r="H11" s="95"/>
-      <c r="I11" s="105" t="s">
+      <c r="I11" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J11" s="95" t="s">
@@ -25696,8 +25703,8 @@
       <c r="L11" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="M11" s="105"/>
-      <c r="N11" s="105"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="103"/>
       <c r="O11" s="96">
         <v>43964</v>
       </c>
@@ -25721,16 +25728,16 @@
       </c>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="104">
+      <c r="A12" s="102">
         <v>15</v>
       </c>
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="103" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="105">
+      <c r="C12" s="103">
         <v>7</v>
       </c>
-      <c r="D12" s="105" t="s">
+      <c r="D12" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E12" s="94" t="s">
@@ -25745,16 +25752,16 @@
       <c r="H12" s="95" t="s">
         <v>134</v>
       </c>
-      <c r="I12" s="105" t="s">
+      <c r="I12" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J12" s="95" t="s">
         <v>133</v>
       </c>
       <c r="K12" s="95"/>
-      <c r="L12" s="105"/>
-      <c r="M12" s="105"/>
-      <c r="N12" s="105"/>
+      <c r="L12" s="103"/>
+      <c r="M12" s="103"/>
+      <c r="N12" s="103"/>
       <c r="O12" s="96">
         <v>43964</v>
       </c>
@@ -25778,16 +25785,16 @@
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="104">
+      <c r="A13" s="102">
         <v>10</v>
       </c>
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="105">
+      <c r="C13" s="103">
         <v>7</v>
       </c>
-      <c r="D13" s="105" t="s">
+      <c r="D13" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="94" t="s">
@@ -25802,16 +25809,16 @@
       <c r="H13" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="I13" s="105" t="s">
+      <c r="I13" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J13" s="95" t="s">
         <v>107</v>
       </c>
       <c r="K13" s="95"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105"/>
-      <c r="N13" s="105"/>
+      <c r="L13" s="103"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="103"/>
       <c r="O13" s="96">
         <v>43964</v>
       </c>
@@ -25833,16 +25840,16 @@
       <c r="U13" s="97"/>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="104">
+      <c r="A14" s="102">
         <v>12</v>
       </c>
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="105">
+      <c r="C14" s="103">
         <v>7</v>
       </c>
-      <c r="D14" s="105" t="s">
+      <c r="D14" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E14" s="94" t="s">
@@ -25855,16 +25862,16 @@
         <v>135</v>
       </c>
       <c r="H14" s="95"/>
-      <c r="I14" s="105" t="s">
+      <c r="I14" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J14" s="95" t="s">
         <v>62</v>
       </c>
       <c r="K14" s="95"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="105"/>
-      <c r="N14" s="105"/>
+      <c r="L14" s="103"/>
+      <c r="M14" s="103"/>
+      <c r="N14" s="103"/>
       <c r="O14" s="96">
         <v>43964</v>
       </c>
@@ -25888,16 +25895,16 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="104">
+      <c r="A15" s="102">
         <v>12</v>
       </c>
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="105">
+      <c r="C15" s="103">
         <v>7</v>
       </c>
-      <c r="D15" s="105" t="s">
+      <c r="D15" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E15" s="94" t="s">
@@ -25910,16 +25917,16 @@
         <v>136</v>
       </c>
       <c r="H15" s="95"/>
-      <c r="I15" s="105" t="s">
+      <c r="I15" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J15" s="95" t="s">
         <v>62</v>
       </c>
       <c r="K15" s="95"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
-      <c r="N15" s="105"/>
+      <c r="L15" s="103"/>
+      <c r="M15" s="103"/>
+      <c r="N15" s="103"/>
       <c r="O15" s="96">
         <v>43964</v>
       </c>
@@ -25943,16 +25950,16 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="104">
+      <c r="A16" s="102">
         <v>13</v>
       </c>
-      <c r="B16" s="105" t="s">
+      <c r="B16" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="105">
+      <c r="C16" s="103">
         <v>7</v>
       </c>
-      <c r="D16" s="105" t="s">
+      <c r="D16" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E16" s="94" t="s">
@@ -25965,16 +25972,16 @@
         <v>117</v>
       </c>
       <c r="H16" s="95"/>
-      <c r="I16" s="105" t="s">
+      <c r="I16" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J16" s="95" t="s">
         <v>115</v>
       </c>
       <c r="K16" s="95"/>
-      <c r="L16" s="105"/>
-      <c r="M16" s="105"/>
-      <c r="N16" s="105"/>
+      <c r="L16" s="103"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="103"/>
       <c r="O16" s="96">
         <v>43964</v>
       </c>
@@ -25998,16 +26005,16 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="104">
+      <c r="A17" s="102">
         <v>13</v>
       </c>
-      <c r="B17" s="105" t="s">
+      <c r="B17" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="105">
+      <c r="C17" s="103">
         <v>7</v>
       </c>
-      <c r="D17" s="105" t="s">
+      <c r="D17" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E17" s="94" t="s">
@@ -26020,16 +26027,16 @@
         <v>118</v>
       </c>
       <c r="H17" s="95"/>
-      <c r="I17" s="105" t="s">
+      <c r="I17" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J17" s="95" t="s">
         <v>115</v>
       </c>
       <c r="K17" s="95"/>
-      <c r="L17" s="105"/>
-      <c r="M17" s="105"/>
-      <c r="N17" s="105"/>
+      <c r="L17" s="103"/>
+      <c r="M17" s="103"/>
+      <c r="N17" s="103"/>
       <c r="O17" s="96">
         <v>43964</v>
       </c>
@@ -26053,16 +26060,16 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="104">
+      <c r="A18" s="102">
         <v>13</v>
       </c>
-      <c r="B18" s="105" t="s">
+      <c r="B18" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="105">
+      <c r="C18" s="103">
         <v>7</v>
       </c>
-      <c r="D18" s="105" t="s">
+      <c r="D18" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E18" s="94" t="s">
@@ -26075,16 +26082,16 @@
         <v>119</v>
       </c>
       <c r="H18" s="95"/>
-      <c r="I18" s="105" t="s">
+      <c r="I18" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J18" s="95" t="s">
         <v>115</v>
       </c>
       <c r="K18" s="95"/>
-      <c r="L18" s="105"/>
-      <c r="M18" s="105"/>
-      <c r="N18" s="105"/>
+      <c r="L18" s="103"/>
+      <c r="M18" s="103"/>
+      <c r="N18" s="103"/>
       <c r="O18" s="96">
         <v>43964</v>
       </c>
@@ -26108,16 +26115,16 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="104">
+      <c r="A19" s="102">
         <v>13</v>
       </c>
-      <c r="B19" s="105" t="s">
+      <c r="B19" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="105">
+      <c r="C19" s="103">
         <v>7</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E19" s="94" t="s">
@@ -26130,16 +26137,16 @@
         <v>120</v>
       </c>
       <c r="H19" s="95"/>
-      <c r="I19" s="105" t="s">
+      <c r="I19" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J19" s="95" t="s">
         <v>115</v>
       </c>
       <c r="K19" s="95"/>
-      <c r="L19" s="105"/>
-      <c r="M19" s="105"/>
-      <c r="N19" s="105"/>
+      <c r="L19" s="103"/>
+      <c r="M19" s="103"/>
+      <c r="N19" s="103"/>
       <c r="O19" s="96">
         <v>43964</v>
       </c>
@@ -26163,16 +26170,16 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="104">
+      <c r="A20" s="102">
         <v>10</v>
       </c>
-      <c r="B20" s="105" t="s">
+      <c r="B20" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="105">
+      <c r="C20" s="103">
         <v>7</v>
       </c>
-      <c r="D20" s="105" t="s">
+      <c r="D20" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E20" s="94" t="s">
@@ -26187,16 +26194,16 @@
       <c r="H20" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="I20" s="105" t="s">
+      <c r="I20" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J20" s="95" t="s">
         <v>107</v>
       </c>
       <c r="K20" s="95"/>
-      <c r="L20" s="105"/>
-      <c r="M20" s="105"/>
-      <c r="N20" s="105"/>
+      <c r="L20" s="103"/>
+      <c r="M20" s="103"/>
+      <c r="N20" s="103"/>
       <c r="O20" s="96">
         <v>43964</v>
       </c>
@@ -26218,16 +26225,16 @@
       <c r="U20" s="97"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="104">
+      <c r="A21" s="102">
         <v>10</v>
       </c>
-      <c r="B21" s="105" t="s">
+      <c r="B21" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="105">
+      <c r="C21" s="103">
         <v>7</v>
       </c>
-      <c r="D21" s="105" t="s">
+      <c r="D21" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E21" s="94" t="s">
@@ -26242,16 +26249,16 @@
       <c r="H21" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="I21" s="105" t="s">
+      <c r="I21" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J21" s="95" t="s">
         <v>107</v>
       </c>
       <c r="K21" s="95"/>
-      <c r="L21" s="105"/>
-      <c r="M21" s="105"/>
-      <c r="N21" s="105"/>
+      <c r="L21" s="103"/>
+      <c r="M21" s="103"/>
+      <c r="N21" s="103"/>
       <c r="O21" s="96">
         <v>43964</v>
       </c>
@@ -26273,16 +26280,16 @@
       <c r="U21" s="97"/>
     </row>
     <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="104">
+      <c r="A22" s="102">
         <v>10</v>
       </c>
-      <c r="B22" s="105" t="s">
+      <c r="B22" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="105">
+      <c r="C22" s="103">
         <v>7</v>
       </c>
-      <c r="D22" s="105" t="s">
+      <c r="D22" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E22" s="94" t="s">
@@ -26297,16 +26304,16 @@
       <c r="H22" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="I22" s="105" t="s">
+      <c r="I22" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J22" s="95" t="s">
         <v>107</v>
       </c>
       <c r="K22" s="95"/>
-      <c r="L22" s="105"/>
-      <c r="M22" s="105"/>
-      <c r="N22" s="105"/>
+      <c r="L22" s="103"/>
+      <c r="M22" s="103"/>
+      <c r="N22" s="103"/>
       <c r="O22" s="96">
         <v>43964</v>
       </c>
@@ -26328,16 +26335,16 @@
       <c r="U22" s="97"/>
     </row>
     <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="104">
+      <c r="A23" s="102">
         <v>10</v>
       </c>
-      <c r="B23" s="105" t="s">
+      <c r="B23" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="105">
+      <c r="C23" s="103">
         <v>7</v>
       </c>
-      <c r="D23" s="105" t="s">
+      <c r="D23" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E23" s="94" t="s">
@@ -26352,16 +26359,16 @@
       <c r="H23" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="I23" s="105" t="s">
+      <c r="I23" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J23" s="95" t="s">
         <v>107</v>
       </c>
       <c r="K23" s="95"/>
-      <c r="L23" s="105"/>
-      <c r="M23" s="105"/>
-      <c r="N23" s="105"/>
+      <c r="L23" s="103"/>
+      <c r="M23" s="103"/>
+      <c r="N23" s="103"/>
       <c r="O23" s="96">
         <v>43964</v>
       </c>
@@ -26383,16 +26390,16 @@
       <c r="U23" s="97"/>
     </row>
     <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="104">
+      <c r="A24" s="102">
         <v>14</v>
       </c>
-      <c r="B24" s="105" t="s">
+      <c r="B24" s="103" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="105">
+      <c r="C24" s="103">
         <v>7</v>
       </c>
-      <c r="D24" s="105" t="s">
+      <c r="D24" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E24" s="94" t="s">
@@ -26407,16 +26414,16 @@
       <c r="H24" s="95" t="s">
         <v>129</v>
       </c>
-      <c r="I24" s="105" t="s">
+      <c r="I24" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J24" s="95" t="s">
         <v>127</v>
       </c>
       <c r="K24" s="95"/>
-      <c r="L24" s="105"/>
-      <c r="M24" s="105"/>
-      <c r="N24" s="105"/>
+      <c r="L24" s="103"/>
+      <c r="M24" s="103"/>
+      <c r="N24" s="103"/>
       <c r="O24" s="96">
         <v>43964</v>
       </c>
@@ -26438,16 +26445,16 @@
       <c r="U24" s="97"/>
     </row>
     <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="104">
+      <c r="A25" s="102">
         <v>15</v>
       </c>
-      <c r="B25" s="105" t="s">
+      <c r="B25" s="103" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="105">
+      <c r="C25" s="103">
         <v>7</v>
       </c>
-      <c r="D25" s="105" t="s">
+      <c r="D25" s="103" t="s">
         <v>88</v>
       </c>
       <c r="E25" s="94" t="s">
@@ -26462,16 +26469,16 @@
       <c r="H25" s="95" t="s">
         <v>134</v>
       </c>
-      <c r="I25" s="105" t="s">
+      <c r="I25" s="103" t="s">
         <v>90</v>
       </c>
       <c r="J25" s="95" t="s">
         <v>133</v>
       </c>
       <c r="K25" s="95"/>
-      <c r="L25" s="105"/>
-      <c r="M25" s="105"/>
-      <c r="N25" s="105"/>
+      <c r="L25" s="103"/>
+      <c r="M25" s="103"/>
+      <c r="N25" s="103"/>
       <c r="O25" s="96">
         <v>43964</v>
       </c>
@@ -26495,220 +26502,220 @@
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="104"/>
-      <c r="B26" s="105"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="105"/>
+      <c r="A26" s="102"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="103"/>
       <c r="E26" s="94"/>
       <c r="F26" s="98"/>
       <c r="G26" s="94"/>
       <c r="H26" s="95"/>
-      <c r="I26" s="105"/>
+      <c r="I26" s="103"/>
       <c r="J26" s="95"/>
       <c r="K26" s="95"/>
-      <c r="L26" s="105"/>
-      <c r="M26" s="105"/>
-      <c r="N26" s="105"/>
+      <c r="L26" s="103"/>
+      <c r="M26" s="103"/>
+      <c r="N26" s="103"/>
       <c r="O26" s="96"/>
       <c r="P26" s="96"/>
       <c r="Q26" s="96"/>
       <c r="U26" s="97"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="104"/>
-      <c r="B27" s="105"/>
-      <c r="C27" s="105"/>
-      <c r="D27" s="105"/>
+      <c r="A27" s="102"/>
+      <c r="B27" s="103"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="103"/>
       <c r="E27" s="94"/>
       <c r="F27" s="98"/>
       <c r="G27" s="94"/>
       <c r="H27" s="95"/>
-      <c r="I27" s="105"/>
+      <c r="I27" s="103"/>
       <c r="J27" s="95"/>
       <c r="K27" s="95"/>
-      <c r="L27" s="105"/>
-      <c r="M27" s="105"/>
-      <c r="N27" s="105"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="103"/>
+      <c r="N27" s="103"/>
       <c r="O27" s="96"/>
       <c r="P27" s="96"/>
       <c r="Q27" s="96"/>
       <c r="U27" s="97"/>
     </row>
     <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="104"/>
-      <c r="B28" s="105"/>
-      <c r="C28" s="105"/>
-      <c r="D28" s="105"/>
+      <c r="A28" s="102"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="103"/>
       <c r="E28" s="94"/>
       <c r="F28" s="98"/>
       <c r="G28" s="94"/>
       <c r="H28" s="95"/>
-      <c r="I28" s="105"/>
+      <c r="I28" s="103"/>
       <c r="J28" s="95"/>
       <c r="K28" s="95"/>
-      <c r="L28" s="105"/>
-      <c r="M28" s="105"/>
-      <c r="N28" s="105"/>
+      <c r="L28" s="103"/>
+      <c r="M28" s="103"/>
+      <c r="N28" s="103"/>
       <c r="O28" s="96"/>
       <c r="P28" s="96"/>
       <c r="Q28" s="96"/>
       <c r="U28" s="97"/>
     </row>
     <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="104"/>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="A29" s="102"/>
+      <c r="B29" s="103"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="103"/>
       <c r="E29" s="94"/>
       <c r="F29" s="98"/>
       <c r="G29" s="94"/>
       <c r="H29" s="95"/>
-      <c r="I29" s="105"/>
+      <c r="I29" s="103"/>
       <c r="J29" s="95"/>
       <c r="K29" s="95"/>
-      <c r="L29" s="105"/>
-      <c r="M29" s="105"/>
-      <c r="N29" s="105"/>
+      <c r="L29" s="103"/>
+      <c r="M29" s="103"/>
+      <c r="N29" s="103"/>
       <c r="O29" s="96"/>
       <c r="P29" s="96"/>
       <c r="Q29" s="96"/>
       <c r="U29" s="97"/>
     </row>
     <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="104"/>
-      <c r="B30" s="105"/>
-      <c r="C30" s="105"/>
-      <c r="D30" s="105"/>
+      <c r="A30" s="102"/>
+      <c r="B30" s="103"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="103"/>
       <c r="E30" s="94"/>
       <c r="F30" s="98"/>
       <c r="G30" s="94"/>
       <c r="H30" s="95"/>
-      <c r="I30" s="105"/>
+      <c r="I30" s="103"/>
       <c r="J30" s="95"/>
       <c r="K30" s="95"/>
-      <c r="L30" s="105"/>
-      <c r="M30" s="105"/>
-      <c r="N30" s="105"/>
+      <c r="L30" s="103"/>
+      <c r="M30" s="103"/>
+      <c r="N30" s="103"/>
       <c r="O30" s="96"/>
       <c r="P30" s="96"/>
       <c r="Q30" s="96"/>
       <c r="U30" s="97"/>
     </row>
     <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="104"/>
-      <c r="B31" s="105"/>
-      <c r="C31" s="105"/>
-      <c r="D31" s="105"/>
+      <c r="A31" s="102"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
+      <c r="D31" s="103"/>
       <c r="E31" s="94"/>
       <c r="F31" s="98"/>
       <c r="G31" s="94"/>
       <c r="H31" s="95"/>
-      <c r="I31" s="105"/>
+      <c r="I31" s="103"/>
       <c r="J31" s="95"/>
       <c r="K31" s="95"/>
-      <c r="L31" s="105"/>
-      <c r="M31" s="105"/>
-      <c r="N31" s="105"/>
+      <c r="L31" s="103"/>
+      <c r="M31" s="103"/>
+      <c r="N31" s="103"/>
       <c r="O31" s="96"/>
       <c r="P31" s="96"/>
       <c r="Q31" s="96"/>
       <c r="U31" s="97"/>
     </row>
     <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="104"/>
-      <c r="B32" s="105"/>
-      <c r="C32" s="105"/>
-      <c r="D32" s="105"/>
+      <c r="A32" s="102"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
       <c r="E32" s="94"/>
       <c r="F32" s="98"/>
       <c r="G32" s="94"/>
       <c r="H32" s="95"/>
-      <c r="I32" s="105"/>
+      <c r="I32" s="103"/>
       <c r="J32" s="95"/>
       <c r="K32" s="95"/>
-      <c r="L32" s="105"/>
-      <c r="M32" s="105"/>
-      <c r="N32" s="105"/>
+      <c r="L32" s="103"/>
+      <c r="M32" s="103"/>
+      <c r="N32" s="103"/>
       <c r="O32" s="96"/>
       <c r="P32" s="96"/>
       <c r="Q32" s="96"/>
       <c r="U32" s="97"/>
     </row>
     <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="104"/>
-      <c r="B33" s="105"/>
-      <c r="C33" s="105"/>
-      <c r="D33" s="105"/>
+      <c r="A33" s="102"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="103"/>
+      <c r="D33" s="103"/>
       <c r="E33" s="94"/>
       <c r="F33" s="98"/>
       <c r="G33" s="94"/>
       <c r="H33" s="95"/>
-      <c r="I33" s="105"/>
+      <c r="I33" s="103"/>
       <c r="J33" s="95"/>
       <c r="K33" s="95"/>
-      <c r="L33" s="105"/>
-      <c r="M33" s="105"/>
-      <c r="N33" s="105"/>
+      <c r="L33" s="103"/>
+      <c r="M33" s="103"/>
+      <c r="N33" s="103"/>
       <c r="O33" s="96"/>
       <c r="P33" s="96"/>
       <c r="Q33" s="96"/>
       <c r="U33" s="97"/>
     </row>
     <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="104"/>
-      <c r="B34" s="105"/>
-      <c r="C34" s="105"/>
-      <c r="D34" s="105"/>
+      <c r="A34" s="102"/>
+      <c r="B34" s="103"/>
+      <c r="C34" s="103"/>
+      <c r="D34" s="103"/>
       <c r="E34" s="94"/>
       <c r="F34" s="98"/>
       <c r="G34" s="94"/>
       <c r="H34" s="95"/>
-      <c r="I34" s="105"/>
+      <c r="I34" s="103"/>
       <c r="J34" s="95"/>
       <c r="K34" s="95"/>
-      <c r="L34" s="105"/>
-      <c r="M34" s="105"/>
-      <c r="N34" s="105"/>
+      <c r="L34" s="103"/>
+      <c r="M34" s="103"/>
+      <c r="N34" s="103"/>
       <c r="O34" s="96"/>
       <c r="P34" s="96"/>
       <c r="Q34" s="96"/>
       <c r="U34" s="97"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="104"/>
-      <c r="B35" s="105"/>
-      <c r="C35" s="105"/>
-      <c r="D35" s="105"/>
+      <c r="A35" s="102"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="103"/>
+      <c r="D35" s="103"/>
       <c r="E35" s="94"/>
       <c r="F35" s="98"/>
       <c r="G35" s="94"/>
       <c r="H35" s="95"/>
-      <c r="I35" s="105"/>
+      <c r="I35" s="103"/>
       <c r="J35" s="95"/>
       <c r="K35" s="95"/>
-      <c r="L35" s="105"/>
-      <c r="M35" s="105"/>
-      <c r="N35" s="105"/>
+      <c r="L35" s="103"/>
+      <c r="M35" s="103"/>
+      <c r="N35" s="103"/>
       <c r="O35" s="96"/>
       <c r="P35" s="96"/>
       <c r="Q35" s="96"/>
       <c r="U35" s="97"/>
     </row>
     <row r="36" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="104"/>
-      <c r="B36" s="105"/>
-      <c r="C36" s="105"/>
-      <c r="D36" s="105"/>
+      <c r="A36" s="102"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="103"/>
+      <c r="D36" s="103"/>
       <c r="E36" s="94"/>
       <c r="F36" s="98"/>
       <c r="G36" s="94"/>
       <c r="H36" s="95"/>
-      <c r="I36" s="105"/>
+      <c r="I36" s="103"/>
       <c r="J36" s="95"/>
       <c r="K36" s="95"/>
-      <c r="L36" s="105"/>
-      <c r="M36" s="105"/>
-      <c r="N36" s="105"/>
+      <c r="L36" s="103"/>
+      <c r="M36" s="103"/>
+      <c r="N36" s="103"/>
       <c r="O36" s="96"/>
       <c r="P36" s="96"/>
       <c r="Q36" s="96"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-21-2020 22-24-41
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="400" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F4E63D52-9C3B-4E39-9CC7-1F94BCCD883F}"/>
+  <xr:revisionPtr revIDLastSave="409" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2D62B888-9B13-410B-A007-42AA3220CB69}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -1224,7 +1224,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1367,9 +1367,6 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="44" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="44" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="34" fillId="38" borderId="0" xfId="44" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1377,6 +1374,10 @@
     <xf numFmtId="0" fontId="34" fillId="39" borderId="0" xfId="44" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Énfasis1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1429,9 +1430,6 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1443,6 +1441,9 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1993,7 +1994,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="1">
   <autoFilter ref="A1:U36" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -2016,7 +2017,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="1"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3873,26 +3874,26 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="104" t="s">
+      <c r="A78" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="105"/>
-      <c r="C78" s="105"/>
-      <c r="D78" s="105"/>
-      <c r="E78" s="105"/>
-      <c r="F78" s="105"/>
-      <c r="G78" s="105"/>
+      <c r="B78" s="108"/>
+      <c r="C78" s="108"/>
+      <c r="D78" s="108"/>
+      <c r="E78" s="108"/>
+      <c r="F78" s="108"/>
+      <c r="G78" s="108"/>
     </row>
     <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="104" t="s">
+      <c r="A79" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="B79" s="105"/>
-      <c r="C79" s="105"/>
-      <c r="D79" s="105"/>
-      <c r="E79" s="105"/>
-      <c r="F79" s="105"/>
-      <c r="G79" s="105"/>
+      <c r="B79" s="108"/>
+      <c r="C79" s="108"/>
+      <c r="D79" s="108"/>
+      <c r="E79" s="108"/>
+      <c r="F79" s="108"/>
+      <c r="G79" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3938,10 +3939,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R504"/>
+  <dimension ref="A1:R513"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A478" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I506" sqref="I506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11535,19 +11536,46 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="503" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B503" s="91" t="s">
+    <row r="502" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A502" s="85"/>
+    </row>
+    <row r="503" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A503" s="85"/>
+    </row>
+    <row r="504" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A504" s="85"/>
+    </row>
+    <row r="505" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A505" s="85"/>
+    </row>
+    <row r="506" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A506" s="85"/>
+    </row>
+    <row r="507" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A507" s="85"/>
+    </row>
+    <row r="508" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A508" s="85"/>
+    </row>
+    <row r="509" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A509" s="85"/>
+    </row>
+    <row r="510" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A510" s="85"/>
+    </row>
+    <row r="512" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B512" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="C503" s="91" t="s">
+      <c r="C512" s="91" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="504" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C504" s="91" t="s">
+    <row r="513" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C513" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="D504" s="91" t="s">
+      <c r="D513" s="91" t="s">
         <v>62</v>
       </c>
     </row>
@@ -11556,14 +11584,14 @@
     <sortCondition ref="S16:S27"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B503" r:id="rId1" xr:uid="{7BAB9C96-11D1-4038-884D-1426BB882084}"/>
+    <hyperlink ref="B512" r:id="rId1" xr:uid="{7BAB9C96-11D1-4038-884D-1426BB882084}"/>
     <hyperlink ref="L2" r:id="rId2" xr:uid="{B8CAFB40-6EA0-4A50-BC16-E7F789B2AAB7}"/>
     <hyperlink ref="R46" r:id="rId3" xr:uid="{B99DA151-0001-4CAD-BDB1-1DD20A148565}"/>
     <hyperlink ref="Q47" r:id="rId4" xr:uid="{3ADA1F83-7764-4410-AF8D-A6B16C6CD6E2}"/>
     <hyperlink ref="E2" r:id="rId5" xr:uid="{B78B62A0-2642-4AC4-8E39-F8778B79B985}"/>
-    <hyperlink ref="C503" r:id="rId6" xr:uid="{DC74A279-FB7D-4692-81BA-5233CB5872ED}"/>
-    <hyperlink ref="C504" r:id="rId7" xr:uid="{1B03CB83-2532-400F-87A6-2CFEFAC99AFC}"/>
-    <hyperlink ref="D504" r:id="rId8" xr:uid="{0633EFE9-A0E8-4D17-936A-545094BB77AB}"/>
+    <hyperlink ref="C512" r:id="rId6" xr:uid="{DC74A279-FB7D-4692-81BA-5233CB5872ED}"/>
+    <hyperlink ref="C513" r:id="rId7" xr:uid="{1B03CB83-2532-400F-87A6-2CFEFAC99AFC}"/>
+    <hyperlink ref="D513" r:id="rId8" xr:uid="{0633EFE9-A0E8-4D17-936A-545094BB77AB}"/>
     <hyperlink ref="Q46" r:id="rId9" xr:uid="{750C159B-27DC-410D-A399-96EEED38238E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25048,7 +25076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB840748-361D-4458-B100-AAECA785CA65}">
   <dimension ref="A1:Y972"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -25078,67 +25106,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="107" t="s">
+      <c r="F1" s="106" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="107" t="s">
+      <c r="G1" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="106" t="s">
+      <c r="H1" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="106" t="s">
+      <c r="I1" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="106" t="s">
+      <c r="J1" s="105" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="106" t="s">
+      <c r="K1" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="106" t="s">
+      <c r="L1" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="M1" s="106" t="s">
+      <c r="M1" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="106" t="s">
+      <c r="N1" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="106" t="s">
+      <c r="O1" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="P1" s="106" t="s">
+      <c r="P1" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" s="106" t="s">
+      <c r="Q1" s="105" t="s">
         <v>82</v>
       </c>
-      <c r="R1" s="106" t="s">
+      <c r="R1" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="S1" s="106" t="s">
+      <c r="S1" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="T1" s="106" t="s">
+      <c r="T1" s="105" t="s">
         <v>85</v>
       </c>
-      <c r="U1" s="106" t="s">
+      <c r="U1" s="105" t="s">
         <v>86</v>
       </c>
       <c r="Y1" s="93" t="s">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-27-2020 01-25-45
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="485" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{47B4BCF7-2FA5-4105-989F-BEC2A0020169}"/>
+  <xr:revisionPtr revIDLastSave="509" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C881D030-6F9F-4D92-92B4-789C54E897A4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7980" yWindow="0" windowWidth="15060" windowHeight="12960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -1215,7 +1215,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1365,6 +1365,7 @@
     <xf numFmtId="0" fontId="34" fillId="39" borderId="0" xfId="44" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1911,8 +1912,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H513" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A3:H513" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H520" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A3:H520" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="19"/>
@@ -1948,8 +1949,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H513" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H513" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H520" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H520" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -3865,26 +3866,26 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="107" t="s">
+      <c r="A78" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="108"/>
-      <c r="C78" s="108"/>
-      <c r="D78" s="108"/>
-      <c r="E78" s="108"/>
-      <c r="F78" s="108"/>
-      <c r="G78" s="108"/>
+      <c r="B78" s="109"/>
+      <c r="C78" s="109"/>
+      <c r="D78" s="109"/>
+      <c r="E78" s="109"/>
+      <c r="F78" s="109"/>
+      <c r="G78" s="109"/>
     </row>
     <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="107" t="s">
+      <c r="A79" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="B79" s="108"/>
-      <c r="C79" s="108"/>
-      <c r="D79" s="108"/>
-      <c r="E79" s="108"/>
-      <c r="F79" s="108"/>
-      <c r="G79" s="108"/>
+      <c r="B79" s="109"/>
+      <c r="C79" s="109"/>
+      <c r="D79" s="109"/>
+      <c r="E79" s="109"/>
+      <c r="F79" s="109"/>
+      <c r="G79" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3930,11 +3931,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R513"/>
+  <dimension ref="A1:R524"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A496" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I512" sqref="I512"/>
+    <sheetView showGridLines="0" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5466,7 +5467,7 @@
         <v>42</v>
       </c>
       <c r="N41" s="62">
-        <v>4729.5</v>
+        <v>4730</v>
       </c>
       <c r="O41">
         <v>6</v>
@@ -11656,10 +11657,10 @@
         <v>24.833600000000001</v>
       </c>
       <c r="C511" s="104">
-        <v>102.95</v>
+        <v>103.6</v>
       </c>
       <c r="D511" s="104">
-        <v>10.73</v>
+        <v>10.93</v>
       </c>
       <c r="E511" s="104">
         <v>69.83</v>
@@ -11697,6 +11698,148 @@
       <c r="F513" s="104"/>
       <c r="G513" s="104"/>
       <c r="H513" s="104"/>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A514" s="85">
+        <v>43976</v>
+      </c>
+      <c r="B514" s="107">
+        <v>24.834499999999998</v>
+      </c>
+      <c r="C514" s="107"/>
+      <c r="D514" s="107"/>
+      <c r="E514" s="107"/>
+      <c r="F514" s="107"/>
+      <c r="G514" s="107"/>
+      <c r="H514" s="107"/>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A515" s="85">
+        <v>43977</v>
+      </c>
+      <c r="B515" s="107">
+        <v>24.835100000000001</v>
+      </c>
+      <c r="C515" s="107">
+        <v>105.08</v>
+      </c>
+      <c r="D515" s="107">
+        <v>11.09</v>
+      </c>
+      <c r="E515" s="107"/>
+      <c r="F515" s="107"/>
+      <c r="G515" s="107"/>
+      <c r="H515" s="107"/>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A516" s="85">
+        <v>43978</v>
+      </c>
+      <c r="B516" s="107">
+        <v>24.835699999999999</v>
+      </c>
+      <c r="C516" s="107"/>
+      <c r="D516" s="107"/>
+      <c r="E516" s="107"/>
+      <c r="F516" s="107"/>
+      <c r="G516" s="107"/>
+      <c r="H516" s="107"/>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A517" s="85">
+        <v>43979</v>
+      </c>
+      <c r="B517" s="107"/>
+      <c r="C517" s="107"/>
+      <c r="D517" s="107"/>
+      <c r="E517" s="107"/>
+      <c r="F517" s="107"/>
+      <c r="G517" s="107"/>
+      <c r="H517" s="107"/>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A518" s="85">
+        <v>43980</v>
+      </c>
+      <c r="B518" s="107"/>
+      <c r="C518" s="107"/>
+      <c r="D518" s="107"/>
+      <c r="E518" s="107">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="F518" s="107">
+        <v>64.31</v>
+      </c>
+      <c r="G518" s="107">
+        <v>54.43</v>
+      </c>
+      <c r="H518" s="107">
+        <v>33.31</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A519" s="85">
+        <v>43981</v>
+      </c>
+      <c r="B519" s="107"/>
+      <c r="C519" s="107"/>
+      <c r="D519" s="107"/>
+      <c r="E519" s="107"/>
+      <c r="F519" s="107"/>
+      <c r="G519" s="107"/>
+      <c r="H519" s="107"/>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A520" s="85">
+        <v>43982</v>
+      </c>
+      <c r="B520" s="107"/>
+      <c r="C520" s="107"/>
+      <c r="D520" s="107"/>
+      <c r="E520" s="107"/>
+      <c r="F520" s="107"/>
+      <c r="G520" s="107"/>
+      <c r="H520" s="107"/>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A521" s="85"/>
+      <c r="B521" s="107"/>
+      <c r="C521" s="107"/>
+      <c r="D521" s="107"/>
+      <c r="E521" s="107"/>
+      <c r="F521" s="107"/>
+      <c r="G521" s="107"/>
+      <c r="H521" s="107"/>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A522" s="85"/>
+      <c r="B522" s="107"/>
+      <c r="C522" s="107"/>
+      <c r="D522" s="107"/>
+      <c r="E522" s="107"/>
+      <c r="F522" s="107"/>
+      <c r="G522" s="107"/>
+      <c r="H522" s="107"/>
+    </row>
+    <row r="523" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A523" s="85"/>
+      <c r="B523" s="107"/>
+      <c r="C523" s="107"/>
+      <c r="D523" s="107"/>
+      <c r="E523" s="107"/>
+      <c r="F523" s="107"/>
+      <c r="G523" s="107"/>
+      <c r="H523" s="107"/>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A524" s="85"/>
+      <c r="B524" s="107"/>
+      <c r="C524" s="107"/>
+      <c r="D524" s="107"/>
+      <c r="E524" s="107"/>
+      <c r="F524" s="107"/>
+      <c r="G524" s="107"/>
+      <c r="H524" s="107"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -11717,11 +11860,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R513"/>
+  <dimension ref="A1:R520"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A496" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E515" sqref="E515"/>
+      <pane ySplit="3" topLeftCell="A505" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B522" sqref="B522"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13791,14 +13934,14 @@
         <v>15.15</v>
       </c>
       <c r="J45" s="86">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="K45" s="86" t="s">
         <v>26</v>
       </c>
       <c r="L45" s="86" t="str">
         <f t="shared" ref="L45" si="1">+K45&amp;", "&amp;J45</f>
-        <v>Junio, 2021</v>
+        <v>Junio, 2020</v>
       </c>
       <c r="M45" s="104"/>
       <c r="N45" s="104"/>
@@ -25337,7 +25480,9 @@
       <c r="A512" s="85">
         <v>43974</v>
       </c>
-      <c r="B512" s="104"/>
+      <c r="B512" s="104">
+        <v>7.6920299999999999</v>
+      </c>
       <c r="C512" s="104"/>
       <c r="D512" s="104"/>
       <c r="E512" s="104"/>
@@ -25349,13 +25494,111 @@
       <c r="A513" s="85">
         <v>43975</v>
       </c>
-      <c r="B513" s="104"/>
+      <c r="B513" s="104">
+        <v>7.6920299999999999</v>
+      </c>
       <c r="C513" s="104"/>
       <c r="D513" s="104"/>
       <c r="E513" s="104"/>
       <c r="F513" s="104"/>
       <c r="G513" s="104"/>
       <c r="H513" s="104"/>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A514" s="85">
+        <v>43976</v>
+      </c>
+      <c r="B514" s="107">
+        <v>7.6934699999999996</v>
+      </c>
+      <c r="C514" s="107"/>
+      <c r="D514" s="107"/>
+      <c r="E514" s="107">
+        <v>18.98</v>
+      </c>
+      <c r="F514" s="107">
+        <v>17.97</v>
+      </c>
+      <c r="G514" s="107">
+        <v>14.7</v>
+      </c>
+      <c r="H514" s="107"/>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A515" s="85">
+        <v>43977</v>
+      </c>
+      <c r="B515" s="107">
+        <v>7.6890999999999998</v>
+      </c>
+      <c r="C515" s="107"/>
+      <c r="D515" s="107"/>
+      <c r="E515" s="107"/>
+      <c r="F515" s="107"/>
+      <c r="G515" s="107"/>
+      <c r="H515" s="107"/>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A516" s="85">
+        <v>43978</v>
+      </c>
+      <c r="B516" s="107">
+        <v>7.6921600000000003</v>
+      </c>
+      <c r="C516" s="107"/>
+      <c r="D516" s="107"/>
+      <c r="E516" s="107"/>
+      <c r="F516" s="107"/>
+      <c r="G516" s="107"/>
+      <c r="H516" s="107"/>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A517" s="85">
+        <v>43979</v>
+      </c>
+      <c r="B517" s="107"/>
+      <c r="C517" s="107"/>
+      <c r="D517" s="107"/>
+      <c r="E517" s="107"/>
+      <c r="F517" s="107"/>
+      <c r="G517" s="107"/>
+      <c r="H517" s="107"/>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A518" s="85">
+        <v>43980</v>
+      </c>
+      <c r="B518" s="107"/>
+      <c r="C518" s="107"/>
+      <c r="D518" s="107"/>
+      <c r="E518" s="107"/>
+      <c r="F518" s="107"/>
+      <c r="G518" s="107"/>
+      <c r="H518" s="107"/>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A519" s="85">
+        <v>43981</v>
+      </c>
+      <c r="B519" s="107"/>
+      <c r="C519" s="107"/>
+      <c r="D519" s="107"/>
+      <c r="E519" s="107"/>
+      <c r="F519" s="107"/>
+      <c r="G519" s="107"/>
+      <c r="H519" s="107"/>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A520" s="85">
+        <v>43982</v>
+      </c>
+      <c r="B520" s="107"/>
+      <c r="C520" s="107"/>
+      <c r="D520" s="107"/>
+      <c r="E520" s="107"/>
+      <c r="F520" s="107"/>
+      <c r="G520" s="107"/>
+      <c r="H520" s="107"/>
     </row>
   </sheetData>
   <phoneticPr fontId="39" type="noConversion"/>
@@ -25372,10 +25615,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-30-2020 01-35-22
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="509" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C881D030-6F9F-4D92-92B4-789C54E897A4}"/>
+  <xr:revisionPtr revIDLastSave="557" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ABBC9A3E-D18E-4ADB-BAD2-571DFEE59200}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="0" windowWidth="15060" windowHeight="12960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCR" sheetId="1" r:id="rId1"/>
@@ -522,13 +522,13 @@
     <t>https://www.mem.gob.gt/</t>
   </si>
   <si>
-    <t>.asp</t>
-  </si>
-  <si>
     <t>https://www.ine.gob.gt/</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>.xls</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1215,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1366,6 +1366,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1421,6 +1422,47 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="25">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="d/m/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF5D7B9D"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1557,47 +1599,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF5D7B9D"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="169" formatCode="d/m/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1912,8 +1913,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H520" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A3:H520" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H527" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A3:H527" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="19"/>
@@ -1929,8 +1930,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R45" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R45" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R46" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R46" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="14"/>
@@ -1949,10 +1950,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H520" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H520" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H527" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A3:H527" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
     <tableColumn id="3" xr3:uid="{47070387-916A-43EA-9250-BD5CD00DE202}" name="Precio Café"/>
     <tableColumn id="4" xr3:uid="{017F8C94-7948-49FE-B245-F576C80EC85B}" name="Precio Azúcar"/>
@@ -1966,18 +1967,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R45" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R45" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R46" totalsRowShown="0" headerRowDxfId="10" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R46" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="7">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{B7D1225A-C849-430C-8F2C-569D3B5E64AD}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="4" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="3" dataCellStyle="Millares [0]"/>
-    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="2" dataCellStyle="Millares [0]"/>
+    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="6" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="5" dataCellStyle="Millares [0]"/>
+    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="4" dataCellStyle="Millares [0]"/>
     <tableColumn id="8" xr3:uid="{552CA574-1C46-4E0F-8C54-8DBCDA6B12C1}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{C793523A-103E-4CA7-94B8-3E3D9A633FDB}" name="Ingresos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1986,7 +1987,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="3">
   <autoFilter ref="A1:U36" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -2009,7 +2010,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3866,26 +3867,26 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="108" t="s">
+      <c r="A78" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="109"/>
-      <c r="C78" s="109"/>
-      <c r="D78" s="109"/>
-      <c r="E78" s="109"/>
-      <c r="F78" s="109"/>
-      <c r="G78" s="109"/>
+      <c r="B78" s="110"/>
+      <c r="C78" s="110"/>
+      <c r="D78" s="110"/>
+      <c r="E78" s="110"/>
+      <c r="F78" s="110"/>
+      <c r="G78" s="110"/>
     </row>
     <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="108" t="s">
+      <c r="A79" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="B79" s="109"/>
-      <c r="C79" s="109"/>
-      <c r="D79" s="109"/>
-      <c r="E79" s="109"/>
-      <c r="F79" s="109"/>
-      <c r="G79" s="109"/>
+      <c r="B79" s="110"/>
+      <c r="C79" s="110"/>
+      <c r="D79" s="110"/>
+      <c r="E79" s="110"/>
+      <c r="F79" s="110"/>
+      <c r="G79" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3931,11 +3932,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R524"/>
+  <dimension ref="A1:R527"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q47" sqref="Q47"/>
+      <selection pane="bottomLeft" activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5615,8 +5616,22 @@
       <c r="D46">
         <v>12.85</v>
       </c>
-      <c r="Q46" s="104"/>
-      <c r="R46" s="104"/>
+      <c r="J46" s="86">
+        <v>2020</v>
+      </c>
+      <c r="K46" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="L46" s="86" t="str">
+        <f t="shared" ref="L46" si="2">+K46&amp;", "&amp;J46</f>
+        <v>Julio, 2020</v>
+      </c>
+      <c r="M46" s="108"/>
+      <c r="N46" s="62"/>
+      <c r="O46" s="108"/>
+      <c r="P46" s="62"/>
+      <c r="Q46" s="108"/>
+      <c r="R46" s="108"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="85">
@@ -11721,10 +11736,10 @@
         <v>24.835100000000001</v>
       </c>
       <c r="C515" s="107">
-        <v>105.08</v>
+        <v>105.1</v>
       </c>
       <c r="D515" s="107">
-        <v>11.09</v>
+        <v>11.05</v>
       </c>
       <c r="E515" s="107"/>
       <c r="F515" s="107"/>
@@ -11738,8 +11753,12 @@
       <c r="B516" s="107">
         <v>24.835699999999999</v>
       </c>
-      <c r="C516" s="107"/>
-      <c r="D516" s="107"/>
+      <c r="C516" s="107">
+        <v>102.5</v>
+      </c>
+      <c r="D516" s="107">
+        <v>10.8</v>
+      </c>
       <c r="E516" s="107"/>
       <c r="F516" s="107"/>
       <c r="G516" s="107"/>
@@ -11749,9 +11768,15 @@
       <c r="A517" s="85">
         <v>43979</v>
       </c>
-      <c r="B517" s="107"/>
-      <c r="C517" s="107"/>
-      <c r="D517" s="107"/>
+      <c r="B517" s="107">
+        <v>24.835699999999999</v>
+      </c>
+      <c r="C517" s="107">
+        <v>99.1</v>
+      </c>
+      <c r="D517" s="108">
+        <v>10.8</v>
+      </c>
       <c r="E517" s="107"/>
       <c r="F517" s="107"/>
       <c r="G517" s="107"/>
@@ -11761,9 +11786,15 @@
       <c r="A518" s="85">
         <v>43980</v>
       </c>
-      <c r="B518" s="107"/>
-      <c r="C518" s="107"/>
-      <c r="D518" s="107"/>
+      <c r="B518" s="107">
+        <v>24.8354</v>
+      </c>
+      <c r="C518" s="107">
+        <v>96.03</v>
+      </c>
+      <c r="D518" s="107">
+        <v>10.91</v>
+      </c>
       <c r="E518" s="107">
         <v>72.099999999999994</v>
       </c>
@@ -11802,44 +11833,90 @@
       <c r="H520" s="107"/>
     </row>
     <row r="521" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A521" s="85"/>
-      <c r="B521" s="107"/>
-      <c r="C521" s="107"/>
-      <c r="D521" s="107"/>
-      <c r="E521" s="107"/>
-      <c r="F521" s="107"/>
-      <c r="G521" s="107"/>
-      <c r="H521" s="107"/>
+      <c r="A521" s="85">
+        <v>43983</v>
+      </c>
+      <c r="B521" s="108">
+        <v>24.835100000000001</v>
+      </c>
+      <c r="C521" s="108"/>
+      <c r="D521" s="108"/>
+      <c r="E521" s="108"/>
+      <c r="F521" s="108"/>
+      <c r="G521" s="108"/>
+      <c r="H521" s="108"/>
     </row>
     <row r="522" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A522" s="85"/>
-      <c r="B522" s="107"/>
-      <c r="C522" s="107"/>
-      <c r="D522" s="107"/>
-      <c r="E522" s="107"/>
-      <c r="F522" s="107"/>
-      <c r="G522" s="107"/>
-      <c r="H522" s="107"/>
+      <c r="A522" s="85">
+        <v>43984</v>
+      </c>
+      <c r="B522" s="108"/>
+      <c r="C522" s="108"/>
+      <c r="D522" s="108"/>
+      <c r="E522" s="108"/>
+      <c r="F522" s="108"/>
+      <c r="G522" s="108"/>
+      <c r="H522" s="108"/>
     </row>
     <row r="523" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A523" s="85"/>
-      <c r="B523" s="107"/>
-      <c r="C523" s="107"/>
-      <c r="D523" s="107"/>
-      <c r="E523" s="107"/>
-      <c r="F523" s="107"/>
-      <c r="G523" s="107"/>
-      <c r="H523" s="107"/>
+      <c r="A523" s="85">
+        <v>43985</v>
+      </c>
+      <c r="B523" s="108"/>
+      <c r="C523" s="108"/>
+      <c r="D523" s="108"/>
+      <c r="E523" s="108"/>
+      <c r="F523" s="108"/>
+      <c r="G523" s="108"/>
+      <c r="H523" s="108"/>
     </row>
     <row r="524" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A524" s="85"/>
-      <c r="B524" s="107"/>
-      <c r="C524" s="107"/>
-      <c r="D524" s="107"/>
-      <c r="E524" s="107"/>
-      <c r="F524" s="107"/>
-      <c r="G524" s="107"/>
-      <c r="H524" s="107"/>
+      <c r="A524" s="85">
+        <v>43986</v>
+      </c>
+      <c r="B524" s="108"/>
+      <c r="C524" s="108"/>
+      <c r="D524" s="108"/>
+      <c r="E524" s="108"/>
+      <c r="F524" s="108"/>
+      <c r="G524" s="108"/>
+      <c r="H524" s="108"/>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A525" s="85">
+        <v>43987</v>
+      </c>
+      <c r="B525" s="108"/>
+      <c r="C525" s="108"/>
+      <c r="D525" s="108"/>
+      <c r="E525" s="108"/>
+      <c r="F525" s="108"/>
+      <c r="G525" s="108"/>
+      <c r="H525" s="108"/>
+    </row>
+    <row r="526" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A526" s="85">
+        <v>43988</v>
+      </c>
+      <c r="B526" s="108"/>
+      <c r="C526" s="108"/>
+      <c r="D526" s="108"/>
+      <c r="E526" s="108"/>
+      <c r="F526" s="108"/>
+      <c r="G526" s="108"/>
+      <c r="H526" s="108"/>
+    </row>
+    <row r="527" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A527" s="85">
+        <v>43989</v>
+      </c>
+      <c r="B527" s="108"/>
+      <c r="C527" s="108"/>
+      <c r="D527" s="108"/>
+      <c r="E527" s="108"/>
+      <c r="F527" s="108"/>
+      <c r="G527" s="108"/>
+      <c r="H527" s="108"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -11860,11 +11937,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R520"/>
+  <dimension ref="A1:R527"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A505" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B522" sqref="B522"/>
+    <sheetView showGridLines="0" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13900,10 +13977,10 @@
         <v>Mayo, 2020</v>
       </c>
       <c r="O44" s="101">
-        <v>4579.6850000000004</v>
+        <v>7609.8950000000004</v>
       </c>
       <c r="P44" s="101">
-        <v>77.81</v>
+        <v>140.26</v>
       </c>
       <c r="Q44" s="99"/>
       <c r="R44" s="99"/>
@@ -13975,8 +14052,22 @@
       <c r="H46" s="99">
         <v>15.15</v>
       </c>
-      <c r="Q46" s="104"/>
-      <c r="R46" s="104"/>
+      <c r="J46" s="86">
+        <v>2020</v>
+      </c>
+      <c r="K46" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="L46" s="86" t="str">
+        <f t="shared" ref="L46" si="2">+K46&amp;", "&amp;J46</f>
+        <v>Julio, 2020</v>
+      </c>
+      <c r="M46" s="108"/>
+      <c r="N46" s="108"/>
+      <c r="O46" s="101"/>
+      <c r="P46" s="101"/>
+      <c r="Q46" s="108"/>
+      <c r="R46" s="108"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="85">
@@ -25432,7 +25523,9 @@
       <c r="E508" s="104"/>
       <c r="F508" s="104"/>
       <c r="G508" s="104"/>
-      <c r="H508" s="104"/>
+      <c r="H508" s="104">
+        <v>9.6</v>
+      </c>
     </row>
     <row r="509" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A509" s="85">
@@ -25446,7 +25539,9 @@
       <c r="E509" s="104"/>
       <c r="F509" s="104"/>
       <c r="G509" s="104"/>
-      <c r="H509" s="104"/>
+      <c r="H509" s="104">
+        <v>9.6</v>
+      </c>
     </row>
     <row r="510" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A510" s="85">
@@ -25455,12 +25550,18 @@
       <c r="B510" s="104">
         <v>7.6928700000000001</v>
       </c>
-      <c r="C510" s="104"/>
-      <c r="D510" s="104"/>
+      <c r="C510" s="104">
+        <v>154.69</v>
+      </c>
+      <c r="D510" s="108">
+        <v>25.9</v>
+      </c>
       <c r="E510" s="104"/>
       <c r="F510" s="104"/>
       <c r="G510" s="104"/>
-      <c r="H510" s="104"/>
+      <c r="H510" s="104">
+        <v>9.6</v>
+      </c>
     </row>
     <row r="511" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A511" s="85">
@@ -25474,7 +25575,9 @@
       <c r="E511" s="104"/>
       <c r="F511" s="104"/>
       <c r="G511" s="104"/>
-      <c r="H511" s="104"/>
+      <c r="H511" s="104">
+        <v>9.6</v>
+      </c>
     </row>
     <row r="512" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A512" s="85">
@@ -25488,7 +25591,9 @@
       <c r="E512" s="104"/>
       <c r="F512" s="104"/>
       <c r="G512" s="104"/>
-      <c r="H512" s="104"/>
+      <c r="H512" s="104">
+        <v>9.6</v>
+      </c>
     </row>
     <row r="513" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A513" s="85">
@@ -25502,7 +25607,9 @@
       <c r="E513" s="104"/>
       <c r="F513" s="104"/>
       <c r="G513" s="104"/>
-      <c r="H513" s="104"/>
+      <c r="H513" s="104">
+        <v>9.6</v>
+      </c>
     </row>
     <row r="514" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A514" s="85">
@@ -25522,7 +25629,9 @@
       <c r="G514" s="107">
         <v>14.7</v>
       </c>
-      <c r="H514" s="107"/>
+      <c r="H514" s="107">
+        <v>10</v>
+      </c>
     </row>
     <row r="515" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A515" s="85">
@@ -25536,7 +25645,9 @@
       <c r="E515" s="107"/>
       <c r="F515" s="107"/>
       <c r="G515" s="107"/>
-      <c r="H515" s="107"/>
+      <c r="H515" s="107">
+        <v>10</v>
+      </c>
     </row>
     <row r="516" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A516" s="85">
@@ -25550,55 +25661,157 @@
       <c r="E516" s="107"/>
       <c r="F516" s="107"/>
       <c r="G516" s="107"/>
-      <c r="H516" s="107"/>
+      <c r="H516" s="107">
+        <v>10</v>
+      </c>
     </row>
     <row r="517" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A517" s="85">
         <v>43979</v>
       </c>
-      <c r="B517" s="107"/>
+      <c r="B517" s="107">
+        <v>7.6915300000000002</v>
+      </c>
       <c r="C517" s="107"/>
       <c r="D517" s="107"/>
       <c r="E517" s="107"/>
       <c r="F517" s="107"/>
       <c r="G517" s="107"/>
-      <c r="H517" s="107"/>
+      <c r="H517" s="107">
+        <v>10</v>
+      </c>
     </row>
     <row r="518" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A518" s="85">
         <v>43980</v>
       </c>
-      <c r="B518" s="107"/>
+      <c r="B518" s="107">
+        <v>7.6894900000000002</v>
+      </c>
       <c r="C518" s="107"/>
       <c r="D518" s="107"/>
       <c r="E518" s="107"/>
       <c r="F518" s="107"/>
       <c r="G518" s="107"/>
-      <c r="H518" s="107"/>
+      <c r="H518" s="107">
+        <v>10</v>
+      </c>
     </row>
     <row r="519" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A519" s="85">
         <v>43981</v>
       </c>
-      <c r="B519" s="107"/>
+      <c r="B519" s="107">
+        <v>7.6894900000000002</v>
+      </c>
       <c r="C519" s="107"/>
       <c r="D519" s="107"/>
       <c r="E519" s="107"/>
       <c r="F519" s="107"/>
       <c r="G519" s="107"/>
-      <c r="H519" s="107"/>
+      <c r="H519" s="107">
+        <v>10</v>
+      </c>
     </row>
     <row r="520" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A520" s="85">
         <v>43982</v>
       </c>
-      <c r="B520" s="107"/>
+      <c r="B520" s="107">
+        <v>7.6894900000000002</v>
+      </c>
       <c r="C520" s="107"/>
       <c r="D520" s="107"/>
       <c r="E520" s="107"/>
       <c r="F520" s="107"/>
       <c r="G520" s="107"/>
-      <c r="H520" s="107"/>
+      <c r="H520" s="107">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A521" s="85">
+        <v>43983</v>
+      </c>
+      <c r="B521" s="108"/>
+      <c r="C521" s="108"/>
+      <c r="D521" s="108"/>
+      <c r="E521" s="108"/>
+      <c r="F521" s="108"/>
+      <c r="G521" s="108"/>
+      <c r="H521" s="108"/>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A522" s="85">
+        <v>43984</v>
+      </c>
+      <c r="B522" s="108"/>
+      <c r="C522" s="108"/>
+      <c r="D522" s="108"/>
+      <c r="E522" s="108"/>
+      <c r="F522" s="108"/>
+      <c r="G522" s="108"/>
+      <c r="H522" s="108"/>
+    </row>
+    <row r="523" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A523" s="85">
+        <v>43985</v>
+      </c>
+      <c r="B523" s="108"/>
+      <c r="C523" s="108"/>
+      <c r="D523" s="108"/>
+      <c r="E523" s="108"/>
+      <c r="F523" s="108"/>
+      <c r="G523" s="108"/>
+      <c r="H523" s="108"/>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A524" s="85">
+        <v>43986</v>
+      </c>
+      <c r="B524" s="108"/>
+      <c r="C524" s="108"/>
+      <c r="D524" s="108"/>
+      <c r="E524" s="108"/>
+      <c r="F524" s="108"/>
+      <c r="G524" s="108"/>
+      <c r="H524" s="108"/>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A525" s="85">
+        <v>43987</v>
+      </c>
+      <c r="B525" s="108"/>
+      <c r="C525" s="108"/>
+      <c r="D525" s="108"/>
+      <c r="E525" s="108"/>
+      <c r="F525" s="108"/>
+      <c r="G525" s="108"/>
+      <c r="H525" s="108"/>
+    </row>
+    <row r="526" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A526" s="85">
+        <v>43988</v>
+      </c>
+      <c r="B526" s="108"/>
+      <c r="C526" s="108"/>
+      <c r="D526" s="108"/>
+      <c r="E526" s="108"/>
+      <c r="F526" s="108"/>
+      <c r="G526" s="108"/>
+      <c r="H526" s="108"/>
+    </row>
+    <row r="527" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A527" s="85">
+        <v>43989</v>
+      </c>
+      <c r="B527" s="108"/>
+      <c r="C527" s="108"/>
+      <c r="D527" s="108"/>
+      <c r="E527" s="108"/>
+      <c r="F527" s="108"/>
+      <c r="G527" s="108"/>
+      <c r="H527" s="108"/>
     </row>
   </sheetData>
   <phoneticPr fontId="39" type="noConversion"/>
@@ -25615,10 +25828,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26169,11 +26382,9 @@
         <v>84</v>
       </c>
       <c r="T9" s="92" t="s">
-        <v>142</v>
-      </c>
-      <c r="U9" s="97" t="s">
-        <v>97</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="U9" s="97"/>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="102">
@@ -26230,11 +26441,9 @@
         <v>84</v>
       </c>
       <c r="T10" s="92" t="s">
-        <v>142</v>
-      </c>
-      <c r="U10" s="97" t="s">
-        <v>97</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="U10" s="97"/>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="102">
@@ -26263,11 +26472,11 @@
         <v>85</v>
       </c>
       <c r="J11" s="95" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K11" s="95"/>
       <c r="L11" s="94" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M11" s="103"/>
       <c r="N11" s="103"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-03-2020 01-47-07
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="557" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ABBC9A3E-D18E-4ADB-BAD2-571DFEE59200}"/>
+  <xr:revisionPtr revIDLastSave="567" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{291E127F-AA58-46B7-B679-9A32077ACE29}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1429,47 +1429,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="169" formatCode="d/m/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF5D7B9D"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <name val="Arial"/>
@@ -1599,6 +1558,47 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF5D7B9D"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="d/m/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1950,10 +1950,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H527" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H527" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A3:H527" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
     <tableColumn id="3" xr3:uid="{47070387-916A-43EA-9250-BD5CD00DE202}" name="Precio Café"/>
     <tableColumn id="4" xr3:uid="{017F8C94-7948-49FE-B245-F576C80EC85B}" name="Precio Azúcar"/>
@@ -1967,18 +1967,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R46" totalsRowShown="0" headerRowDxfId="10" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R46" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R46" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="5">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{B7D1225A-C849-430C-8F2C-569D3B5E64AD}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="6" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="5" dataCellStyle="Millares [0]"/>
-    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="4" dataCellStyle="Millares [0]"/>
+    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="4" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="3" dataCellStyle="Millares [0]"/>
+    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="2" dataCellStyle="Millares [0]"/>
     <tableColumn id="8" xr3:uid="{552CA574-1C46-4E0F-8C54-8DBCDA6B12C1}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{C793523A-103E-4CA7-94B8-3E3D9A633FDB}" name="Ingresos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1987,7 +1987,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="1">
   <autoFilter ref="A1:U36" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -2010,7 +2010,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3934,9 +3934,9 @@
   </sheetPr>
   <dimension ref="A1:R527"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S48" sqref="S48"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A505" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D529" sqref="D529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11790,7 +11790,7 @@
         <v>24.8354</v>
       </c>
       <c r="C518" s="107">
-        <v>96.03</v>
+        <v>96.3</v>
       </c>
       <c r="D518" s="107">
         <v>10.91</v>
@@ -11839,8 +11839,12 @@
       <c r="B521" s="108">
         <v>24.835100000000001</v>
       </c>
-      <c r="C521" s="108"/>
-      <c r="D521" s="108"/>
+      <c r="C521" s="108">
+        <v>98.3</v>
+      </c>
+      <c r="D521" s="108">
+        <v>11</v>
+      </c>
       <c r="E521" s="108"/>
       <c r="F521" s="108"/>
       <c r="G521" s="108"/>
@@ -11850,9 +11854,15 @@
       <c r="A522" s="85">
         <v>43984</v>
       </c>
-      <c r="B522" s="108"/>
-      <c r="C522" s="108"/>
-      <c r="D522" s="108"/>
+      <c r="B522" s="108">
+        <v>24.8323</v>
+      </c>
+      <c r="C522" s="108">
+        <v>97.95</v>
+      </c>
+      <c r="D522" s="108">
+        <v>11.25</v>
+      </c>
       <c r="E522" s="108"/>
       <c r="F522" s="108"/>
       <c r="G522" s="108"/>
@@ -11862,7 +11872,9 @@
       <c r="A523" s="85">
         <v>43985</v>
       </c>
-      <c r="B523" s="108"/>
+      <c r="B523" s="108">
+        <v>24.829499999999999</v>
+      </c>
       <c r="C523" s="108"/>
       <c r="D523" s="108"/>
       <c r="E523" s="108"/>
@@ -11939,9 +11951,9 @@
   </sheetPr>
   <dimension ref="A1:R527"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S48" sqref="S48"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A507" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I523" sqref="I523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25733,7 +25745,9 @@
       <c r="A521" s="85">
         <v>43983</v>
       </c>
-      <c r="B521" s="108"/>
+      <c r="B521" s="108">
+        <v>7.6896199999999997</v>
+      </c>
       <c r="C521" s="108"/>
       <c r="D521" s="108"/>
       <c r="E521" s="108"/>
@@ -25745,7 +25759,9 @@
       <c r="A522" s="85">
         <v>43984</v>
       </c>
-      <c r="B522" s="108"/>
+      <c r="B522" s="108">
+        <v>7.6859599999999997</v>
+      </c>
       <c r="C522" s="108"/>
       <c r="D522" s="108"/>
       <c r="E522" s="108"/>
@@ -25828,10 +25844,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-06-2020 01-56-08
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="567" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{291E127F-AA58-46B7-B679-9A32077ACE29}"/>
+  <xr:revisionPtr revIDLastSave="607" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{327C2646-4E9C-436E-AAC6-D8B5A8FA1638}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1215,7 +1215,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1367,10 +1367,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Énfasis1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1913,8 +1915,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H527" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A3:H527" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H534" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A3:H534" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="19"/>
@@ -1950,8 +1952,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H527" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H527" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H534" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H534" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -3867,26 +3869,26 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="109" t="s">
+      <c r="A78" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="110"/>
-      <c r="C78" s="110"/>
-      <c r="D78" s="110"/>
-      <c r="E78" s="110"/>
-      <c r="F78" s="110"/>
-      <c r="G78" s="110"/>
+      <c r="B78" s="111"/>
+      <c r="C78" s="111"/>
+      <c r="D78" s="111"/>
+      <c r="E78" s="111"/>
+      <c r="F78" s="111"/>
+      <c r="G78" s="111"/>
     </row>
     <row r="79" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="109" t="s">
+      <c r="A79" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="B79" s="110"/>
-      <c r="C79" s="110"/>
-      <c r="D79" s="110"/>
-      <c r="E79" s="110"/>
-      <c r="F79" s="110"/>
-      <c r="G79" s="110"/>
+      <c r="B79" s="111"/>
+      <c r="C79" s="111"/>
+      <c r="D79" s="111"/>
+      <c r="E79" s="111"/>
+      <c r="F79" s="111"/>
+      <c r="G79" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3932,11 +3934,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R527"/>
+  <dimension ref="A1:R534"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A505" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D529" sqref="D529"/>
+      <pane ySplit="3" topLeftCell="A512" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B537" sqref="B537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5528,7 +5530,7 @@
         <v>0</v>
       </c>
       <c r="R42">
-        <v>358.1</v>
+        <v>362.5</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
@@ -5552,10 +5554,13 @@
         <v>0</v>
       </c>
       <c r="O43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P43" s="62">
-        <v>0</v>
+        <v>400</v>
+      </c>
+      <c r="R43">
+        <v>327.3</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
@@ -5571,6 +5576,12 @@
       <c r="L44" s="86" t="str">
         <f t="shared" si="0"/>
         <v>Mayo, 2020</v>
+      </c>
+      <c r="O44">
+        <v>2</v>
+      </c>
+      <c r="P44">
+        <v>650</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
@@ -11858,10 +11869,10 @@
         <v>24.8323</v>
       </c>
       <c r="C522" s="108">
-        <v>97.95</v>
+        <v>98.2</v>
       </c>
       <c r="D522" s="108">
-        <v>11.25</v>
+        <v>11.22</v>
       </c>
       <c r="E522" s="108"/>
       <c r="F522" s="108"/>
@@ -11875,8 +11886,12 @@
       <c r="B523" s="108">
         <v>24.829499999999999</v>
       </c>
-      <c r="C523" s="108"/>
-      <c r="D523" s="108"/>
+      <c r="C523" s="108">
+        <v>99.1</v>
+      </c>
+      <c r="D523" s="108">
+        <v>11.62</v>
+      </c>
       <c r="E523" s="108"/>
       <c r="F523" s="108"/>
       <c r="G523" s="108"/>
@@ -11886,31 +11901,47 @@
       <c r="A524" s="85">
         <v>43986</v>
       </c>
-      <c r="B524" s="108"/>
-      <c r="C524" s="108"/>
-      <c r="D524" s="108"/>
-      <c r="E524" s="108"/>
-      <c r="F524" s="108"/>
-      <c r="G524" s="108"/>
-      <c r="H524" s="108"/>
+      <c r="B524" s="108">
+        <v>24.8233</v>
+      </c>
+      <c r="C524" s="108">
+        <v>98.15</v>
+      </c>
+      <c r="D524" s="108">
+        <v>11.73</v>
+      </c>
     </row>
     <row r="525" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A525" s="85">
         <v>43987</v>
       </c>
-      <c r="B525" s="108"/>
-      <c r="C525" s="108"/>
-      <c r="D525" s="108"/>
-      <c r="E525" s="108"/>
-      <c r="F525" s="108"/>
-      <c r="G525" s="108"/>
-      <c r="H525" s="108"/>
+      <c r="B525" s="108">
+        <v>24.822700000000001</v>
+      </c>
+      <c r="C525" s="108">
+        <v>98.93</v>
+      </c>
+      <c r="D525" s="108">
+        <v>12.02</v>
+      </c>
+      <c r="E525" s="108">
+        <v>73.84</v>
+      </c>
+      <c r="F525" s="108">
+        <v>65.819999999999993</v>
+      </c>
+      <c r="G525" s="108">
+        <v>55.9</v>
+      </c>
+      <c r="H525" s="108">
+        <v>35.090000000000003</v>
+      </c>
     </row>
     <row r="526" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A526" s="85">
         <v>43988</v>
       </c>
-      <c r="B526" s="108"/>
+      <c r="B526" s="112"/>
       <c r="C526" s="108"/>
       <c r="D526" s="108"/>
       <c r="E526" s="108"/>
@@ -11929,6 +11960,92 @@
       <c r="F527" s="108"/>
       <c r="G527" s="108"/>
       <c r="H527" s="108"/>
+    </row>
+    <row r="528" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A528" s="85">
+        <v>43990</v>
+      </c>
+      <c r="B528" s="108">
+        <v>24.8184</v>
+      </c>
+      <c r="C528" s="109"/>
+      <c r="D528" s="109"/>
+      <c r="E528" s="109"/>
+      <c r="F528" s="109"/>
+      <c r="G528" s="109"/>
+      <c r="H528" s="109"/>
+    </row>
+    <row r="529" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A529" s="85">
+        <v>43991</v>
+      </c>
+      <c r="B529" s="109"/>
+      <c r="C529" s="109"/>
+      <c r="D529" s="109"/>
+      <c r="E529" s="109"/>
+      <c r="F529" s="109"/>
+      <c r="G529" s="109"/>
+      <c r="H529" s="109"/>
+    </row>
+    <row r="530" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A530" s="85">
+        <v>43992</v>
+      </c>
+      <c r="B530" s="109"/>
+      <c r="C530" s="109"/>
+      <c r="D530" s="109"/>
+      <c r="E530" s="109"/>
+      <c r="F530" s="109"/>
+      <c r="G530" s="109"/>
+      <c r="H530" s="109"/>
+    </row>
+    <row r="531" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A531" s="85">
+        <v>43993</v>
+      </c>
+      <c r="B531" s="109"/>
+      <c r="C531" s="109"/>
+      <c r="D531" s="109"/>
+      <c r="E531" s="109"/>
+      <c r="F531" s="109"/>
+      <c r="G531" s="109"/>
+      <c r="H531" s="109"/>
+    </row>
+    <row r="532" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A532" s="85">
+        <v>43994</v>
+      </c>
+      <c r="B532" s="109"/>
+      <c r="C532" s="109"/>
+      <c r="D532" s="109"/>
+      <c r="E532" s="109"/>
+      <c r="F532" s="109"/>
+      <c r="G532" s="109"/>
+      <c r="H532" s="109"/>
+    </row>
+    <row r="533" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A533" s="85">
+        <v>43995</v>
+      </c>
+      <c r="B533" s="109"/>
+      <c r="C533" s="109"/>
+      <c r="D533" s="109"/>
+      <c r="E533" s="109"/>
+      <c r="F533" s="109"/>
+      <c r="G533" s="109"/>
+      <c r="H533" s="109"/>
+    </row>
+    <row r="534" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A534" s="85">
+        <v>43996</v>
+      </c>
+      <c r="B534" s="109"/>
+      <c r="C534" s="109"/>
+      <c r="D534" s="109"/>
+      <c r="E534" s="109"/>
+      <c r="F534" s="109"/>
+      <c r="G534" s="109"/>
+      <c r="H534" s="109"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -11949,11 +12066,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R527"/>
+  <dimension ref="A1:R534"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A507" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I523" sqref="I523"/>
+      <pane ySplit="3" topLeftCell="A515" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A537" sqref="A537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13951,7 +14068,9 @@
         <v>118.745</v>
       </c>
       <c r="Q43" s="99"/>
-      <c r="R43" s="99"/>
+      <c r="R43" s="99">
+        <v>689.6</v>
+      </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="85">
@@ -25684,8 +25803,12 @@
       <c r="B517" s="107">
         <v>7.6915300000000002</v>
       </c>
-      <c r="C517" s="107"/>
-      <c r="D517" s="107"/>
+      <c r="C517" s="107">
+        <v>149.69</v>
+      </c>
+      <c r="D517" s="107">
+        <v>25.85</v>
+      </c>
       <c r="E517" s="107"/>
       <c r="F517" s="107"/>
       <c r="G517" s="107"/>
@@ -25750,10 +25873,18 @@
       </c>
       <c r="C521" s="108"/>
       <c r="D521" s="108"/>
-      <c r="E521" s="108"/>
-      <c r="F521" s="108"/>
-      <c r="G521" s="108"/>
-      <c r="H521" s="108"/>
+      <c r="E521" s="108">
+        <v>18.98</v>
+      </c>
+      <c r="F521" s="108">
+        <v>17.97</v>
+      </c>
+      <c r="G521" s="108">
+        <v>14.7</v>
+      </c>
+      <c r="H521" s="108">
+        <v>10.199999999999999</v>
+      </c>
     </row>
     <row r="522" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A522" s="85">
@@ -25767,43 +25898,57 @@
       <c r="E522" s="108"/>
       <c r="F522" s="108"/>
       <c r="G522" s="108"/>
-      <c r="H522" s="108"/>
+      <c r="H522" s="108">
+        <v>10.050000000000001</v>
+      </c>
     </row>
     <row r="523" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A523" s="85">
         <v>43985</v>
       </c>
-      <c r="B523" s="108"/>
+      <c r="B523" s="108">
+        <v>7.6857100000000003</v>
+      </c>
       <c r="C523" s="108"/>
       <c r="D523" s="108"/>
       <c r="E523" s="108"/>
       <c r="F523" s="108"/>
       <c r="G523" s="108"/>
-      <c r="H523" s="108"/>
+      <c r="H523" s="108">
+        <v>10.050000000000001</v>
+      </c>
     </row>
     <row r="524" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A524" s="85">
         <v>43986</v>
       </c>
-      <c r="B524" s="108"/>
+      <c r="B524" s="108">
+        <v>7.6835000000000004</v>
+      </c>
       <c r="C524" s="108"/>
       <c r="D524" s="108"/>
       <c r="E524" s="108"/>
       <c r="F524" s="108"/>
       <c r="G524" s="108"/>
-      <c r="H524" s="108"/>
+      <c r="H524" s="108">
+        <v>10.050000000000001</v>
+      </c>
     </row>
     <row r="525" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A525" s="85">
         <v>43987</v>
       </c>
-      <c r="B525" s="108"/>
+      <c r="B525" s="108">
+        <v>7.6854100000000001</v>
+      </c>
       <c r="C525" s="108"/>
       <c r="D525" s="108"/>
       <c r="E525" s="108"/>
       <c r="F525" s="108"/>
       <c r="G525" s="108"/>
-      <c r="H525" s="108"/>
+      <c r="H525" s="108">
+        <v>10.050000000000001</v>
+      </c>
     </row>
     <row r="526" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A526" s="85">
@@ -25815,7 +25960,9 @@
       <c r="E526" s="108"/>
       <c r="F526" s="108"/>
       <c r="G526" s="108"/>
-      <c r="H526" s="108"/>
+      <c r="H526" s="108">
+        <v>10.050000000000001</v>
+      </c>
     </row>
     <row r="527" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A527" s="85">
@@ -25827,7 +25974,93 @@
       <c r="E527" s="108"/>
       <c r="F527" s="108"/>
       <c r="G527" s="108"/>
-      <c r="H527" s="108"/>
+      <c r="H527" s="108">
+        <v>10.050000000000001</v>
+      </c>
+    </row>
+    <row r="528" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A528" s="85">
+        <v>43990</v>
+      </c>
+      <c r="B528" s="109"/>
+      <c r="C528" s="109"/>
+      <c r="D528" s="109"/>
+      <c r="E528" s="109"/>
+      <c r="F528" s="109"/>
+      <c r="G528" s="109"/>
+      <c r="H528" s="109"/>
+    </row>
+    <row r="529" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A529" s="85">
+        <v>43991</v>
+      </c>
+      <c r="B529" s="109"/>
+      <c r="C529" s="109"/>
+      <c r="D529" s="109"/>
+      <c r="E529" s="109"/>
+      <c r="F529" s="109"/>
+      <c r="G529" s="109"/>
+      <c r="H529" s="109"/>
+    </row>
+    <row r="530" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A530" s="85">
+        <v>43992</v>
+      </c>
+      <c r="B530" s="109"/>
+      <c r="C530" s="109"/>
+      <c r="D530" s="109"/>
+      <c r="E530" s="109"/>
+      <c r="F530" s="109"/>
+      <c r="G530" s="109"/>
+      <c r="H530" s="109"/>
+    </row>
+    <row r="531" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A531" s="85">
+        <v>43993</v>
+      </c>
+      <c r="B531" s="109"/>
+      <c r="C531" s="109"/>
+      <c r="D531" s="109"/>
+      <c r="E531" s="109"/>
+      <c r="F531" s="109"/>
+      <c r="G531" s="109"/>
+      <c r="H531" s="109"/>
+    </row>
+    <row r="532" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A532" s="85">
+        <v>43994</v>
+      </c>
+      <c r="B532" s="109"/>
+      <c r="C532" s="109"/>
+      <c r="D532" s="109"/>
+      <c r="E532" s="109"/>
+      <c r="F532" s="109"/>
+      <c r="G532" s="109"/>
+      <c r="H532" s="109"/>
+    </row>
+    <row r="533" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A533" s="85">
+        <v>43995</v>
+      </c>
+      <c r="B533" s="109"/>
+      <c r="C533" s="109"/>
+      <c r="D533" s="109"/>
+      <c r="E533" s="109"/>
+      <c r="F533" s="109"/>
+      <c r="G533" s="109"/>
+      <c r="H533" s="109"/>
+    </row>
+    <row r="534" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A534" s="85">
+        <v>43996</v>
+      </c>
+      <c r="B534" s="109"/>
+      <c r="C534" s="109"/>
+      <c r="D534" s="109"/>
+      <c r="E534" s="109"/>
+      <c r="F534" s="109"/>
+      <c r="G534" s="109"/>
+      <c r="H534" s="109"/>
     </row>
   </sheetData>
   <phoneticPr fontId="39" type="noConversion"/>
@@ -25847,7 +26080,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-17-2020 02-24-35
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Guatemala/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="666" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BACA4CAA-0D77-4D76-9785-5C151C905BF4}"/>
+  <xr:revisionPtr revIDLastSave="686" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FC7578A-B474-41D2-82A4-9E071588B6AC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1202,27 +1202,6 @@
   </cellStyles>
   <dxfs count="29">
     <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1517,6 +1496,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1605,31 +1605,31 @@
   <autoFilter ref="A3:H541" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Café" dataDxfId="5" dataCellStyle="Millares [0]"/>
-    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Azúcar" dataDxfId="4" dataCellStyle="Millares [0]"/>
-    <tableColumn id="6" xr3:uid="{1A412D0D-9DDD-4532-ADAC-BC90F0ABB038}" name="Combustible Súper" dataDxfId="3" dataCellStyle="Millares [0]"/>
-    <tableColumn id="7" xr3:uid="{6C9802FB-03D0-4F94-9942-ED195CC86D50}" name="Combustible Regular" dataDxfId="2" dataCellStyle="Millares [0]"/>
-    <tableColumn id="8" xr3:uid="{EBFE959D-24EF-495E-9BE7-BDEC4C8061F8}" name="Combustible Diesel" dataDxfId="1" dataCellStyle="Millares [0]"/>
-    <tableColumn id="9" xr3:uid="{9FD84C7A-E59C-4373-B11B-E77745B4DBA6}" name="Combustible Kerosene" dataDxfId="0" dataCellStyle="Millares [0]"/>
+    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Café" dataDxfId="22" dataCellStyle="Millares [0]"/>
+    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Azúcar" dataDxfId="21" dataCellStyle="Millares [0]"/>
+    <tableColumn id="6" xr3:uid="{1A412D0D-9DDD-4532-ADAC-BC90F0ABB038}" name="Combustible Súper" dataDxfId="20" dataCellStyle="Millares [0]"/>
+    <tableColumn id="7" xr3:uid="{6C9802FB-03D0-4F94-9942-ED195CC86D50}" name="Combustible Regular" dataDxfId="19" dataCellStyle="Millares [0]"/>
+    <tableColumn id="8" xr3:uid="{EBFE959D-24EF-495E-9BE7-BDEC4C8061F8}" name="Combustible Diesel" dataDxfId="18" dataCellStyle="Millares [0]"/>
+    <tableColumn id="9" xr3:uid="{9FD84C7A-E59C-4373-B11B-E77745B4DBA6}" name="Combustible Kerosene" dataDxfId="17" dataCellStyle="Millares [0]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R46" totalsRowShown="0" headerRowDxfId="23" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R46" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R46" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="13">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{8FC1825F-E2AC-4830-AA41-5B12F2C15972}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Monto Inversión (millones de lempiras)" dataDxfId="19" dataCellStyle="Millares"/>
+    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Monto Inversión (millones de lempiras)" dataDxfId="12" dataCellStyle="Millares"/>
     <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Solicitudes Crédito"/>
-    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Monto Crédito (millones de lempiras)" dataDxfId="18" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Monto Crédito (millones de lempiras)" dataDxfId="11" dataCellStyle="Millares"/>
     <tableColumn id="8" xr3:uid="{1A570E63-F800-45DF-9E5A-B8961BEFE222}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{7E984A16-0976-4747-9D31-12709D8A9C2E}" name="Ingesos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1638,10 +1638,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H541" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H541" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A3:H541" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
     <tableColumn id="3" xr3:uid="{47070387-916A-43EA-9250-BD5CD00DE202}" name="Precio Café"/>
     <tableColumn id="4" xr3:uid="{017F8C94-7948-49FE-B245-F576C80EC85B}" name="Precio Azúcar"/>
@@ -1655,18 +1655,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R46" totalsRowShown="0" headerRowDxfId="15" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R46" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R46" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="5">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{B7D1225A-C849-430C-8F2C-569D3B5E64AD}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="11" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="10" dataCellStyle="Millares [0]"/>
-    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="9" dataCellStyle="Millares [0]"/>
+    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="4" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="3" dataCellStyle="Millares [0]"/>
+    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="2" dataCellStyle="Millares [0]"/>
     <tableColumn id="8" xr3:uid="{552CA574-1C46-4E0F-8C54-8DBCDA6B12C1}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{C793523A-103E-4CA7-94B8-3E3D9A633FDB}" name="Ingresos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1675,7 +1675,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="1">
   <autoFilter ref="A1:U36" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -1698,7 +1698,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1974,7 +1974,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H545" sqref="H545"/>
+      <selection pane="bottomLeft" activeCell="E543" sqref="E543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12391,10 +12391,10 @@
         <v>24.799299999999999</v>
       </c>
       <c r="C532" s="22">
-        <v>94.98</v>
+        <v>95.2</v>
       </c>
       <c r="D532" s="22">
-        <v>11.88</v>
+        <v>11.87</v>
       </c>
       <c r="E532" s="22">
         <v>75.849999999999994</v>
@@ -12440,8 +12440,12 @@
       <c r="B535" s="27">
         <v>24.790500000000002</v>
       </c>
-      <c r="C535" s="22"/>
-      <c r="D535" s="22"/>
+      <c r="C535" s="22">
+        <v>94</v>
+      </c>
+      <c r="D535" s="22">
+        <v>12.04</v>
+      </c>
       <c r="E535" s="22"/>
       <c r="F535" s="22"/>
       <c r="G535" s="22"/>
@@ -12451,9 +12455,15 @@
       <c r="A536" s="8">
         <v>43998</v>
       </c>
-      <c r="B536" s="27"/>
-      <c r="C536" s="22"/>
-      <c r="D536" s="22"/>
+      <c r="B536" s="27">
+        <v>24.7818</v>
+      </c>
+      <c r="C536" s="22">
+        <v>93.65</v>
+      </c>
+      <c r="D536" s="22">
+        <v>12.14</v>
+      </c>
       <c r="E536" s="22"/>
       <c r="F536" s="22"/>
       <c r="G536" s="22"/>
@@ -12463,7 +12473,9 @@
       <c r="A537" s="8">
         <v>43999</v>
       </c>
-      <c r="B537" s="27"/>
+      <c r="B537" s="27">
+        <v>24.773399999999999</v>
+      </c>
       <c r="C537" s="22"/>
       <c r="D537" s="22"/>
       <c r="E537" s="22"/>
@@ -12490,10 +12502,18 @@
       <c r="B539" s="27"/>
       <c r="C539" s="22"/>
       <c r="D539" s="22"/>
-      <c r="E539" s="22"/>
-      <c r="F539" s="22"/>
-      <c r="G539" s="22"/>
-      <c r="H539" s="22"/>
+      <c r="E539" s="22">
+        <v>77.59</v>
+      </c>
+      <c r="F539" s="22">
+        <v>69.42</v>
+      </c>
+      <c r="G539" s="22">
+        <v>59.31</v>
+      </c>
+      <c r="H539" s="22">
+        <v>39.1</v>
+      </c>
     </row>
     <row r="540" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A540" s="8">
@@ -12541,8 +12561,8 @@
   <dimension ref="A1:R541"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A543" sqref="A543"/>
+      <pane ySplit="3" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C544" sqref="C544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26665,7 +26685,9 @@
       <c r="A533" s="8">
         <v>43995</v>
       </c>
-      <c r="B533" s="27"/>
+      <c r="B533" s="27">
+        <v>7.7004099999999998</v>
+      </c>
       <c r="C533" s="27"/>
       <c r="D533" s="27"/>
       <c r="E533" s="27"/>
@@ -26679,7 +26701,9 @@
       <c r="A534" s="8">
         <v>43996</v>
       </c>
-      <c r="B534" s="27"/>
+      <c r="B534" s="27">
+        <v>7.7004099999999998</v>
+      </c>
       <c r="C534" s="27"/>
       <c r="D534" s="27"/>
       <c r="E534" s="27"/>
@@ -26693,19 +26717,29 @@
       <c r="A535" s="8">
         <v>43997</v>
       </c>
-      <c r="B535" s="27"/>
+      <c r="B535" s="27">
+        <v>7.7026199999999996</v>
+      </c>
       <c r="C535" s="27"/>
       <c r="D535" s="27"/>
-      <c r="E535" s="27"/>
-      <c r="F535" s="27"/>
-      <c r="G535" s="27"/>
+      <c r="E535" s="27">
+        <v>19.95</v>
+      </c>
+      <c r="F535" s="27">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="G535" s="27">
+        <v>15.18</v>
+      </c>
       <c r="H535" s="27"/>
     </row>
     <row r="536" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A536" s="8">
         <v>43998</v>
       </c>
-      <c r="B536" s="27"/>
+      <c r="B536" s="27">
+        <v>7.7079199999999997</v>
+      </c>
       <c r="C536" s="27"/>
       <c r="D536" s="27"/>
       <c r="E536" s="27"/>
@@ -26791,7 +26825,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-20-2020 02-31-29
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Guatemala/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="686" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FC7578A-B474-41D2-82A4-9E071588B6AC}"/>
+  <xr:revisionPtr revIDLastSave="711" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8F8E4AD4-C049-44E6-B6AE-697B112E1CEB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1601,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H541" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H541" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H548" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H548" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1638,8 +1638,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H541" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H541" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H548" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H548" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1970,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R541"/>
+  <dimension ref="A1:R548"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E543" sqref="E543"/>
+      <pane ySplit="3" topLeftCell="A535" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B550" sqref="B550"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12462,7 +12462,7 @@
         <v>93.65</v>
       </c>
       <c r="D536" s="22">
-        <v>12.14</v>
+        <v>12.19</v>
       </c>
       <c r="E536" s="22"/>
       <c r="F536" s="22"/>
@@ -12476,8 +12476,12 @@
       <c r="B537" s="27">
         <v>24.773399999999999</v>
       </c>
-      <c r="C537" s="22"/>
-      <c r="D537" s="22"/>
+      <c r="C537" s="22">
+        <v>96.25</v>
+      </c>
+      <c r="D537" s="22">
+        <v>12.11</v>
+      </c>
       <c r="E537" s="22"/>
       <c r="F537" s="22"/>
       <c r="G537" s="22"/>
@@ -12487,9 +12491,15 @@
       <c r="A538" s="8">
         <v>44000</v>
       </c>
-      <c r="B538" s="27"/>
-      <c r="C538" s="22"/>
-      <c r="D538" s="22"/>
+      <c r="B538" s="27">
+        <v>24.758900000000001</v>
+      </c>
+      <c r="C538" s="22">
+        <v>94.6</v>
+      </c>
+      <c r="D538" s="22">
+        <v>11.89</v>
+      </c>
       <c r="E538" s="22"/>
       <c r="F538" s="22"/>
       <c r="G538" s="22"/>
@@ -12499,9 +12509,15 @@
       <c r="A539" s="8">
         <v>44001</v>
       </c>
-      <c r="B539" s="27"/>
-      <c r="C539" s="22"/>
-      <c r="D539" s="22"/>
+      <c r="B539" s="27">
+        <v>24.7469</v>
+      </c>
+      <c r="C539" s="22">
+        <v>94.12</v>
+      </c>
+      <c r="D539" s="22">
+        <v>12.02</v>
+      </c>
       <c r="E539" s="22">
         <v>77.59</v>
       </c>
@@ -12538,6 +12554,92 @@
       <c r="F541" s="22"/>
       <c r="G541" s="22"/>
       <c r="H541" s="22"/>
+    </row>
+    <row r="542" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A542" s="8">
+        <v>44004</v>
+      </c>
+      <c r="B542" s="27">
+        <v>24.734300000000001</v>
+      </c>
+      <c r="C542" s="22"/>
+      <c r="D542" s="22"/>
+      <c r="E542" s="22"/>
+      <c r="F542" s="22"/>
+      <c r="G542" s="22"/>
+      <c r="H542" s="22"/>
+    </row>
+    <row r="543" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A543" s="8">
+        <v>44005</v>
+      </c>
+      <c r="B543" s="27"/>
+      <c r="C543" s="22"/>
+      <c r="D543" s="22"/>
+      <c r="E543" s="22"/>
+      <c r="F543" s="22"/>
+      <c r="G543" s="22"/>
+      <c r="H543" s="22"/>
+    </row>
+    <row r="544" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A544" s="8">
+        <v>44006</v>
+      </c>
+      <c r="B544" s="27"/>
+      <c r="C544" s="22"/>
+      <c r="D544" s="22"/>
+      <c r="E544" s="22"/>
+      <c r="F544" s="22"/>
+      <c r="G544" s="22"/>
+      <c r="H544" s="22"/>
+    </row>
+    <row r="545" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A545" s="8">
+        <v>44007</v>
+      </c>
+      <c r="B545" s="27"/>
+      <c r="C545" s="22"/>
+      <c r="D545" s="22"/>
+      <c r="E545" s="22"/>
+      <c r="F545" s="22"/>
+      <c r="G545" s="22"/>
+      <c r="H545" s="22"/>
+    </row>
+    <row r="546" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A546" s="8">
+        <v>44008</v>
+      </c>
+      <c r="B546" s="27"/>
+      <c r="C546" s="22"/>
+      <c r="D546" s="22"/>
+      <c r="E546" s="22"/>
+      <c r="F546" s="22"/>
+      <c r="G546" s="22"/>
+      <c r="H546" s="22"/>
+    </row>
+    <row r="547" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A547" s="8">
+        <v>44009</v>
+      </c>
+      <c r="B547" s="27"/>
+      <c r="C547" s="22"/>
+      <c r="D547" s="22"/>
+      <c r="E547" s="22"/>
+      <c r="F547" s="22"/>
+      <c r="G547" s="22"/>
+      <c r="H547" s="22"/>
+    </row>
+    <row r="548" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A548" s="8">
+        <v>44010</v>
+      </c>
+      <c r="B548" s="27"/>
+      <c r="C548" s="22"/>
+      <c r="D548" s="22"/>
+      <c r="E548" s="22"/>
+      <c r="F548" s="22"/>
+      <c r="G548" s="22"/>
+      <c r="H548" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -12558,11 +12660,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R541"/>
+  <dimension ref="A1:R548"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C544" sqref="C544"/>
+      <pane ySplit="3" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A563" sqref="A563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14699,7 +14801,7 @@
       <c r="M44" s="27"/>
       <c r="N44" s="27"/>
       <c r="O44" s="22">
-        <v>7609.8950000000004</v>
+        <v>7913.0232159999996</v>
       </c>
       <c r="P44" s="22">
         <v>140.26</v>
@@ -14745,8 +14847,12 @@
       </c>
       <c r="M45" s="27"/>
       <c r="N45" s="27"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="22"/>
+      <c r="O45" s="22">
+        <v>2442.7399999999998</v>
+      </c>
+      <c r="P45" s="22">
+        <v>193.79</v>
+      </c>
       <c r="Q45" s="27"/>
       <c r="R45" s="27"/>
     </row>
@@ -26731,7 +26837,9 @@
       <c r="G535" s="27">
         <v>15.18</v>
       </c>
-      <c r="H535" s="27"/>
+      <c r="H535" s="27">
+        <v>10.7</v>
+      </c>
     </row>
     <row r="536" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A536" s="8">
@@ -26745,43 +26853,57 @@
       <c r="E536" s="27"/>
       <c r="F536" s="27"/>
       <c r="G536" s="27"/>
-      <c r="H536" s="27"/>
+      <c r="H536" s="27">
+        <v>10.7</v>
+      </c>
     </row>
     <row r="537" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A537" s="8">
         <v>43999</v>
       </c>
-      <c r="B537" s="27"/>
+      <c r="B537" s="27">
+        <v>7.7046400000000004</v>
+      </c>
       <c r="C537" s="27"/>
       <c r="D537" s="27"/>
       <c r="E537" s="27"/>
       <c r="F537" s="27"/>
       <c r="G537" s="27"/>
-      <c r="H537" s="27"/>
+      <c r="H537" s="27">
+        <v>10.7</v>
+      </c>
     </row>
     <row r="538" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A538" s="8">
         <v>44000</v>
       </c>
-      <c r="B538" s="27"/>
+      <c r="B538" s="27">
+        <v>7.7064599999999999</v>
+      </c>
       <c r="C538" s="27"/>
       <c r="D538" s="27"/>
       <c r="E538" s="27"/>
       <c r="F538" s="27"/>
       <c r="G538" s="27"/>
-      <c r="H538" s="27"/>
+      <c r="H538" s="27">
+        <v>10.7</v>
+      </c>
     </row>
     <row r="539" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A539" s="8">
         <v>44001</v>
       </c>
-      <c r="B539" s="27"/>
+      <c r="B539" s="27">
+        <v>7.7086699999999997</v>
+      </c>
       <c r="C539" s="27"/>
       <c r="D539" s="27"/>
       <c r="E539" s="27"/>
       <c r="F539" s="27"/>
       <c r="G539" s="27"/>
-      <c r="H539" s="27"/>
+      <c r="H539" s="27">
+        <v>10.7</v>
+      </c>
     </row>
     <row r="540" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A540" s="8">
@@ -26793,7 +26915,9 @@
       <c r="E540" s="27"/>
       <c r="F540" s="27"/>
       <c r="G540" s="27"/>
-      <c r="H540" s="27"/>
+      <c r="H540" s="27">
+        <v>10.7</v>
+      </c>
     </row>
     <row r="541" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A541" s="8">
@@ -26805,7 +26929,44 @@
       <c r="E541" s="27"/>
       <c r="F541" s="27"/>
       <c r="G541" s="27"/>
-      <c r="H541" s="27"/>
+      <c r="H541" s="27">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="542" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A542" s="8">
+        <v>44004</v>
+      </c>
+    </row>
+    <row r="543" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A543" s="8">
+        <v>44005</v>
+      </c>
+    </row>
+    <row r="544" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A544" s="8">
+        <v>44006</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A545" s="8">
+        <v>44007</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A546" s="8">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A547" s="8">
+        <v>44009</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A548" s="8">
+        <v>44010</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="32" type="noConversion"/>
@@ -26825,7 +26986,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-24-2020 02-49-45
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Guatemala/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="711" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8F8E4AD4-C049-44E6-B6AE-697B112E1CEB}"/>
+  <xr:revisionPtr revIDLastSave="731" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4F05E9FA-B2A4-4DB2-B771-DBC9FC597906}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1974,7 +1974,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A535" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B550" sqref="B550"/>
+      <selection pane="bottomLeft" activeCell="B551" sqref="B551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12513,10 +12513,10 @@
         <v>24.7469</v>
       </c>
       <c r="C539" s="22">
-        <v>94.12</v>
+        <v>93.75</v>
       </c>
       <c r="D539" s="22">
-        <v>12.02</v>
+        <v>12.05</v>
       </c>
       <c r="E539" s="22">
         <v>77.59</v>
@@ -12562,8 +12562,12 @@
       <c r="B542" s="27">
         <v>24.734300000000001</v>
       </c>
-      <c r="C542" s="22"/>
-      <c r="D542" s="22"/>
+      <c r="C542" s="22">
+        <v>95.95</v>
+      </c>
+      <c r="D542" s="22">
+        <v>11.92</v>
+      </c>
       <c r="E542" s="22"/>
       <c r="F542" s="22"/>
       <c r="G542" s="22"/>
@@ -12573,9 +12577,15 @@
       <c r="A543" s="8">
         <v>44005</v>
       </c>
-      <c r="B543" s="27"/>
-      <c r="C543" s="22"/>
-      <c r="D543" s="22"/>
+      <c r="B543" s="27">
+        <v>24.7271</v>
+      </c>
+      <c r="C543" s="22">
+        <v>98.18</v>
+      </c>
+      <c r="D543" s="22">
+        <v>11.79</v>
+      </c>
       <c r="E543" s="22"/>
       <c r="F543" s="22"/>
       <c r="G543" s="22"/>
@@ -12585,7 +12595,9 @@
       <c r="A544" s="8">
         <v>44006</v>
       </c>
-      <c r="B544" s="27"/>
+      <c r="B544" s="27">
+        <v>24.712599999999998</v>
+      </c>
       <c r="C544" s="22"/>
       <c r="D544" s="22"/>
       <c r="E544" s="22"/>
@@ -12612,10 +12624,18 @@
       <c r="B546" s="27"/>
       <c r="C546" s="22"/>
       <c r="D546" s="22"/>
-      <c r="E546" s="22"/>
-      <c r="F546" s="22"/>
-      <c r="G546" s="22"/>
-      <c r="H546" s="22"/>
+      <c r="E546" s="22">
+        <v>78.73</v>
+      </c>
+      <c r="F546" s="22">
+        <v>71.27</v>
+      </c>
+      <c r="G546" s="22">
+        <v>60.75</v>
+      </c>
+      <c r="H546" s="22">
+        <v>40.57</v>
+      </c>
     </row>
     <row r="547" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A547" s="8">
@@ -12663,8 +12683,8 @@
   <dimension ref="A1:R548"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A563" sqref="A563"/>
+      <pane ySplit="3" topLeftCell="A531" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A550" sqref="A550"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26909,7 +26929,9 @@
       <c r="A540" s="8">
         <v>44002</v>
       </c>
-      <c r="B540" s="27"/>
+      <c r="B540" s="27">
+        <v>7.7086699999999997</v>
+      </c>
       <c r="C540" s="27"/>
       <c r="D540" s="27"/>
       <c r="E540" s="27"/>
@@ -26923,7 +26945,9 @@
       <c r="A541" s="8">
         <v>44003</v>
       </c>
-      <c r="B541" s="27"/>
+      <c r="B541" s="27">
+        <v>7.7086699999999997</v>
+      </c>
       <c r="C541" s="27"/>
       <c r="D541" s="27"/>
       <c r="E541" s="27"/>
@@ -26937,15 +26961,33 @@
       <c r="A542" s="8">
         <v>44004</v>
       </c>
+      <c r="B542" s="4">
+        <v>7.7035900000000002</v>
+      </c>
+      <c r="E542" s="4">
+        <v>20.69</v>
+      </c>
+      <c r="F542" s="4">
+        <v>19.88</v>
+      </c>
+      <c r="G542" s="4">
+        <v>15.8</v>
+      </c>
     </row>
     <row r="543" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A543" s="8">
         <v>44005</v>
       </c>
+      <c r="B543" s="4">
+        <v>7.6988899999999996</v>
+      </c>
     </row>
     <row r="544" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A544" s="8">
         <v>44006</v>
+      </c>
+      <c r="B544" s="4">
+        <v>7.7027999999999999</v>
       </c>
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.3">
@@ -26986,7 +27028,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-26-2020 23-59-00
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Guatemala/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="731" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4F05E9FA-B2A4-4DB2-B771-DBC9FC597906}"/>
+  <xr:revisionPtr revIDLastSave="758" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F6425536-2F55-4CE4-A73B-70F6E2601396}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8412" yWindow="0" windowWidth="14616" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="133">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1600,9 +1600,57 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>541</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>11375</xdr:colOff>
+      <xdr:row>562</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D613A986-B0E6-44E5-82F1-E19BC08A4A54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect b="22713"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8145782" y="99852480"/>
+          <a:ext cx="5269173" cy="3863340"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H548" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H548" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H555" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H555" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1618,8 +1666,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R46" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R46" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R47" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R47" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="14"/>
@@ -1638,8 +1686,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H548" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H548" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H555" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H555" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1655,8 +1703,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R46" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R46" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R47" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R47" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="6"/>
@@ -1970,11 +2018,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R548"/>
+  <dimension ref="A1:R555"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A535" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B551" sqref="B551"/>
+      <pane ySplit="3" topLeftCell="A540" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B558" sqref="B558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3915,7 +3963,9 @@
         <v>650</v>
       </c>
       <c r="Q44" s="27"/>
-      <c r="R44" s="27"/>
+      <c r="R44" s="27">
+        <v>329.8</v>
+      </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
@@ -3950,7 +4000,9 @@
       <c r="O45" s="27"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="27"/>
-      <c r="R45" s="27"/>
+      <c r="R45" s="27">
+        <v>412.7</v>
+      </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
@@ -3977,7 +4029,7 @@
         <v>27</v>
       </c>
       <c r="L46" s="9" t="str">
-        <f t="shared" ref="L46" si="2">+K46&amp;", "&amp;J46</f>
+        <f t="shared" ref="L46:L47" si="2">+K46&amp;", "&amp;J46</f>
         <v>Julio, 2020</v>
       </c>
       <c r="M46" s="27"/>
@@ -4005,13 +4057,20 @@
       <c r="G47" s="22"/>
       <c r="H47" s="22"/>
       <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="27"/>
+      <c r="J47" s="9">
+        <v>2020</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L47" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>Agosto, 2020</v>
+      </c>
       <c r="M47" s="27"/>
-      <c r="N47" s="27"/>
+      <c r="N47" s="2"/>
       <c r="O47" s="27"/>
-      <c r="P47" s="27"/>
+      <c r="P47" s="2"/>
       <c r="Q47" s="27"/>
       <c r="R47" s="27"/>
     </row>
@@ -12581,7 +12640,7 @@
         <v>24.7271</v>
       </c>
       <c r="C543" s="22">
-        <v>98.18</v>
+        <v>96.25</v>
       </c>
       <c r="D543" s="22">
         <v>11.79</v>
@@ -12598,8 +12657,12 @@
       <c r="B544" s="27">
         <v>24.712599999999998</v>
       </c>
-      <c r="C544" s="22"/>
-      <c r="D544" s="22"/>
+      <c r="C544" s="22">
+        <v>96.65</v>
+      </c>
+      <c r="D544" s="22">
+        <v>11.75</v>
+      </c>
       <c r="E544" s="22"/>
       <c r="F544" s="22"/>
       <c r="G544" s="22"/>
@@ -12609,9 +12672,15 @@
       <c r="A545" s="8">
         <v>44007</v>
       </c>
-      <c r="B545" s="27"/>
-      <c r="C545" s="22"/>
-      <c r="D545" s="22"/>
+      <c r="B545" s="27">
+        <v>24.711400000000001</v>
+      </c>
+      <c r="C545" s="22">
+        <v>94.85</v>
+      </c>
+      <c r="D545" s="22">
+        <v>11.81</v>
+      </c>
       <c r="E545" s="22"/>
       <c r="F545" s="22"/>
       <c r="G545" s="22"/>
@@ -12621,9 +12690,15 @@
       <c r="A546" s="8">
         <v>44008</v>
       </c>
-      <c r="B546" s="27"/>
-      <c r="C546" s="22"/>
-      <c r="D546" s="22"/>
+      <c r="B546" s="27">
+        <v>24.7135</v>
+      </c>
+      <c r="C546" s="22">
+        <v>96.63</v>
+      </c>
+      <c r="D546" s="22">
+        <v>11.52</v>
+      </c>
       <c r="E546" s="22">
         <v>78.73</v>
       </c>
@@ -12660,6 +12735,92 @@
       <c r="F548" s="22"/>
       <c r="G548" s="22"/>
       <c r="H548" s="22"/>
+    </row>
+    <row r="549" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A549" s="8">
+        <v>44011</v>
+      </c>
+      <c r="B549" s="27">
+        <v>24.717099999999999</v>
+      </c>
+      <c r="C549" s="22"/>
+      <c r="D549" s="22"/>
+      <c r="E549" s="22"/>
+      <c r="F549" s="22"/>
+      <c r="G549" s="22"/>
+      <c r="H549" s="22"/>
+    </row>
+    <row r="550" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A550" s="8">
+        <v>44012</v>
+      </c>
+      <c r="B550" s="28"/>
+      <c r="C550" s="22"/>
+      <c r="D550" s="22"/>
+      <c r="E550" s="22"/>
+      <c r="F550" s="22"/>
+      <c r="G550" s="22"/>
+      <c r="H550" s="22"/>
+    </row>
+    <row r="551" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A551" s="8">
+        <v>44013</v>
+      </c>
+      <c r="B551" s="28"/>
+      <c r="C551" s="22"/>
+      <c r="D551" s="22"/>
+      <c r="E551" s="22"/>
+      <c r="F551" s="22"/>
+      <c r="G551" s="22"/>
+      <c r="H551" s="22"/>
+    </row>
+    <row r="552" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A552" s="8">
+        <v>44014</v>
+      </c>
+      <c r="B552" s="28"/>
+      <c r="C552" s="22"/>
+      <c r="D552" s="22"/>
+      <c r="E552" s="22"/>
+      <c r="F552" s="22"/>
+      <c r="G552" s="22"/>
+      <c r="H552" s="22"/>
+    </row>
+    <row r="553" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A553" s="8">
+        <v>44015</v>
+      </c>
+      <c r="B553" s="28"/>
+      <c r="C553" s="22"/>
+      <c r="D553" s="22"/>
+      <c r="E553" s="22"/>
+      <c r="F553" s="22"/>
+      <c r="G553" s="22"/>
+      <c r="H553" s="22"/>
+    </row>
+    <row r="554" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A554" s="8">
+        <v>44016</v>
+      </c>
+      <c r="B554" s="28"/>
+      <c r="C554" s="22"/>
+      <c r="D554" s="22"/>
+      <c r="E554" s="22"/>
+      <c r="F554" s="22"/>
+      <c r="G554" s="22"/>
+      <c r="H554" s="22"/>
+    </row>
+    <row r="555" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A555" s="8">
+        <v>44017</v>
+      </c>
+      <c r="B555" s="28"/>
+      <c r="C555" s="22"/>
+      <c r="D555" s="22"/>
+      <c r="E555" s="22"/>
+      <c r="F555" s="22"/>
+      <c r="G555" s="22"/>
+      <c r="H555" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -12680,11 +12841,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R548"/>
+  <dimension ref="A1:R555"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A531" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A550" sqref="A550"/>
+      <pane ySplit="3" topLeftCell="A540" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A557" sqref="A557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14909,7 +15070,7 @@
         <v>27</v>
       </c>
       <c r="L46" s="9" t="str">
-        <f t="shared" ref="L46" si="2">+K46&amp;", "&amp;J46</f>
+        <f t="shared" ref="L46:L47" si="2">+K46&amp;", "&amp;J46</f>
         <v>Julio, 2020</v>
       </c>
       <c r="M46" s="27"/>
@@ -14945,13 +15106,20 @@
         <v>15.15</v>
       </c>
       <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="27"/>
+      <c r="J47" s="9">
+        <v>2020</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L47" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>Agosto, 2020</v>
+      </c>
       <c r="M47" s="27"/>
-      <c r="N47" s="27"/>
-      <c r="O47" s="27"/>
-      <c r="P47" s="27"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="22"/>
+      <c r="P47" s="22"/>
       <c r="Q47" s="27"/>
       <c r="R47" s="27"/>
     </row>
@@ -26990,32 +27158,96 @@
         <v>7.7027999999999999</v>
       </c>
     </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A545" s="8">
         <v>44007</v>
       </c>
-    </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B545" s="4">
+        <v>7.7002800000000002</v>
+      </c>
+    </row>
+    <row r="546" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A546" s="8">
         <v>44008</v>
       </c>
-    </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B546" s="4">
+        <v>7.7002600000000001</v>
+      </c>
+    </row>
+    <row r="547" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A547" s="8">
         <v>44009</v>
       </c>
-    </row>
-    <row r="548" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B547" s="4">
+        <v>7.7002600000000001</v>
+      </c>
+    </row>
+    <row r="548" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A548" s="8">
         <v>44010</v>
       </c>
+      <c r="B548" s="4">
+        <v>7.7002600000000001</v>
+      </c>
+    </row>
+    <row r="549" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A549" s="8">
+        <v>44011</v>
+      </c>
+      <c r="B549" s="4">
+        <v>7.7002600000000001</v>
+      </c>
+      <c r="H549" s="27"/>
+    </row>
+    <row r="550" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A550" s="8">
+        <v>44012</v>
+      </c>
+      <c r="B550" s="4">
+        <v>7.7002600000000001</v>
+      </c>
+      <c r="H550" s="27"/>
+    </row>
+    <row r="551" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A551" s="8">
+        <v>44013</v>
+      </c>
+      <c r="B551" s="4">
+        <v>7.7042099999999998</v>
+      </c>
+      <c r="H551" s="27"/>
+    </row>
+    <row r="552" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A552" s="8">
+        <v>44014</v>
+      </c>
+      <c r="H552" s="27"/>
+    </row>
+    <row r="553" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A553" s="8">
+        <v>44015</v>
+      </c>
+      <c r="H553" s="27"/>
+    </row>
+    <row r="554" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A554" s="8">
+        <v>44016</v>
+      </c>
+      <c r="H554" s="27"/>
+    </row>
+    <row r="555" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A555" s="8">
+        <v>44017</v>
+      </c>
+      <c r="H555" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -27025,10 +27257,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-01-2020 00-11-12
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Guatemala/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="758" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F6425536-2F55-4CE4-A73B-70F6E2601396}"/>
+  <xr:revisionPtr revIDLastSave="782" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3AEE20DC-AFA0-47A5-9139-3E38BBEE2B8A}"/>
   <bookViews>
-    <workbookView xWindow="8412" yWindow="0" windowWidth="14616" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7992" yWindow="0" windowWidth="15024" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -1202,6 +1202,68 @@
   </cellStyles>
   <dxfs count="29">
     <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF5D7B9D"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1496,68 +1558,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF5D7B9D"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD9E2F3"/>
@@ -1600,84 +1600,36 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2</xdr:colOff>
-      <xdr:row>541</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>11375</xdr:colOff>
-      <xdr:row>562</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D613A986-B0E6-44E5-82F1-E19BC08A4A54}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect b="22713"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8145782" y="99852480"/>
-          <a:ext cx="5269173" cy="3863340"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H555" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H555" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H562" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A3:H562" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Café" dataDxfId="22" dataCellStyle="Millares [0]"/>
-    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Azúcar" dataDxfId="21" dataCellStyle="Millares [0]"/>
-    <tableColumn id="6" xr3:uid="{1A412D0D-9DDD-4532-ADAC-BC90F0ABB038}" name="Combustible Súper" dataDxfId="20" dataCellStyle="Millares [0]"/>
-    <tableColumn id="7" xr3:uid="{6C9802FB-03D0-4F94-9942-ED195CC86D50}" name="Combustible Regular" dataDxfId="19" dataCellStyle="Millares [0]"/>
-    <tableColumn id="8" xr3:uid="{EBFE959D-24EF-495E-9BE7-BDEC4C8061F8}" name="Combustible Diesel" dataDxfId="18" dataCellStyle="Millares [0]"/>
-    <tableColumn id="9" xr3:uid="{9FD84C7A-E59C-4373-B11B-E77745B4DBA6}" name="Combustible Kerosene" dataDxfId="17" dataCellStyle="Millares [0]"/>
+    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Café" dataDxfId="5" dataCellStyle="Millares [0]"/>
+    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Azúcar" dataDxfId="4" dataCellStyle="Millares [0]"/>
+    <tableColumn id="6" xr3:uid="{1A412D0D-9DDD-4532-ADAC-BC90F0ABB038}" name="Combustible Súper" dataDxfId="3" dataCellStyle="Millares [0]"/>
+    <tableColumn id="7" xr3:uid="{6C9802FB-03D0-4F94-9942-ED195CC86D50}" name="Combustible Regular" dataDxfId="2" dataCellStyle="Millares [0]"/>
+    <tableColumn id="8" xr3:uid="{EBFE959D-24EF-495E-9BE7-BDEC4C8061F8}" name="Combustible Diesel" dataDxfId="1" dataCellStyle="Millares [0]"/>
+    <tableColumn id="9" xr3:uid="{9FD84C7A-E59C-4373-B11B-E77745B4DBA6}" name="Combustible Kerosene" dataDxfId="0" dataCellStyle="Millares [0]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R47" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R47" totalsRowShown="0" headerRowDxfId="25" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R47" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="22">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{8FC1825F-E2AC-4830-AA41-5B12F2C15972}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Monto Inversión (millones de lempiras)" dataDxfId="12" dataCellStyle="Millares"/>
+    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Monto Inversión (millones de lempiras)" dataDxfId="21" dataCellStyle="Millares"/>
     <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Solicitudes Crédito"/>
-    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Monto Crédito (millones de lempiras)" dataDxfId="11" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Monto Crédito (millones de lempiras)" dataDxfId="20" dataCellStyle="Millares"/>
     <tableColumn id="8" xr3:uid="{1A570E63-F800-45DF-9E5A-B8961BEFE222}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{7E984A16-0976-4747-9D31-12709D8A9C2E}" name="Ingesos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1686,10 +1638,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H555" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H555" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="A3:H555" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="18"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
     <tableColumn id="3" xr3:uid="{47070387-916A-43EA-9250-BD5CD00DE202}" name="Precio Café"/>
     <tableColumn id="4" xr3:uid="{017F8C94-7948-49FE-B245-F576C80EC85B}" name="Precio Azúcar"/>
@@ -1703,18 +1655,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R47" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R47" totalsRowShown="0" headerRowDxfId="17" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R47" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="14">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{B7D1225A-C849-430C-8F2C-569D3B5E64AD}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="4" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="3" dataCellStyle="Millares [0]"/>
-    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="2" dataCellStyle="Millares [0]"/>
+    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="13" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="12" dataCellStyle="Millares [0]"/>
+    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="11" dataCellStyle="Millares [0]"/>
     <tableColumn id="8" xr3:uid="{552CA574-1C46-4E0F-8C54-8DBCDA6B12C1}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{C793523A-103E-4CA7-94B8-3E3D9A633FDB}" name="Ingresos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1723,7 +1675,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="10">
   <autoFilter ref="A1:U36" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -1746,7 +1698,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2018,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R555"/>
+  <dimension ref="A1:R562"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A540" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B558" sqref="B558"/>
+      <pane ySplit="3" topLeftCell="A543" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B565" sqref="B565"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12694,10 +12646,10 @@
         <v>24.7135</v>
       </c>
       <c r="C546" s="22">
-        <v>96.63</v>
+        <v>95.65</v>
       </c>
       <c r="D546" s="22">
-        <v>11.52</v>
+        <v>11.55</v>
       </c>
       <c r="E546" s="22">
         <v>78.73</v>
@@ -12743,8 +12695,12 @@
       <c r="B549" s="27">
         <v>24.717099999999999</v>
       </c>
-      <c r="C549" s="22"/>
-      <c r="D549" s="22"/>
+      <c r="C549" s="22">
+        <v>98.65</v>
+      </c>
+      <c r="D549" s="22">
+        <v>11.71</v>
+      </c>
       <c r="E549" s="22"/>
       <c r="F549" s="22"/>
       <c r="G549" s="22"/>
@@ -12754,9 +12710,15 @@
       <c r="A550" s="8">
         <v>44012</v>
       </c>
-      <c r="B550" s="28"/>
-      <c r="C550" s="22"/>
-      <c r="D550" s="22"/>
+      <c r="B550" s="28">
+        <v>24.7149</v>
+      </c>
+      <c r="C550" s="22">
+        <v>101.13</v>
+      </c>
+      <c r="D550" s="22">
+        <v>11.93</v>
+      </c>
       <c r="E550" s="22"/>
       <c r="F550" s="22"/>
       <c r="G550" s="22"/>
@@ -12766,7 +12728,9 @@
       <c r="A551" s="8">
         <v>44013</v>
       </c>
-      <c r="B551" s="28"/>
+      <c r="B551" s="28">
+        <v>24.71</v>
+      </c>
       <c r="C551" s="22"/>
       <c r="D551" s="22"/>
       <c r="E551" s="22"/>
@@ -12817,10 +12781,102 @@
       <c r="B555" s="28"/>
       <c r="C555" s="22"/>
       <c r="D555" s="22"/>
-      <c r="E555" s="22"/>
-      <c r="F555" s="22"/>
-      <c r="G555" s="22"/>
-      <c r="H555" s="22"/>
+      <c r="E555" s="22">
+        <v>79.83</v>
+      </c>
+      <c r="F555" s="22">
+        <v>72.56</v>
+      </c>
+      <c r="G555" s="22">
+        <v>61.85</v>
+      </c>
+      <c r="H555" s="22">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="556" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A556" s="8">
+        <v>44018</v>
+      </c>
+      <c r="B556" s="28"/>
+      <c r="C556" s="22"/>
+      <c r="D556" s="22"/>
+      <c r="E556" s="22"/>
+      <c r="F556" s="22"/>
+      <c r="G556" s="22"/>
+      <c r="H556" s="22"/>
+    </row>
+    <row r="557" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A557" s="8">
+        <v>44019</v>
+      </c>
+      <c r="B557" s="28"/>
+      <c r="C557" s="22"/>
+      <c r="D557" s="22"/>
+      <c r="E557" s="22"/>
+      <c r="F557" s="22"/>
+      <c r="G557" s="22"/>
+      <c r="H557" s="22"/>
+    </row>
+    <row r="558" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A558" s="8">
+        <v>44020</v>
+      </c>
+      <c r="B558" s="28"/>
+      <c r="C558" s="22"/>
+      <c r="D558" s="22"/>
+      <c r="E558" s="22"/>
+      <c r="F558" s="22"/>
+      <c r="G558" s="22"/>
+      <c r="H558" s="22"/>
+    </row>
+    <row r="559" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A559" s="8">
+        <v>44021</v>
+      </c>
+      <c r="B559" s="28"/>
+      <c r="C559" s="22"/>
+      <c r="D559" s="22"/>
+      <c r="E559" s="22"/>
+      <c r="F559" s="22"/>
+      <c r="G559" s="22"/>
+      <c r="H559" s="22"/>
+    </row>
+    <row r="560" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A560" s="8">
+        <v>44022</v>
+      </c>
+      <c r="B560" s="28"/>
+      <c r="C560" s="22"/>
+      <c r="D560" s="22"/>
+      <c r="E560" s="22"/>
+      <c r="F560" s="22"/>
+      <c r="G560" s="22"/>
+      <c r="H560" s="22"/>
+    </row>
+    <row r="561" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A561" s="8">
+        <v>44023</v>
+      </c>
+      <c r="B561" s="28"/>
+      <c r="C561" s="22"/>
+      <c r="D561" s="22"/>
+      <c r="E561" s="22"/>
+      <c r="F561" s="22"/>
+      <c r="G561" s="22"/>
+      <c r="H561" s="22"/>
+    </row>
+    <row r="562" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A562" s="8">
+        <v>44024</v>
+      </c>
+      <c r="B562" s="28"/>
+      <c r="C562" s="22"/>
+      <c r="D562" s="22"/>
+      <c r="E562" s="22"/>
+      <c r="F562" s="22"/>
+      <c r="G562" s="22"/>
+      <c r="H562" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -12844,8 +12900,8 @@
   <dimension ref="A1:R555"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A540" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A557" sqref="A557"/>
+      <pane ySplit="3" topLeftCell="A544" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A565" sqref="A565"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27141,6 +27197,9 @@
       <c r="G542" s="4">
         <v>15.8</v>
       </c>
+      <c r="H542" s="4">
+        <v>10.9</v>
+      </c>
     </row>
     <row r="543" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A543" s="8">
@@ -27149,6 +27208,9 @@
       <c r="B543" s="4">
         <v>7.6988899999999996</v>
       </c>
+      <c r="H543" s="4">
+        <v>10.9</v>
+      </c>
     </row>
     <row r="544" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A544" s="8">
@@ -27157,6 +27219,9 @@
       <c r="B544" s="4">
         <v>7.7027999999999999</v>
       </c>
+      <c r="H544" s="4">
+        <v>10.9</v>
+      </c>
     </row>
     <row r="545" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A545" s="8">
@@ -27165,6 +27230,9 @@
       <c r="B545" s="4">
         <v>7.7002800000000002</v>
       </c>
+      <c r="H545" s="4">
+        <v>10.9</v>
+      </c>
     </row>
     <row r="546" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A546" s="8">
@@ -27173,6 +27241,9 @@
       <c r="B546" s="4">
         <v>7.7002600000000001</v>
       </c>
+      <c r="H546" s="4">
+        <v>10.9</v>
+      </c>
     </row>
     <row r="547" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A547" s="8">
@@ -27181,6 +27252,9 @@
       <c r="B547" s="4">
         <v>7.7002600000000001</v>
       </c>
+      <c r="H547" s="4">
+        <v>10.9</v>
+      </c>
     </row>
     <row r="548" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A548" s="8">
@@ -27189,6 +27263,9 @@
       <c r="B548" s="4">
         <v>7.7002600000000001</v>
       </c>
+      <c r="H548" s="4">
+        <v>10.9</v>
+      </c>
     </row>
     <row r="549" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A549" s="8">
@@ -27197,6 +27274,15 @@
       <c r="B549" s="4">
         <v>7.7002600000000001</v>
       </c>
+      <c r="E549" s="4">
+        <v>22.16</v>
+      </c>
+      <c r="F549" s="4">
+        <v>21.35</v>
+      </c>
+      <c r="G549" s="4">
+        <v>17.25</v>
+      </c>
       <c r="H549" s="27"/>
     </row>
     <row r="550" spans="1:8" x14ac:dyDescent="0.3">
@@ -27244,10 +27330,9 @@
   </sheetData>
   <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
   <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -27260,7 +27345,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-04-2020 02-31-39
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Guatemala/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="782" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3AEE20DC-AFA0-47A5-9139-3E38BBEE2B8A}"/>
+  <xr:revisionPtr revIDLastSave="803" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DB5521D0-6C0F-493B-B9B8-5EBF8E14D94C}"/>
   <bookViews>
-    <workbookView xWindow="7992" yWindow="0" windowWidth="15024" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8208" yWindow="0" windowWidth="14808" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -1202,68 +1202,6 @@
   </cellStyles>
   <dxfs count="29">
     <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF5D7B9D"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1558,6 +1496,68 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF5D7B9D"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD9E2F3"/>
@@ -1601,35 +1601,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H562" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H562" totalsRowShown="0" headerRowDxfId="25">
   <autoFilter ref="A3:H562" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Café" dataDxfId="5" dataCellStyle="Millares [0]"/>
-    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Azúcar" dataDxfId="4" dataCellStyle="Millares [0]"/>
-    <tableColumn id="6" xr3:uid="{1A412D0D-9DDD-4532-ADAC-BC90F0ABB038}" name="Combustible Súper" dataDxfId="3" dataCellStyle="Millares [0]"/>
-    <tableColumn id="7" xr3:uid="{6C9802FB-03D0-4F94-9942-ED195CC86D50}" name="Combustible Regular" dataDxfId="2" dataCellStyle="Millares [0]"/>
-    <tableColumn id="8" xr3:uid="{EBFE959D-24EF-495E-9BE7-BDEC4C8061F8}" name="Combustible Diesel" dataDxfId="1" dataCellStyle="Millares [0]"/>
-    <tableColumn id="9" xr3:uid="{9FD84C7A-E59C-4373-B11B-E77745B4DBA6}" name="Combustible Kerosene" dataDxfId="0" dataCellStyle="Millares [0]"/>
+    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Café" dataDxfId="22" dataCellStyle="Millares [0]"/>
+    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Azúcar" dataDxfId="21" dataCellStyle="Millares [0]"/>
+    <tableColumn id="6" xr3:uid="{1A412D0D-9DDD-4532-ADAC-BC90F0ABB038}" name="Combustible Súper" dataDxfId="20" dataCellStyle="Millares [0]"/>
+    <tableColumn id="7" xr3:uid="{6C9802FB-03D0-4F94-9942-ED195CC86D50}" name="Combustible Regular" dataDxfId="19" dataCellStyle="Millares [0]"/>
+    <tableColumn id="8" xr3:uid="{EBFE959D-24EF-495E-9BE7-BDEC4C8061F8}" name="Combustible Diesel" dataDxfId="18" dataCellStyle="Millares [0]"/>
+    <tableColumn id="9" xr3:uid="{9FD84C7A-E59C-4373-B11B-E77745B4DBA6}" name="Combustible Kerosene" dataDxfId="17" dataCellStyle="Millares [0]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R47" totalsRowShown="0" headerRowDxfId="25" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R47" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R47" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="13">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{8FC1825F-E2AC-4830-AA41-5B12F2C15972}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Monto Inversión (millones de lempiras)" dataDxfId="21" dataCellStyle="Millares"/>
+    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Monto Inversión (millones de lempiras)" dataDxfId="12" dataCellStyle="Millares"/>
     <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Solicitudes Crédito"/>
-    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Monto Crédito (millones de lempiras)" dataDxfId="20" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Monto Crédito (millones de lempiras)" dataDxfId="11" dataCellStyle="Millares"/>
     <tableColumn id="8" xr3:uid="{1A570E63-F800-45DF-9E5A-B8961BEFE222}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{7E984A16-0976-4747-9D31-12709D8A9C2E}" name="Ingesos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1638,10 +1638,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H555" totalsRowShown="0" headerRowDxfId="19">
-  <autoFilter ref="A3:H555" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H562" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H562" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
     <tableColumn id="3" xr3:uid="{47070387-916A-43EA-9250-BD5CD00DE202}" name="Precio Café"/>
     <tableColumn id="4" xr3:uid="{017F8C94-7948-49FE-B245-F576C80EC85B}" name="Precio Azúcar"/>
@@ -1655,18 +1655,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R47" totalsRowShown="0" headerRowDxfId="17" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R47" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R47" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="5">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{B7D1225A-C849-430C-8F2C-569D3B5E64AD}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="13" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="12" dataCellStyle="Millares [0]"/>
-    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="11" dataCellStyle="Millares [0]"/>
+    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="4" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="3" dataCellStyle="Millares [0]"/>
+    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="2" dataCellStyle="Millares [0]"/>
     <tableColumn id="8" xr3:uid="{552CA574-1C46-4E0F-8C54-8DBCDA6B12C1}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{C793523A-103E-4CA7-94B8-3E3D9A633FDB}" name="Ingresos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1675,7 +1675,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="1">
   <autoFilter ref="A1:U36" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -1698,7 +1698,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1973,8 +1973,8 @@
   <dimension ref="A1:R562"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A543" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B565" sqref="B565"/>
+      <pane ySplit="3" topLeftCell="A546" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D565" sqref="D565"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3949,8 +3949,12 @@
       </c>
       <c r="M45" s="27"/>
       <c r="N45" s="2"/>
-      <c r="O45" s="27"/>
-      <c r="P45" s="2"/>
+      <c r="O45" s="27">
+        <v>1</v>
+      </c>
+      <c r="P45" s="2">
+        <v>500</v>
+      </c>
       <c r="Q45" s="27"/>
       <c r="R45" s="27">
         <v>412.7</v>
@@ -12714,10 +12718,10 @@
         <v>24.7149</v>
       </c>
       <c r="C550" s="22">
-        <v>101.13</v>
+        <v>100.05</v>
       </c>
       <c r="D550" s="22">
-        <v>11.93</v>
+        <v>11.84</v>
       </c>
       <c r="E550" s="22"/>
       <c r="F550" s="22"/>
@@ -12731,8 +12735,12 @@
       <c r="B551" s="28">
         <v>24.71</v>
       </c>
-      <c r="C551" s="22"/>
-      <c r="D551" s="22"/>
+      <c r="C551" s="22">
+        <v>103.05</v>
+      </c>
+      <c r="D551" s="22">
+        <v>12.17</v>
+      </c>
       <c r="E551" s="22"/>
       <c r="F551" s="22"/>
       <c r="G551" s="22"/>
@@ -12742,9 +12750,15 @@
       <c r="A552" s="8">
         <v>44014</v>
       </c>
-      <c r="B552" s="28"/>
-      <c r="C552" s="22"/>
-      <c r="D552" s="22"/>
+      <c r="B552" s="28">
+        <v>24.710100000000001</v>
+      </c>
+      <c r="C552" s="22">
+        <v>102.25</v>
+      </c>
+      <c r="D552" s="22">
+        <v>12.24</v>
+      </c>
       <c r="E552" s="22"/>
       <c r="F552" s="22"/>
       <c r="G552" s="22"/>
@@ -12754,7 +12768,9 @@
       <c r="A553" s="8">
         <v>44015</v>
       </c>
-      <c r="B553" s="28"/>
+      <c r="B553" s="28">
+        <v>24.706399999999999</v>
+      </c>
       <c r="C553" s="22"/>
       <c r="D553" s="22"/>
       <c r="E553" s="22"/>
@@ -12798,7 +12814,9 @@
       <c r="A556" s="8">
         <v>44018</v>
       </c>
-      <c r="B556" s="28"/>
+      <c r="B556" s="28">
+        <v>24.703700000000001</v>
+      </c>
       <c r="C556" s="22"/>
       <c r="D556" s="22"/>
       <c r="E556" s="22"/>
@@ -12897,11 +12915,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R555"/>
+  <dimension ref="A1:R562"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A544" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A565" sqref="A565"/>
+      <pane ySplit="3" topLeftCell="A545" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A566" sqref="A566"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14996,7 +15014,7 @@
       </c>
       <c r="Q43" s="27"/>
       <c r="R43" s="27">
-        <v>689.6</v>
+        <v>690.6</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
@@ -15044,7 +15062,9 @@
         <v>140.26</v>
       </c>
       <c r="Q44" s="27"/>
-      <c r="R44" s="27"/>
+      <c r="R44" s="27">
+        <v>836.6</v>
+      </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
@@ -15085,10 +15105,10 @@
       <c r="M45" s="27"/>
       <c r="N45" s="27"/>
       <c r="O45" s="22">
-        <v>2442.7399999999998</v>
+        <v>3698.3909100000001</v>
       </c>
       <c r="P45" s="22">
-        <v>193.79</v>
+        <v>214.45</v>
       </c>
       <c r="Q45" s="27"/>
       <c r="R45" s="27"/>
@@ -15131,8 +15151,12 @@
       </c>
       <c r="M46" s="27"/>
       <c r="N46" s="27"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="22"/>
+      <c r="O46" s="22">
+        <v>355.57</v>
+      </c>
+      <c r="P46" s="22">
+        <v>41.19</v>
+      </c>
       <c r="Q46" s="27"/>
       <c r="R46" s="27"/>
     </row>
@@ -27283,7 +27307,9 @@
       <c r="G549" s="4">
         <v>17.25</v>
       </c>
-      <c r="H549" s="27"/>
+      <c r="H549" s="27">
+        <v>10.98</v>
+      </c>
     </row>
     <row r="550" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A550" s="8">
@@ -27292,7 +27318,9 @@
       <c r="B550" s="4">
         <v>7.7002600000000001</v>
       </c>
-      <c r="H550" s="27"/>
+      <c r="H550" s="27">
+        <v>10.98</v>
+      </c>
     </row>
     <row r="551" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A551" s="8">
@@ -27301,31 +27329,91 @@
       <c r="B551" s="4">
         <v>7.7042099999999998</v>
       </c>
-      <c r="H551" s="27"/>
+      <c r="H551" s="27">
+        <v>10.98</v>
+      </c>
     </row>
     <row r="552" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A552" s="8">
         <v>44014</v>
       </c>
-      <c r="H552" s="27"/>
+      <c r="B552" s="4">
+        <v>7.6991100000000001</v>
+      </c>
+      <c r="H552" s="27">
+        <v>10.98</v>
+      </c>
     </row>
     <row r="553" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A553" s="8">
         <v>44015</v>
       </c>
-      <c r="H553" s="27"/>
+      <c r="B553" s="4">
+        <v>7.7036499999999997</v>
+      </c>
+      <c r="H553" s="27">
+        <v>10.98</v>
+      </c>
     </row>
     <row r="554" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A554" s="8">
         <v>44016</v>
       </c>
-      <c r="H554" s="27"/>
+      <c r="B554" s="4">
+        <v>7.7036499999999997</v>
+      </c>
+      <c r="H554" s="27">
+        <v>10.98</v>
+      </c>
     </row>
     <row r="555" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A555" s="8">
         <v>44017</v>
       </c>
-      <c r="H555" s="27"/>
+      <c r="B555" s="4">
+        <v>7.7036499999999997</v>
+      </c>
+      <c r="H555" s="27">
+        <v>10.98</v>
+      </c>
+    </row>
+    <row r="556" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A556" s="8">
+        <v>44018</v>
+      </c>
+      <c r="B556" s="4">
+        <v>7.7041599999999999</v>
+      </c>
+    </row>
+    <row r="557" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A557" s="8">
+        <v>44019</v>
+      </c>
+    </row>
+    <row r="558" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A558" s="8">
+        <v>44020</v>
+      </c>
+    </row>
+    <row r="559" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A559" s="8">
+        <v>44021</v>
+      </c>
+    </row>
+    <row r="560" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A560" s="8">
+        <v>44022</v>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A561" s="8">
+        <v>44023</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A562" s="8">
+        <v>44024</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="32" type="noConversion"/>
@@ -27345,7 +27433,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-07-2020 23-44-17
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Guatemala/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="803" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DB5521D0-6C0F-493B-B9B8-5EBF8E14D94C}"/>
+  <xr:revisionPtr revIDLastSave="823" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{745A3D0C-F33F-4257-B663-3C8688C1F79F}"/>
   <bookViews>
-    <workbookView xWindow="8208" yWindow="0" windowWidth="14808" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -1601,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H562" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H562" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H569" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H569" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1970,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R562"/>
+  <dimension ref="A1:R569"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A546" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D565" sqref="D565"/>
+      <pane ySplit="3" topLeftCell="A556" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A572" sqref="A572"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12817,8 +12817,12 @@
       <c r="B556" s="28">
         <v>24.703700000000001</v>
       </c>
-      <c r="C556" s="22"/>
-      <c r="D556" s="22"/>
+      <c r="C556" s="22">
+        <v>97.2</v>
+      </c>
+      <c r="D556" s="22">
+        <v>11.93</v>
+      </c>
       <c r="E556" s="22"/>
       <c r="F556" s="22"/>
       <c r="G556" s="22"/>
@@ -12828,9 +12832,15 @@
       <c r="A557" s="8">
         <v>44019</v>
       </c>
-      <c r="B557" s="28"/>
-      <c r="C557" s="22"/>
-      <c r="D557" s="22"/>
+      <c r="B557" s="28">
+        <v>24.700800000000001</v>
+      </c>
+      <c r="C557" s="22">
+        <v>100.05</v>
+      </c>
+      <c r="D557" s="22">
+        <v>12.13</v>
+      </c>
       <c r="E557" s="22"/>
       <c r="F557" s="22"/>
       <c r="G557" s="22"/>
@@ -12840,7 +12850,9 @@
       <c r="A558" s="8">
         <v>44020</v>
       </c>
-      <c r="B558" s="28"/>
+      <c r="B558" s="28">
+        <v>24.7012</v>
+      </c>
       <c r="C558" s="22"/>
       <c r="D558" s="22"/>
       <c r="E558" s="22"/>
@@ -12891,10 +12903,102 @@
       <c r="B562" s="28"/>
       <c r="C562" s="22"/>
       <c r="D562" s="22"/>
-      <c r="E562" s="22"/>
-      <c r="F562" s="22"/>
-      <c r="G562" s="22"/>
-      <c r="H562" s="22"/>
+      <c r="E562" s="22">
+        <v>89.89</v>
+      </c>
+      <c r="F562" s="22">
+        <v>73.62</v>
+      </c>
+      <c r="G562" s="22">
+        <v>62.94</v>
+      </c>
+      <c r="H562" s="22">
+        <v>42.51</v>
+      </c>
+    </row>
+    <row r="563" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A563" s="8">
+        <v>44025</v>
+      </c>
+      <c r="B563" s="28"/>
+      <c r="C563" s="22"/>
+      <c r="D563" s="22"/>
+      <c r="E563" s="22"/>
+      <c r="F563" s="22"/>
+      <c r="G563" s="22"/>
+      <c r="H563" s="22"/>
+    </row>
+    <row r="564" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A564" s="8">
+        <v>44026</v>
+      </c>
+      <c r="B564" s="28"/>
+      <c r="C564" s="22"/>
+      <c r="D564" s="22"/>
+      <c r="E564" s="22"/>
+      <c r="F564" s="22"/>
+      <c r="G564" s="22"/>
+      <c r="H564" s="22"/>
+    </row>
+    <row r="565" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A565" s="8">
+        <v>44027</v>
+      </c>
+      <c r="B565" s="28"/>
+      <c r="C565" s="22"/>
+      <c r="D565" s="22"/>
+      <c r="E565" s="22"/>
+      <c r="F565" s="22"/>
+      <c r="G565" s="22"/>
+      <c r="H565" s="22"/>
+    </row>
+    <row r="566" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A566" s="8">
+        <v>44028</v>
+      </c>
+      <c r="B566" s="28"/>
+      <c r="C566" s="22"/>
+      <c r="D566" s="22"/>
+      <c r="E566" s="22"/>
+      <c r="F566" s="22"/>
+      <c r="G566" s="22"/>
+      <c r="H566" s="22"/>
+    </row>
+    <row r="567" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A567" s="8">
+        <v>44029</v>
+      </c>
+      <c r="B567" s="28"/>
+      <c r="C567" s="22"/>
+      <c r="D567" s="22"/>
+      <c r="E567" s="22"/>
+      <c r="F567" s="22"/>
+      <c r="G567" s="22"/>
+      <c r="H567" s="22"/>
+    </row>
+    <row r="568" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A568" s="8">
+        <v>44030</v>
+      </c>
+      <c r="B568" s="28"/>
+      <c r="C568" s="22"/>
+      <c r="D568" s="22"/>
+      <c r="E568" s="22"/>
+      <c r="F568" s="22"/>
+      <c r="G568" s="22"/>
+      <c r="H568" s="22"/>
+    </row>
+    <row r="569" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A569" s="8">
+        <v>44031</v>
+      </c>
+      <c r="B569" s="28"/>
+      <c r="C569" s="22"/>
+      <c r="D569" s="22"/>
+      <c r="E569" s="22"/>
+      <c r="F569" s="22"/>
+      <c r="G569" s="22"/>
+      <c r="H569" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -12918,8 +13022,8 @@
   <dimension ref="A1:R562"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A545" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A566" sqref="A566"/>
+      <pane ySplit="3" topLeftCell="A548" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E564" sqref="E564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27384,15 +27488,30 @@
       <c r="B556" s="4">
         <v>7.7041599999999999</v>
       </c>
+      <c r="E556" s="4">
+        <v>22.42</v>
+      </c>
+      <c r="F556" s="4">
+        <v>21.61</v>
+      </c>
+      <c r="G556" s="4">
+        <v>17.23</v>
+      </c>
     </row>
     <row r="557" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A557" s="8">
         <v>44019</v>
       </c>
+      <c r="B557" s="4">
+        <v>7.7040100000000002</v>
+      </c>
     </row>
     <row r="558" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A558" s="8">
         <v>44020</v>
+      </c>
+      <c r="B558" s="4">
+        <v>7.6993900000000002</v>
       </c>
     </row>
     <row r="559" spans="1:8" x14ac:dyDescent="0.3">
@@ -27430,10 +27549,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-15-2020 00-07-25
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Guatemala/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="845" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3663EC7F-2512-47D1-BCBA-AE66C8BCA372}"/>
+  <xr:revisionPtr revIDLastSave="867" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B7F62A7D-617D-4C75-9E7D-DAC42AD3B83A}"/>
   <bookViews>
-    <workbookView xWindow="5784" yWindow="0" windowWidth="17220" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7464" yWindow="696" windowWidth="15552" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -1601,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H569" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H569" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H576" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H576" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1638,8 +1638,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H569" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H569" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H576" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H576" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1970,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R569"/>
+  <dimension ref="A1:R576"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A555" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A577" sqref="A577"/>
+      <pane ySplit="3" topLeftCell="A558" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A581" sqref="A581"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12890,7 +12890,7 @@
         <v>24.6968</v>
       </c>
       <c r="C560" s="22">
-        <v>96.93</v>
+        <v>96.15</v>
       </c>
       <c r="D560" s="22">
         <v>11.76</v>
@@ -12939,8 +12939,12 @@
       <c r="B563" s="28">
         <v>24.6907</v>
       </c>
-      <c r="C563" s="22"/>
-      <c r="D563" s="22"/>
+      <c r="C563" s="22">
+        <v>97.4</v>
+      </c>
+      <c r="D563" s="22">
+        <v>11.58</v>
+      </c>
       <c r="E563" s="22"/>
       <c r="F563" s="22"/>
       <c r="G563" s="22"/>
@@ -12950,9 +12954,15 @@
       <c r="A564" s="8">
         <v>44026</v>
       </c>
-      <c r="B564" s="28"/>
-      <c r="C564" s="22"/>
-      <c r="D564" s="22"/>
+      <c r="B564" s="28">
+        <v>24.6875</v>
+      </c>
+      <c r="C564" s="22">
+        <v>97.73</v>
+      </c>
+      <c r="D564" s="22">
+        <v>11.36</v>
+      </c>
       <c r="E564" s="22"/>
       <c r="F564" s="22"/>
       <c r="G564" s="22"/>
@@ -12962,7 +12972,9 @@
       <c r="A565" s="8">
         <v>44027</v>
       </c>
-      <c r="B565" s="28"/>
+      <c r="B565" s="28">
+        <v>24.6798</v>
+      </c>
       <c r="C565" s="22"/>
       <c r="D565" s="22"/>
       <c r="E565" s="22"/>
@@ -13013,10 +13025,102 @@
       <c r="B569" s="28"/>
       <c r="C569" s="22"/>
       <c r="D569" s="22"/>
-      <c r="E569" s="22"/>
-      <c r="F569" s="22"/>
-      <c r="G569" s="22"/>
-      <c r="H569" s="22"/>
+      <c r="E569" s="22">
+        <v>81.19</v>
+      </c>
+      <c r="F569" s="22">
+        <v>74</v>
+      </c>
+      <c r="G569" s="22">
+        <v>63.59</v>
+      </c>
+      <c r="H569" s="22">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="570" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A570" s="8">
+        <v>44032</v>
+      </c>
+      <c r="B570" s="28"/>
+      <c r="C570" s="22"/>
+      <c r="D570" s="22"/>
+      <c r="E570" s="22"/>
+      <c r="F570" s="22"/>
+      <c r="G570" s="22"/>
+      <c r="H570" s="22"/>
+    </row>
+    <row r="571" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A571" s="8">
+        <v>44033</v>
+      </c>
+      <c r="B571" s="28"/>
+      <c r="C571" s="22"/>
+      <c r="D571" s="22"/>
+      <c r="E571" s="22"/>
+      <c r="F571" s="22"/>
+      <c r="G571" s="22"/>
+      <c r="H571" s="22"/>
+    </row>
+    <row r="572" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A572" s="8">
+        <v>44034</v>
+      </c>
+      <c r="B572" s="28"/>
+      <c r="C572" s="22"/>
+      <c r="D572" s="22"/>
+      <c r="E572" s="22"/>
+      <c r="F572" s="22"/>
+      <c r="G572" s="22"/>
+      <c r="H572" s="22"/>
+    </row>
+    <row r="573" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A573" s="8">
+        <v>44035</v>
+      </c>
+      <c r="B573" s="28"/>
+      <c r="C573" s="22"/>
+      <c r="D573" s="22"/>
+      <c r="E573" s="22"/>
+      <c r="F573" s="22"/>
+      <c r="G573" s="22"/>
+      <c r="H573" s="22"/>
+    </row>
+    <row r="574" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A574" s="8">
+        <v>44036</v>
+      </c>
+      <c r="B574" s="28"/>
+      <c r="C574" s="22"/>
+      <c r="D574" s="22"/>
+      <c r="E574" s="22"/>
+      <c r="F574" s="22"/>
+      <c r="G574" s="22"/>
+      <c r="H574" s="22"/>
+    </row>
+    <row r="575" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A575" s="8">
+        <v>44037</v>
+      </c>
+      <c r="B575" s="28"/>
+      <c r="C575" s="22"/>
+      <c r="D575" s="22"/>
+      <c r="E575" s="22"/>
+      <c r="F575" s="22"/>
+      <c r="G575" s="22"/>
+      <c r="H575" s="22"/>
+    </row>
+    <row r="576" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A576" s="8">
+        <v>44038</v>
+      </c>
+      <c r="B576" s="28"/>
+      <c r="C576" s="22"/>
+      <c r="D576" s="22"/>
+      <c r="E576" s="22"/>
+      <c r="F576" s="22"/>
+      <c r="G576" s="22"/>
+      <c r="H576" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -13037,11 +13141,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R569"/>
+  <dimension ref="A1:R576"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A553" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A575" sqref="A575"/>
+      <pane ySplit="3" topLeftCell="A564" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A581" sqref="A581"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27515,6 +27619,9 @@
       <c r="G556" s="4">
         <v>16.2</v>
       </c>
+      <c r="H556" s="4">
+        <v>10.83</v>
+      </c>
     </row>
     <row r="557" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A557" s="8">
@@ -27523,6 +27630,9 @@
       <c r="B557" s="4">
         <v>7.7040100000000002</v>
       </c>
+      <c r="H557" s="27">
+        <v>10.83</v>
+      </c>
     </row>
     <row r="558" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A558" s="8">
@@ -27531,6 +27641,9 @@
       <c r="B558" s="4">
         <v>7.6993900000000002</v>
       </c>
+      <c r="H558" s="27">
+        <v>10.83</v>
+      </c>
     </row>
     <row r="559" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A559" s="8">
@@ -27539,6 +27652,9 @@
       <c r="B559" s="4">
         <v>7.6955099999999996</v>
       </c>
+      <c r="H559" s="27">
+        <v>10.83</v>
+      </c>
     </row>
     <row r="560" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A560" s="8">
@@ -27547,59 +27663,118 @@
       <c r="B560" s="4">
         <v>7.6977099999999998</v>
       </c>
-    </row>
-    <row r="561" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="H560" s="27">
+        <v>10.83</v>
+      </c>
+    </row>
+    <row r="561" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A561" s="8">
         <v>44023</v>
       </c>
       <c r="B561" s="4">
         <v>7.6977099999999998</v>
       </c>
-    </row>
-    <row r="562" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="H561" s="27">
+        <v>10.83</v>
+      </c>
+    </row>
+    <row r="562" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A562" s="8">
         <v>44024</v>
       </c>
       <c r="B562" s="27">
         <v>7.6977099999999998</v>
       </c>
-    </row>
-    <row r="563" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="H562" s="27">
+        <v>10.83</v>
+      </c>
+    </row>
+    <row r="563" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A563" s="8">
         <v>44025</v>
       </c>
       <c r="B563" s="4">
         <v>7.6929600000000002</v>
       </c>
-    </row>
-    <row r="564" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E563" s="4">
+        <v>21.48</v>
+      </c>
+      <c r="F563" s="4">
+        <v>20.68</v>
+      </c>
+      <c r="G563" s="27">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="564" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A564" s="8">
         <v>44026</v>
       </c>
-    </row>
-    <row r="565" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B564" s="4">
+        <v>7.6919300000000002</v>
+      </c>
+    </row>
+    <row r="565" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A565" s="8">
         <v>44027</v>
       </c>
-    </row>
-    <row r="566" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B565" s="4">
+        <v>7.6916799999999999</v>
+      </c>
+    </row>
+    <row r="566" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A566" s="8">
         <v>44028</v>
       </c>
     </row>
-    <row r="567" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="567" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A567" s="8">
         <v>44029</v>
       </c>
     </row>
-    <row r="568" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="568" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A568" s="8">
         <v>44030</v>
       </c>
     </row>
-    <row r="569" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="569" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A569" s="8">
         <v>44031</v>
+      </c>
+    </row>
+    <row r="570" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A570" s="8">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="571" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A571" s="8">
+        <v>44033</v>
+      </c>
+    </row>
+    <row r="572" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A572" s="8">
+        <v>44034</v>
+      </c>
+    </row>
+    <row r="573" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A573" s="8">
+        <v>44035</v>
+      </c>
+    </row>
+    <row r="574" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A574" s="8">
+        <v>44036</v>
+      </c>
+    </row>
+    <row r="575" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A575" s="8">
+        <v>44037</v>
+      </c>
+    </row>
+    <row r="576" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A576" s="8">
+        <v>44038</v>
       </c>
     </row>
   </sheetData>
@@ -27620,7 +27795,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-18-2020 02-28-38
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Guatemala/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="867" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B7F62A7D-617D-4C75-9E7D-DAC42AD3B83A}"/>
+  <xr:revisionPtr revIDLastSave="886" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{13C38A21-3455-4EA8-BB8F-7C8A16012006}"/>
   <bookViews>
-    <workbookView xWindow="7464" yWindow="696" windowWidth="15552" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6516" yWindow="0" windowWidth="16524" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -1973,8 +1973,8 @@
   <dimension ref="A1:R576"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A558" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A581" sqref="A581"/>
+      <pane ySplit="3" topLeftCell="A560" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A585" sqref="A585"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12958,10 +12958,10 @@
         <v>24.6875</v>
       </c>
       <c r="C564" s="22">
-        <v>97.73</v>
+        <v>96.7</v>
       </c>
       <c r="D564" s="22">
-        <v>11.36</v>
+        <v>11.32</v>
       </c>
       <c r="E564" s="22"/>
       <c r="F564" s="22"/>
@@ -12975,8 +12975,12 @@
       <c r="B565" s="28">
         <v>24.6798</v>
       </c>
-      <c r="C565" s="22"/>
-      <c r="D565" s="22"/>
+      <c r="C565" s="22">
+        <v>95.95</v>
+      </c>
+      <c r="D565" s="22">
+        <v>11.82</v>
+      </c>
       <c r="E565" s="22"/>
       <c r="F565" s="22"/>
       <c r="G565" s="22"/>
@@ -12986,9 +12990,15 @@
       <c r="A566" s="8">
         <v>44028</v>
       </c>
-      <c r="B566" s="28"/>
-      <c r="C566" s="22"/>
-      <c r="D566" s="22"/>
+      <c r="B566" s="28">
+        <v>24.673100000000002</v>
+      </c>
+      <c r="C566" s="22">
+        <v>97.1</v>
+      </c>
+      <c r="D566" s="22">
+        <v>11.79</v>
+      </c>
       <c r="E566" s="22"/>
       <c r="F566" s="22"/>
       <c r="G566" s="22"/>
@@ -12998,9 +13008,15 @@
       <c r="A567" s="8">
         <v>44029</v>
       </c>
-      <c r="B567" s="28"/>
-      <c r="C567" s="22"/>
-      <c r="D567" s="22"/>
+      <c r="B567" s="28">
+        <v>24.672899999999998</v>
+      </c>
+      <c r="C567" s="22">
+        <v>101.5</v>
+      </c>
+      <c r="D567" s="22">
+        <v>11.75</v>
+      </c>
       <c r="E567" s="22"/>
       <c r="F567" s="22"/>
       <c r="G567" s="22"/>
@@ -13042,7 +13058,9 @@
       <c r="A570" s="8">
         <v>44032</v>
       </c>
-      <c r="B570" s="28"/>
+      <c r="B570" s="28">
+        <v>24.6693</v>
+      </c>
       <c r="C570" s="22"/>
       <c r="D570" s="22"/>
       <c r="E570" s="22"/>
@@ -13144,8 +13162,8 @@
   <dimension ref="A1:R576"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A564" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A581" sqref="A581"/>
+      <pane ySplit="3" topLeftCell="A563" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A578" sqref="A578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27705,6 +27723,9 @@
       <c r="G563" s="27">
         <v>16.2</v>
       </c>
+      <c r="H563" s="4">
+        <v>11.33</v>
+      </c>
     </row>
     <row r="564" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A564" s="8">
@@ -27713,6 +27734,9 @@
       <c r="B564" s="4">
         <v>7.6919300000000002</v>
       </c>
+      <c r="H564" s="4">
+        <v>11.33</v>
+      </c>
     </row>
     <row r="565" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A565" s="8">
@@ -27721,61 +27745,97 @@
       <c r="B565" s="4">
         <v>7.6916799999999999</v>
       </c>
+      <c r="H565" s="4">
+        <v>11.33</v>
+      </c>
     </row>
     <row r="566" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A566" s="8">
         <v>44028</v>
       </c>
+      <c r="B566" s="27">
+        <v>7.6905099999999997</v>
+      </c>
+      <c r="H566" s="4">
+        <v>11.33</v>
+      </c>
     </row>
     <row r="567" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A567" s="8">
         <v>44029</v>
       </c>
+      <c r="B567" s="27">
+        <v>7.6899199999999999</v>
+      </c>
+      <c r="H567" s="4">
+        <v>11.33</v>
+      </c>
     </row>
     <row r="568" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A568" s="8">
         <v>44030</v>
       </c>
+      <c r="B568" s="27">
+        <v>7.6899199999999999</v>
+      </c>
+      <c r="H568" s="4">
+        <v>11.33</v>
+      </c>
     </row>
     <row r="569" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A569" s="8">
         <v>44031</v>
       </c>
+      <c r="B569" s="27">
+        <v>7.6899199999999999</v>
+      </c>
+      <c r="H569" s="4">
+        <v>11.33</v>
+      </c>
     </row>
     <row r="570" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A570" s="8">
         <v>44032</v>
       </c>
+      <c r="B570" s="27">
+        <v>7.6914499999999997</v>
+      </c>
     </row>
     <row r="571" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A571" s="8">
         <v>44033</v>
       </c>
+      <c r="B571" s="27"/>
     </row>
     <row r="572" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A572" s="8">
         <v>44034</v>
       </c>
+      <c r="B572" s="27"/>
     </row>
     <row r="573" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A573" s="8">
         <v>44035</v>
       </c>
+      <c r="B573" s="27"/>
     </row>
     <row r="574" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A574" s="8">
         <v>44036</v>
       </c>
+      <c r="B574" s="27"/>
     </row>
     <row r="575" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A575" s="8">
         <v>44037</v>
       </c>
+      <c r="B575" s="27"/>
     </row>
     <row r="576" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A576" s="8">
         <v>44038</v>
       </c>
+      <c r="B576" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="32" type="noConversion"/>
@@ -27795,7 +27855,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-25-2020 02-56-51
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Guatemala/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="905" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EC1778CD-0BDD-419B-BBCB-911DC92F7136}"/>
+  <xr:revisionPtr revIDLastSave="930" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDC70EC4-D409-490C-911B-09095B57625E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10128" yWindow="1248" windowWidth="12912" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -22,9 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1973,8 +1971,8 @@
   <dimension ref="A1:R583"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A562" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E587" sqref="E587"/>
+      <pane ySplit="3" topLeftCell="A568" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A593" sqref="A593"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3877,7 +3875,7 @@
       </c>
       <c r="Q43" s="27"/>
       <c r="R43" s="27">
-        <v>327.3</v>
+        <v>329.8</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
@@ -3916,7 +3914,7 @@
       </c>
       <c r="Q44" s="27"/>
       <c r="R44" s="27">
-        <v>329.8</v>
+        <v>412.7</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
@@ -3956,9 +3954,7 @@
         <v>500</v>
       </c>
       <c r="Q45" s="27"/>
-      <c r="R45" s="27">
-        <v>412.7</v>
-      </c>
+      <c r="R45" s="27"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
@@ -13080,10 +13076,10 @@
         <v>24.667000000000002</v>
       </c>
       <c r="C571" s="22">
-        <v>101.83</v>
+        <v>100.5</v>
       </c>
       <c r="D571" s="22">
-        <v>11.66</v>
+        <v>11.67</v>
       </c>
       <c r="E571" s="22"/>
       <c r="F571" s="22"/>
@@ -13097,8 +13093,12 @@
       <c r="B572" s="28">
         <v>24.669599999999999</v>
       </c>
-      <c r="C572" s="22"/>
-      <c r="D572" s="22"/>
+      <c r="C572" s="22">
+        <v>108.35</v>
+      </c>
+      <c r="D572" s="22">
+        <v>11.86</v>
+      </c>
       <c r="E572" s="22"/>
       <c r="F572" s="22"/>
       <c r="G572" s="22"/>
@@ -13108,9 +13108,15 @@
       <c r="A573" s="8">
         <v>44035</v>
       </c>
-      <c r="B573" s="28"/>
-      <c r="C573" s="22"/>
-      <c r="D573" s="22"/>
+      <c r="B573" s="28">
+        <v>24.669899999999998</v>
+      </c>
+      <c r="C573" s="22">
+        <v>107.5</v>
+      </c>
+      <c r="D573" s="22">
+        <v>11.77</v>
+      </c>
       <c r="E573" s="22"/>
       <c r="F573" s="22"/>
       <c r="G573" s="22"/>
@@ -13120,9 +13126,15 @@
       <c r="A574" s="8">
         <v>44036</v>
       </c>
-      <c r="B574" s="28"/>
-      <c r="C574" s="22"/>
-      <c r="D574" s="22"/>
+      <c r="B574" s="28">
+        <v>24.6676</v>
+      </c>
+      <c r="C574" s="22">
+        <v>108.3</v>
+      </c>
+      <c r="D574" s="22">
+        <v>11.5</v>
+      </c>
       <c r="E574" s="22"/>
       <c r="F574" s="22"/>
       <c r="G574" s="22"/>
@@ -13164,7 +13176,9 @@
       <c r="A577" s="8">
         <v>44039</v>
       </c>
-      <c r="B577" s="28"/>
+      <c r="B577" s="28">
+        <v>24.664999999999999</v>
+      </c>
       <c r="C577" s="22"/>
       <c r="D577" s="22"/>
       <c r="E577" s="22"/>
@@ -13266,8 +13280,8 @@
   <dimension ref="A1:R583"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A566" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E586" sqref="E586"/>
+      <pane ySplit="3" topLeftCell="A571" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B586" sqref="B586"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27913,6 +27927,9 @@
       <c r="G570" s="4">
         <v>16.2</v>
       </c>
+      <c r="H570" s="27">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="571" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A571" s="8">
@@ -27921,6 +27938,9 @@
       <c r="B571" s="27">
         <v>7.6888500000000004</v>
       </c>
+      <c r="H571" s="27">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="572" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A572" s="8">
@@ -27929,62 +27949,89 @@
       <c r="B572" s="27">
         <v>7.6917600000000004</v>
       </c>
+      <c r="H572" s="27">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="573" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A573" s="8">
         <v>44035</v>
       </c>
-      <c r="B573" s="27"/>
+      <c r="B573" s="27">
+        <v>7.69095</v>
+      </c>
+      <c r="H573" s="27">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="574" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A574" s="8">
         <v>44036</v>
       </c>
-      <c r="B574" s="27"/>
+      <c r="B574" s="27">
+        <v>7.6886299999999999</v>
+      </c>
+      <c r="H574" s="27">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="575" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A575" s="8">
         <v>44037</v>
       </c>
-      <c r="B575" s="27"/>
+      <c r="B575" s="27">
+        <v>7.6886299999999999</v>
+      </c>
+      <c r="H575" s="27">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="576" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A576" s="8">
         <v>44038</v>
       </c>
-      <c r="B576" s="27"/>
-    </row>
-    <row r="577" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B576" s="27">
+        <v>7.6886299999999999</v>
+      </c>
+      <c r="H576" s="27">
+        <v>11.38</v>
+      </c>
+    </row>
+    <row r="577" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A577" s="8">
         <v>44039</v>
       </c>
-    </row>
-    <row r="578" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B577" s="4">
+        <v>7.6942700000000004</v>
+      </c>
+      <c r="H577" s="27"/>
+    </row>
+    <row r="578" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A578" s="8">
         <v>44040</v>
       </c>
     </row>
-    <row r="579" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A579" s="8">
         <v>44041</v>
       </c>
     </row>
-    <row r="580" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A580" s="8">
         <v>44042</v>
       </c>
     </row>
-    <row r="581" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A581" s="8">
         <v>44043</v>
       </c>
     </row>
-    <row r="582" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A582" s="8">
         <v>44044</v>
       </c>
     </row>
-    <row r="583" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A583" s="8">
         <v>44045</v>
       </c>
@@ -28004,10 +28051,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-29-2020 00-10-30
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="930" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDC70EC4-D409-490C-911B-09095B57625E}"/>
+  <xr:revisionPtr revIDLastSave="952" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF8E50B1-8D2B-4CE1-9882-AC0231646DF0}"/>
   <bookViews>
-    <workbookView xWindow="10128" yWindow="1248" windowWidth="12912" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -1599,8 +1599,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H583" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H583" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H590" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H590" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1636,8 +1636,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H583" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H583" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H590" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H590" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1968,11 +1968,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R583"/>
+  <dimension ref="A1:R590"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A568" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A593" sqref="A593"/>
+      <pane ySplit="3" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A595" sqref="A595"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13130,10 +13130,10 @@
         <v>24.6676</v>
       </c>
       <c r="C574" s="22">
-        <v>108.3</v>
+        <v>108.4</v>
       </c>
       <c r="D574" s="22">
-        <v>11.5</v>
+        <v>11.49</v>
       </c>
       <c r="E574" s="22"/>
       <c r="F574" s="22"/>
@@ -13179,8 +13179,12 @@
       <c r="B577" s="28">
         <v>24.664999999999999</v>
       </c>
-      <c r="C577" s="22"/>
-      <c r="D577" s="22"/>
+      <c r="C577" s="22">
+        <v>110.4</v>
+      </c>
+      <c r="D577" s="22">
+        <v>12.12</v>
+      </c>
       <c r="E577" s="22"/>
       <c r="F577" s="22"/>
       <c r="G577" s="22"/>
@@ -13190,9 +13194,15 @@
       <c r="A578" s="8">
         <v>44040</v>
       </c>
-      <c r="B578" s="28"/>
-      <c r="C578" s="22"/>
-      <c r="D578" s="22"/>
+      <c r="B578" s="28">
+        <v>24.657599999999999</v>
+      </c>
+      <c r="C578" s="22">
+        <v>109.93</v>
+      </c>
+      <c r="D578" s="22">
+        <v>12.02</v>
+      </c>
       <c r="E578" s="22"/>
       <c r="F578" s="22"/>
       <c r="G578" s="22"/>
@@ -13202,7 +13212,9 @@
       <c r="A579" s="8">
         <v>44041</v>
       </c>
-      <c r="B579" s="28"/>
+      <c r="B579" s="28">
+        <v>24.648900000000001</v>
+      </c>
       <c r="C579" s="22"/>
       <c r="D579" s="22"/>
       <c r="E579" s="22"/>
@@ -13253,10 +13265,102 @@
       <c r="B583" s="28"/>
       <c r="C583" s="22"/>
       <c r="D583" s="22"/>
-      <c r="E583" s="22"/>
-      <c r="F583" s="22"/>
-      <c r="G583" s="22"/>
-      <c r="H583" s="22"/>
+      <c r="E583" s="22">
+        <v>81.760000000000005</v>
+      </c>
+      <c r="F583" s="22">
+        <v>74.37</v>
+      </c>
+      <c r="G583" s="22">
+        <v>64.61</v>
+      </c>
+      <c r="H583" s="22">
+        <v>43.94</v>
+      </c>
+    </row>
+    <row r="584" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A584" s="8">
+        <v>44046</v>
+      </c>
+      <c r="B584" s="28"/>
+      <c r="C584" s="22"/>
+      <c r="D584" s="22"/>
+      <c r="E584" s="22"/>
+      <c r="F584" s="22"/>
+      <c r="G584" s="22"/>
+      <c r="H584" s="22"/>
+    </row>
+    <row r="585" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A585" s="8">
+        <v>44047</v>
+      </c>
+      <c r="B585" s="28"/>
+      <c r="C585" s="22"/>
+      <c r="D585" s="22"/>
+      <c r="E585" s="22"/>
+      <c r="F585" s="22"/>
+      <c r="G585" s="22"/>
+      <c r="H585" s="22"/>
+    </row>
+    <row r="586" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A586" s="8">
+        <v>44048</v>
+      </c>
+      <c r="B586" s="28"/>
+      <c r="C586" s="22"/>
+      <c r="D586" s="22"/>
+      <c r="E586" s="22"/>
+      <c r="F586" s="22"/>
+      <c r="G586" s="22"/>
+      <c r="H586" s="22"/>
+    </row>
+    <row r="587" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A587" s="8">
+        <v>44049</v>
+      </c>
+      <c r="B587" s="28"/>
+      <c r="C587" s="22"/>
+      <c r="D587" s="22"/>
+      <c r="E587" s="22"/>
+      <c r="F587" s="22"/>
+      <c r="G587" s="22"/>
+      <c r="H587" s="22"/>
+    </row>
+    <row r="588" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A588" s="8">
+        <v>44050</v>
+      </c>
+      <c r="B588" s="28"/>
+      <c r="C588" s="22"/>
+      <c r="D588" s="22"/>
+      <c r="E588" s="22"/>
+      <c r="F588" s="22"/>
+      <c r="G588" s="22"/>
+      <c r="H588" s="22"/>
+    </row>
+    <row r="589" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A589" s="8">
+        <v>44051</v>
+      </c>
+      <c r="B589" s="28"/>
+      <c r="C589" s="22"/>
+      <c r="D589" s="22"/>
+      <c r="E589" s="22"/>
+      <c r="F589" s="22"/>
+      <c r="G589" s="22"/>
+      <c r="H589" s="22"/>
+    </row>
+    <row r="590" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A590" s="8">
+        <v>44052</v>
+      </c>
+      <c r="B590" s="28"/>
+      <c r="C590" s="22"/>
+      <c r="D590" s="22"/>
+      <c r="E590" s="22"/>
+      <c r="F590" s="22"/>
+      <c r="G590" s="22"/>
+      <c r="H590" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -13277,11 +13381,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R583"/>
+  <dimension ref="A1:R590"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A571" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B586" sqref="B586"/>
+      <pane ySplit="3" topLeftCell="A575" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B592" sqref="B592"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28004,17 +28108,32 @@
       <c r="B577" s="4">
         <v>7.6942700000000004</v>
       </c>
+      <c r="E577" s="4">
+        <v>21.65</v>
+      </c>
+      <c r="F577" s="4">
+        <v>20.83</v>
+      </c>
+      <c r="G577" s="4">
+        <v>16.77</v>
+      </c>
       <c r="H577" s="27"/>
     </row>
     <row r="578" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A578" s="8">
         <v>44040</v>
       </c>
+      <c r="B578" s="4">
+        <v>7.6956300000000004</v>
+      </c>
     </row>
     <row r="579" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A579" s="8">
         <v>44041</v>
       </c>
+      <c r="B579" s="4">
+        <v>7.6988000000000003</v>
+      </c>
     </row>
     <row r="580" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A580" s="8">
@@ -28034,6 +28153,41 @@
     <row r="583" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A583" s="8">
         <v>44045</v>
+      </c>
+    </row>
+    <row r="584" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A584" s="8">
+        <v>44046</v>
+      </c>
+    </row>
+    <row r="585" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A585" s="8">
+        <v>44047</v>
+      </c>
+    </row>
+    <row r="586" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A586" s="8">
+        <v>44048</v>
+      </c>
+    </row>
+    <row r="587" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A587" s="8">
+        <v>44049</v>
+      </c>
+    </row>
+    <row r="588" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A588" s="8">
+        <v>44050</v>
+      </c>
+    </row>
+    <row r="589" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A589" s="8">
+        <v>44051</v>
+      </c>
+    </row>
+    <row r="590" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A590" s="8">
+        <v>44052</v>
       </c>
     </row>
   </sheetData>
@@ -28051,10 +28205,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-01-2020 03-19-51
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="952" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF8E50B1-8D2B-4CE1-9882-AC0231646DF0}"/>
+  <xr:revisionPtr revIDLastSave="968" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A07954DA-3D10-4DE8-A025-FC6840C883EC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8736" yWindow="0" windowWidth="14268" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
     <sheet name="GUATEMALA" sheetId="4" r:id="rId2"/>
     <sheet name="Fuentes" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1971,8 +1973,8 @@
   <dimension ref="A1:R590"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A595" sqref="A595"/>
+      <pane ySplit="3" topLeftCell="A568" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A592" sqref="A592"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13198,10 +13200,10 @@
         <v>24.657599999999999</v>
       </c>
       <c r="C578" s="22">
-        <v>109.93</v>
+        <v>109.65</v>
       </c>
       <c r="D578" s="22">
-        <v>12.02</v>
+        <v>12.01</v>
       </c>
       <c r="E578" s="22"/>
       <c r="F578" s="22"/>
@@ -13215,8 +13217,12 @@
       <c r="B579" s="28">
         <v>24.648900000000001</v>
       </c>
-      <c r="C579" s="22"/>
-      <c r="D579" s="22"/>
+      <c r="C579" s="22">
+        <v>111.6</v>
+      </c>
+      <c r="D579" s="22">
+        <v>12.01</v>
+      </c>
       <c r="E579" s="22"/>
       <c r="F579" s="22"/>
       <c r="G579" s="22"/>
@@ -13226,9 +13232,15 @@
       <c r="A580" s="8">
         <v>44042</v>
       </c>
-      <c r="B580" s="28"/>
-      <c r="C580" s="22"/>
-      <c r="D580" s="22"/>
+      <c r="B580" s="28">
+        <v>24.642800000000001</v>
+      </c>
+      <c r="C580" s="22">
+        <v>115.35</v>
+      </c>
+      <c r="D580" s="22">
+        <v>12.11</v>
+      </c>
       <c r="E580" s="22"/>
       <c r="F580" s="22"/>
       <c r="G580" s="22"/>
@@ -13238,9 +13250,15 @@
       <c r="A581" s="8">
         <v>44043</v>
       </c>
-      <c r="B581" s="28"/>
-      <c r="C581" s="22"/>
-      <c r="D581" s="22"/>
+      <c r="B581" s="28">
+        <v>24.635100000000001</v>
+      </c>
+      <c r="C581" s="22">
+        <v>118.75</v>
+      </c>
+      <c r="D581" s="22">
+        <v>12.62</v>
+      </c>
       <c r="E581" s="22"/>
       <c r="F581" s="22"/>
       <c r="G581" s="22"/>
@@ -13282,7 +13300,9 @@
       <c r="A584" s="8">
         <v>44046</v>
       </c>
-      <c r="B584" s="28"/>
+      <c r="B584" s="28">
+        <v>24.626799999999999</v>
+      </c>
       <c r="C584" s="22"/>
       <c r="D584" s="22"/>
       <c r="E584" s="22"/>
@@ -13384,8 +13404,8 @@
   <dimension ref="A1:R590"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A575" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B592" sqref="B592"/>
+      <pane ySplit="3" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A594" sqref="A594"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28117,7 +28137,9 @@
       <c r="G577" s="4">
         <v>16.77</v>
       </c>
-      <c r="H577" s="27"/>
+      <c r="H577" s="27">
+        <v>11.3</v>
+      </c>
     </row>
     <row r="578" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A578" s="8">
@@ -28126,6 +28148,9 @@
       <c r="B578" s="4">
         <v>7.6956300000000004</v>
       </c>
+      <c r="H578" s="4">
+        <v>11.3</v>
+      </c>
     </row>
     <row r="579" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A579" s="8">
@@ -28134,25 +28159,49 @@
       <c r="B579" s="4">
         <v>7.6988000000000003</v>
       </c>
+      <c r="H579" s="4">
+        <v>11.3</v>
+      </c>
     </row>
     <row r="580" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A580" s="8">
         <v>44042</v>
       </c>
+      <c r="B580" s="4">
+        <v>7.7013299999999996</v>
+      </c>
+      <c r="H580" s="4">
+        <v>11.3</v>
+      </c>
     </row>
     <row r="581" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A581" s="8">
         <v>44043</v>
       </c>
+      <c r="B581" s="4">
+        <v>7.70871</v>
+      </c>
+      <c r="H581" s="4">
+        <v>11.3</v>
+      </c>
     </row>
     <row r="582" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A582" s="8">
         <v>44044</v>
       </c>
+      <c r="B582" s="27">
+        <v>7.70871</v>
+      </c>
+      <c r="H582" s="4">
+        <v>11.3</v>
+      </c>
     </row>
     <row r="583" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A583" s="8">
         <v>44045</v>
+      </c>
+      <c r="H583" s="4">
+        <v>11.3</v>
       </c>
     </row>
     <row r="584" spans="1:8" x14ac:dyDescent="0.3">
@@ -28208,7 +28257,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-05-2020 01-25-45
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="968" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A07954DA-3D10-4DE8-A025-FC6840C883EC}"/>
+  <xr:revisionPtr revIDLastSave="994" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{466B7F89-D39E-47DB-AACC-E7F1F4141BAC}"/>
   <bookViews>
-    <workbookView xWindow="8736" yWindow="0" windowWidth="14268" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -1601,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H590" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H590" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H597" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H597" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1638,8 +1638,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H590" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H590" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H597" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H597" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1970,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R590"/>
+  <dimension ref="A1:R597"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A568" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A592" sqref="A592"/>
+      <pane ySplit="3" topLeftCell="A577" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A599" sqref="A599"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3956,7 +3956,9 @@
         <v>500</v>
       </c>
       <c r="Q45" s="27"/>
-      <c r="R45" s="27"/>
+      <c r="R45" s="27">
+        <v>491.8</v>
+      </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
@@ -13254,10 +13256,10 @@
         <v>24.635100000000001</v>
       </c>
       <c r="C581" s="22">
-        <v>118.75</v>
+        <v>118.95</v>
       </c>
       <c r="D581" s="22">
-        <v>12.62</v>
+        <v>12.64</v>
       </c>
       <c r="E581" s="22"/>
       <c r="F581" s="22"/>
@@ -13303,8 +13305,12 @@
       <c r="B584" s="28">
         <v>24.626799999999999</v>
       </c>
-      <c r="C584" s="22"/>
-      <c r="D584" s="22"/>
+      <c r="C584" s="22">
+        <v>117.9</v>
+      </c>
+      <c r="D584" s="22">
+        <v>12.72</v>
+      </c>
       <c r="E584" s="22"/>
       <c r="F584" s="22"/>
       <c r="G584" s="22"/>
@@ -13314,9 +13320,15 @@
       <c r="A585" s="8">
         <v>44047</v>
       </c>
-      <c r="B585" s="28"/>
-      <c r="C585" s="22"/>
-      <c r="D585" s="22"/>
+      <c r="B585" s="28">
+        <v>24.614699999999999</v>
+      </c>
+      <c r="C585" s="22">
+        <v>120.1</v>
+      </c>
+      <c r="D585" s="22">
+        <v>12.77</v>
+      </c>
       <c r="E585" s="22"/>
       <c r="F585" s="22"/>
       <c r="G585" s="22"/>
@@ -13326,7 +13338,9 @@
       <c r="A586" s="8">
         <v>44048</v>
       </c>
-      <c r="B586" s="28"/>
+      <c r="B586" s="28">
+        <v>24.601400000000002</v>
+      </c>
       <c r="C586" s="22"/>
       <c r="D586" s="22"/>
       <c r="E586" s="22"/>
@@ -13377,10 +13391,102 @@
       <c r="B590" s="28"/>
       <c r="C590" s="22"/>
       <c r="D590" s="22"/>
-      <c r="E590" s="22"/>
-      <c r="F590" s="22"/>
-      <c r="G590" s="22"/>
-      <c r="H590" s="22"/>
+      <c r="E590" s="22">
+        <v>81.680000000000007</v>
+      </c>
+      <c r="F590" s="22">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="G590" s="22">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="H590" s="22">
+        <v>44.55</v>
+      </c>
+    </row>
+    <row r="591" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A591" s="8">
+        <v>44053</v>
+      </c>
+      <c r="B591" s="28"/>
+      <c r="C591" s="22"/>
+      <c r="D591" s="22"/>
+      <c r="E591" s="22"/>
+      <c r="F591" s="22"/>
+      <c r="G591" s="22"/>
+      <c r="H591" s="22"/>
+    </row>
+    <row r="592" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A592" s="8">
+        <v>44054</v>
+      </c>
+      <c r="B592" s="28"/>
+      <c r="C592" s="22"/>
+      <c r="D592" s="22"/>
+      <c r="E592" s="22"/>
+      <c r="F592" s="22"/>
+      <c r="G592" s="22"/>
+      <c r="H592" s="22"/>
+    </row>
+    <row r="593" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A593" s="8">
+        <v>44055</v>
+      </c>
+      <c r="B593" s="28"/>
+      <c r="C593" s="22"/>
+      <c r="D593" s="22"/>
+      <c r="E593" s="22"/>
+      <c r="F593" s="22"/>
+      <c r="G593" s="22"/>
+      <c r="H593" s="22"/>
+    </row>
+    <row r="594" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A594" s="8">
+        <v>44056</v>
+      </c>
+      <c r="B594" s="28"/>
+      <c r="C594" s="22"/>
+      <c r="D594" s="22"/>
+      <c r="E594" s="22"/>
+      <c r="F594" s="22"/>
+      <c r="G594" s="22"/>
+      <c r="H594" s="22"/>
+    </row>
+    <row r="595" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A595" s="8">
+        <v>44057</v>
+      </c>
+      <c r="B595" s="28"/>
+      <c r="C595" s="22"/>
+      <c r="D595" s="22"/>
+      <c r="E595" s="22"/>
+      <c r="F595" s="22"/>
+      <c r="G595" s="22"/>
+      <c r="H595" s="22"/>
+    </row>
+    <row r="596" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A596" s="8">
+        <v>44058</v>
+      </c>
+      <c r="B596" s="28"/>
+      <c r="C596" s="22"/>
+      <c r="D596" s="22"/>
+      <c r="E596" s="22"/>
+      <c r="F596" s="22"/>
+      <c r="G596" s="22"/>
+      <c r="H596" s="22"/>
+    </row>
+    <row r="597" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A597" s="8">
+        <v>44059</v>
+      </c>
+      <c r="B597" s="28"/>
+      <c r="C597" s="22"/>
+      <c r="D597" s="22"/>
+      <c r="E597" s="22"/>
+      <c r="F597" s="22"/>
+      <c r="G597" s="22"/>
+      <c r="H597" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -13401,11 +13507,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R590"/>
+  <dimension ref="A1:R597"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A594" sqref="A594"/>
+      <pane ySplit="3" topLeftCell="A592" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A602" sqref="A602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15597,7 +15703,9 @@
         <v>214.45</v>
       </c>
       <c r="Q45" s="27"/>
-      <c r="R45" s="27"/>
+      <c r="R45" s="27">
+        <v>963</v>
+      </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
@@ -15638,10 +15746,10 @@
       <c r="M46" s="27"/>
       <c r="N46" s="27"/>
       <c r="O46" s="22">
-        <v>355.57</v>
+        <v>2413.9850000000001</v>
       </c>
       <c r="P46" s="22">
-        <v>41.19</v>
+        <v>103.02</v>
       </c>
       <c r="Q46" s="27"/>
       <c r="R46" s="27"/>
@@ -28200,6 +28308,9 @@
       <c r="A583" s="8">
         <v>44045</v>
       </c>
+      <c r="B583" s="27">
+        <v>7.70871</v>
+      </c>
       <c r="H583" s="4">
         <v>11.3</v>
       </c>
@@ -28208,16 +28319,34 @@
       <c r="A584" s="8">
         <v>44046</v>
       </c>
+      <c r="B584" s="4">
+        <v>7.7088799999999997</v>
+      </c>
+      <c r="E584" s="4">
+        <v>21.46</v>
+      </c>
+      <c r="F584" s="4">
+        <v>20.66</v>
+      </c>
+      <c r="G584" s="4">
+        <v>16.739999999999998</v>
+      </c>
     </row>
     <row r="585" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A585" s="8">
         <v>44047</v>
       </c>
+      <c r="B585" s="4">
+        <v>7.7069799999999997</v>
+      </c>
     </row>
     <row r="586" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A586" s="8">
         <v>44048</v>
       </c>
+      <c r="B586" s="4">
+        <v>7.7055499999999997</v>
+      </c>
     </row>
     <row r="587" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A587" s="8">
@@ -28237,6 +28366,41 @@
     <row r="590" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A590" s="8">
         <v>44052</v>
+      </c>
+    </row>
+    <row r="591" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A591" s="8">
+        <v>44053</v>
+      </c>
+    </row>
+    <row r="592" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A592" s="8">
+        <v>44054</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A593" s="8">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A594" s="8">
+        <v>44056</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A595" s="8">
+        <v>44057</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A596" s="8">
+        <v>44058</v>
+      </c>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A597" s="8">
+        <v>44059</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-07-2020 23-42-22
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="994" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{466B7F89-D39E-47DB-AACC-E7F1F4141BAC}"/>
+  <xr:revisionPtr revIDLastSave="1011" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E0987C32-F64A-4719-943F-9B55DD58D831}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1973,8 +1973,8 @@
   <dimension ref="A1:R597"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A577" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A599" sqref="A599"/>
+      <pane ySplit="3" topLeftCell="A585" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A601" sqref="A601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13324,10 +13324,10 @@
         <v>24.614699999999999</v>
       </c>
       <c r="C585" s="22">
-        <v>120.1</v>
+        <v>121.05</v>
       </c>
       <c r="D585" s="22">
-        <v>12.77</v>
+        <v>12.78</v>
       </c>
       <c r="E585" s="22"/>
       <c r="F585" s="22"/>
@@ -13341,8 +13341,12 @@
       <c r="B586" s="28">
         <v>24.601400000000002</v>
       </c>
-      <c r="C586" s="22"/>
-      <c r="D586" s="22"/>
+      <c r="C586" s="22">
+        <v>121.55</v>
+      </c>
+      <c r="D586" s="22">
+        <v>12.54</v>
+      </c>
       <c r="E586" s="22"/>
       <c r="F586" s="22"/>
       <c r="G586" s="22"/>
@@ -13352,9 +13356,15 @@
       <c r="A587" s="8">
         <v>44049</v>
       </c>
-      <c r="B587" s="28"/>
-      <c r="C587" s="22"/>
-      <c r="D587" s="22"/>
+      <c r="B587" s="28">
+        <v>24.587399999999999</v>
+      </c>
+      <c r="C587" s="22">
+        <v>117</v>
+      </c>
+      <c r="D587" s="22">
+        <v>12.94</v>
+      </c>
       <c r="E587" s="22"/>
       <c r="F587" s="22"/>
       <c r="G587" s="22"/>
@@ -13364,9 +13374,15 @@
       <c r="A588" s="8">
         <v>44050</v>
       </c>
-      <c r="B588" s="28"/>
-      <c r="C588" s="22"/>
-      <c r="D588" s="22"/>
+      <c r="B588" s="28">
+        <v>24.575800000000001</v>
+      </c>
+      <c r="C588" s="22">
+        <v>114.83</v>
+      </c>
+      <c r="D588" s="22">
+        <v>12.66</v>
+      </c>
       <c r="E588" s="22"/>
       <c r="F588" s="22"/>
       <c r="G588" s="22"/>
@@ -13408,7 +13424,9 @@
       <c r="A591" s="8">
         <v>44053</v>
       </c>
-      <c r="B591" s="28"/>
+      <c r="B591" s="28">
+        <v>24.562100000000001</v>
+      </c>
       <c r="C591" s="22"/>
       <c r="D591" s="22"/>
       <c r="E591" s="22"/>
@@ -13510,8 +13528,8 @@
   <dimension ref="A1:R597"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A592" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A602" sqref="A602"/>
+      <pane ySplit="3" topLeftCell="A586" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A608" sqref="A608"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28331,6 +28349,9 @@
       <c r="G584" s="4">
         <v>16.739999999999998</v>
       </c>
+      <c r="H584" s="4">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="585" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A585" s="8">
@@ -28339,6 +28360,9 @@
       <c r="B585" s="4">
         <v>7.7069799999999997</v>
       </c>
+      <c r="H585" s="4">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="586" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A586" s="8">
@@ -28347,30 +28371,60 @@
       <c r="B586" s="4">
         <v>7.7055499999999997</v>
       </c>
+      <c r="H586" s="4">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="587" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A587" s="8">
         <v>44049</v>
       </c>
+      <c r="B587" s="4">
+        <v>7.7008599999999996</v>
+      </c>
+      <c r="H587" s="4">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="588" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A588" s="8">
         <v>44050</v>
       </c>
+      <c r="B588" s="4">
+        <v>7.7007000000000003</v>
+      </c>
+      <c r="H588" s="4">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="589" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A589" s="8">
         <v>44051</v>
       </c>
+      <c r="B589" s="4">
+        <v>7.7007000000000003</v>
+      </c>
+      <c r="H589" s="4">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="590" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A590" s="8">
         <v>44052</v>
       </c>
+      <c r="B590" s="27">
+        <v>7.7007000000000003</v>
+      </c>
+      <c r="H590" s="4">
+        <v>11.38</v>
+      </c>
     </row>
     <row r="591" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A591" s="8">
         <v>44053</v>
+      </c>
+      <c r="B591" s="4">
+        <v>7.7002499999999996</v>
       </c>
     </row>
     <row r="592" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-14-2020 22-01-02
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1011" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E0987C32-F64A-4719-943F-9B55DD58D831}"/>
+  <xr:revisionPtr revIDLastSave="1047" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5BA93871-64F9-421B-8BB9-0F1CA501309C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1601,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H597" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H597" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H604" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H604" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1638,8 +1638,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H597" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H597" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H604" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H604" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1970,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R597"/>
+  <dimension ref="A1:R604"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A585" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A601" sqref="A601"/>
+      <pane ySplit="3" topLeftCell="A587" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A608" sqref="A608"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13378,10 +13378,10 @@
         <v>24.575800000000001</v>
       </c>
       <c r="C588" s="22">
-        <v>114.83</v>
+        <v>115.45</v>
       </c>
       <c r="D588" s="22">
-        <v>12.66</v>
+        <v>12.67</v>
       </c>
       <c r="E588" s="22"/>
       <c r="F588" s="22"/>
@@ -13427,8 +13427,12 @@
       <c r="B591" s="28">
         <v>24.562100000000001</v>
       </c>
-      <c r="C591" s="22"/>
-      <c r="D591" s="22"/>
+      <c r="C591" s="22">
+        <v>112.6</v>
+      </c>
+      <c r="D591" s="22">
+        <v>12.55</v>
+      </c>
       <c r="E591" s="22"/>
       <c r="F591" s="22"/>
       <c r="G591" s="22"/>
@@ -13438,9 +13442,15 @@
       <c r="A592" s="8">
         <v>44054</v>
       </c>
-      <c r="B592" s="28"/>
-      <c r="C592" s="22"/>
-      <c r="D592" s="22"/>
+      <c r="B592" s="28">
+        <v>24.550899999999999</v>
+      </c>
+      <c r="C592" s="22">
+        <v>111.35</v>
+      </c>
+      <c r="D592" s="22">
+        <v>12.74</v>
+      </c>
       <c r="E592" s="22"/>
       <c r="F592" s="22"/>
       <c r="G592" s="22"/>
@@ -13450,9 +13460,15 @@
       <c r="A593" s="8">
         <v>44055</v>
       </c>
-      <c r="B593" s="28"/>
-      <c r="C593" s="22"/>
-      <c r="D593" s="22"/>
+      <c r="B593" s="28">
+        <v>24.534099999999999</v>
+      </c>
+      <c r="C593" s="22">
+        <v>112.05</v>
+      </c>
+      <c r="D593" s="22">
+        <v>12.84</v>
+      </c>
       <c r="E593" s="22"/>
       <c r="F593" s="22"/>
       <c r="G593" s="22"/>
@@ -13462,9 +13478,15 @@
       <c r="A594" s="8">
         <v>44056</v>
       </c>
-      <c r="B594" s="28"/>
-      <c r="C594" s="22"/>
-      <c r="D594" s="22"/>
+      <c r="B594" s="28">
+        <v>24.5261</v>
+      </c>
+      <c r="C594" s="22">
+        <v>116.2</v>
+      </c>
+      <c r="D594" s="22">
+        <v>13.11</v>
+      </c>
       <c r="E594" s="22"/>
       <c r="F594" s="22"/>
       <c r="G594" s="22"/>
@@ -13474,9 +13496,15 @@
       <c r="A595" s="8">
         <v>44057</v>
       </c>
-      <c r="B595" s="28"/>
-      <c r="C595" s="22"/>
-      <c r="D595" s="22"/>
+      <c r="B595" s="28">
+        <v>24.523900000000001</v>
+      </c>
+      <c r="C595" s="22">
+        <v>115.2</v>
+      </c>
+      <c r="D595" s="22">
+        <v>13.11</v>
+      </c>
       <c r="E595" s="22"/>
       <c r="F595" s="22"/>
       <c r="G595" s="22"/>
@@ -13501,10 +13529,104 @@
       <c r="B597" s="28"/>
       <c r="C597" s="22"/>
       <c r="D597" s="22"/>
-      <c r="E597" s="22"/>
-      <c r="F597" s="22"/>
-      <c r="G597" s="22"/>
-      <c r="H597" s="22"/>
+      <c r="E597" s="22">
+        <v>81.260000000000005</v>
+      </c>
+      <c r="F597" s="22">
+        <v>74.45</v>
+      </c>
+      <c r="G597" s="22">
+        <v>65.209999999999994</v>
+      </c>
+      <c r="H597" s="22">
+        <v>44.89</v>
+      </c>
+    </row>
+    <row r="598" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A598" s="8">
+        <v>44060</v>
+      </c>
+      <c r="B598" s="28">
+        <v>24.514700000000001</v>
+      </c>
+      <c r="C598" s="22"/>
+      <c r="D598" s="22"/>
+      <c r="E598" s="22"/>
+      <c r="F598" s="22"/>
+      <c r="G598" s="22"/>
+      <c r="H598" s="22"/>
+    </row>
+    <row r="599" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A599" s="8">
+        <v>44061</v>
+      </c>
+      <c r="B599" s="28"/>
+      <c r="C599" s="22"/>
+      <c r="D599" s="22"/>
+      <c r="E599" s="22"/>
+      <c r="F599" s="22"/>
+      <c r="G599" s="22"/>
+      <c r="H599" s="22"/>
+    </row>
+    <row r="600" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A600" s="8">
+        <v>44062</v>
+      </c>
+      <c r="B600" s="28"/>
+      <c r="C600" s="22"/>
+      <c r="D600" s="22"/>
+      <c r="E600" s="22"/>
+      <c r="F600" s="22"/>
+      <c r="G600" s="22"/>
+      <c r="H600" s="22"/>
+    </row>
+    <row r="601" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A601" s="8">
+        <v>44063</v>
+      </c>
+      <c r="B601" s="28"/>
+      <c r="C601" s="22"/>
+      <c r="D601" s="22"/>
+      <c r="E601" s="22"/>
+      <c r="F601" s="22"/>
+      <c r="G601" s="22"/>
+      <c r="H601" s="22"/>
+    </row>
+    <row r="602" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A602" s="8">
+        <v>44064</v>
+      </c>
+      <c r="B602" s="28"/>
+      <c r="C602" s="22"/>
+      <c r="D602" s="22"/>
+      <c r="E602" s="22"/>
+      <c r="F602" s="22"/>
+      <c r="G602" s="22"/>
+      <c r="H602" s="22"/>
+    </row>
+    <row r="603" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A603" s="8">
+        <v>44065</v>
+      </c>
+      <c r="B603" s="28"/>
+      <c r="C603" s="22"/>
+      <c r="D603" s="22"/>
+      <c r="E603" s="22"/>
+      <c r="F603" s="22"/>
+      <c r="G603" s="22"/>
+      <c r="H603" s="22"/>
+    </row>
+    <row r="604" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A604" s="8">
+        <v>44066</v>
+      </c>
+      <c r="B604" s="28"/>
+      <c r="C604" s="22"/>
+      <c r="D604" s="22"/>
+      <c r="E604" s="22"/>
+      <c r="F604" s="22"/>
+      <c r="G604" s="22"/>
+      <c r="H604" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -13525,11 +13647,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R597"/>
+  <dimension ref="A1:R604"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A586" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A608" sqref="A608"/>
+      <pane ySplit="3" topLeftCell="A587" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A609" sqref="A609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28431,30 +28553,86 @@
       <c r="A592" s="8">
         <v>44054</v>
       </c>
-    </row>
-    <row r="593" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B592" s="4">
+        <v>7.6997200000000001</v>
+      </c>
+    </row>
+    <row r="593" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A593" s="8">
         <v>44055</v>
       </c>
-    </row>
-    <row r="594" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B593" s="4">
+        <v>7.70296</v>
+      </c>
+    </row>
+    <row r="594" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A594" s="8">
         <v>44056</v>
       </c>
-    </row>
-    <row r="595" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B594" s="4">
+        <v>7.7010500000000004</v>
+      </c>
+    </row>
+    <row r="595" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A595" s="8">
         <v>44057</v>
       </c>
-    </row>
-    <row r="596" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B595" s="27">
+        <v>7.7010500000000004</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A596" s="8">
         <v>44058</v>
       </c>
-    </row>
-    <row r="597" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B596" s="27">
+        <v>7.7010500000000004</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A597" s="8">
         <v>44059</v>
+      </c>
+      <c r="B597" s="27">
+        <v>7.7010500000000004</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A598" s="8">
+        <v>44060</v>
+      </c>
+      <c r="B598" s="4">
+        <v>7.70024</v>
+      </c>
+    </row>
+    <row r="599" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A599" s="8">
+        <v>44061</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A600" s="8">
+        <v>44062</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A601" s="8">
+        <v>44063</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A602" s="8">
+        <v>44064</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A603" s="8">
+        <v>44065</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A604" s="8">
+        <v>44066</v>
       </c>
     </row>
   </sheetData>
@@ -28472,10 +28650,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-19-2020 06-21-40
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1047" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5BA93871-64F9-421B-8BB9-0F1CA501309C}"/>
+  <xr:revisionPtr revIDLastSave="1063" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{931D7990-0B81-4AF5-8476-BAE6B9D8E53D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="0" windowWidth="14904" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -1601,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H604" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H604" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H611" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H611" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1970,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R604"/>
+  <dimension ref="A1:R611"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A587" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A608" sqref="A608"/>
+      <pane ySplit="3" topLeftCell="A593" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A614" sqref="A614"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13500,10 +13500,10 @@
         <v>24.523900000000001</v>
       </c>
       <c r="C595" s="22">
-        <v>115.2</v>
+        <v>114.7</v>
       </c>
       <c r="D595" s="22">
-        <v>13.11</v>
+        <v>13.1</v>
       </c>
       <c r="E595" s="22"/>
       <c r="F595" s="22"/>
@@ -13549,8 +13549,12 @@
       <c r="B598" s="28">
         <v>24.514700000000001</v>
       </c>
-      <c r="C598" s="22"/>
-      <c r="D598" s="22"/>
+      <c r="C598" s="22">
+        <v>115.55</v>
+      </c>
+      <c r="D598" s="22">
+        <v>13.06</v>
+      </c>
       <c r="E598" s="22"/>
       <c r="F598" s="22"/>
       <c r="G598" s="22"/>
@@ -13560,9 +13564,15 @@
       <c r="A599" s="8">
         <v>44061</v>
       </c>
-      <c r="B599" s="28"/>
-      <c r="C599" s="22"/>
-      <c r="D599" s="22"/>
+      <c r="B599" s="28">
+        <v>24.5123</v>
+      </c>
+      <c r="C599" s="22">
+        <v>120.53</v>
+      </c>
+      <c r="D599" s="22">
+        <v>12.89</v>
+      </c>
       <c r="E599" s="22"/>
       <c r="F599" s="22"/>
       <c r="G599" s="22"/>
@@ -13572,7 +13582,9 @@
       <c r="A600" s="8">
         <v>44062</v>
       </c>
-      <c r="B600" s="28"/>
+      <c r="B600" s="28">
+        <v>24.5016</v>
+      </c>
       <c r="C600" s="22"/>
       <c r="D600" s="22"/>
       <c r="E600" s="22"/>
@@ -13623,10 +13635,102 @@
       <c r="B604" s="28"/>
       <c r="C604" s="22"/>
       <c r="D604" s="22"/>
-      <c r="E604" s="22"/>
-      <c r="F604" s="22"/>
-      <c r="G604" s="22"/>
-      <c r="H604" s="22"/>
+      <c r="E604" s="22">
+        <v>81.040000000000006</v>
+      </c>
+      <c r="F604" s="22">
+        <v>74.489999999999995</v>
+      </c>
+      <c r="G604" s="22">
+        <v>65.180000000000007</v>
+      </c>
+      <c r="H604" s="22">
+        <v>45.08</v>
+      </c>
+    </row>
+    <row r="605" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A605" s="8">
+        <v>44067</v>
+      </c>
+      <c r="B605" s="28"/>
+      <c r="C605" s="22"/>
+      <c r="D605" s="22"/>
+      <c r="E605" s="22"/>
+      <c r="F605" s="22"/>
+      <c r="G605" s="22"/>
+      <c r="H605" s="22"/>
+    </row>
+    <row r="606" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A606" s="8">
+        <v>44068</v>
+      </c>
+      <c r="B606" s="28"/>
+      <c r="C606" s="22"/>
+      <c r="D606" s="22"/>
+      <c r="E606" s="22"/>
+      <c r="F606" s="22"/>
+      <c r="G606" s="22"/>
+      <c r="H606" s="22"/>
+    </row>
+    <row r="607" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A607" s="8">
+        <v>44069</v>
+      </c>
+      <c r="B607" s="28"/>
+      <c r="C607" s="22"/>
+      <c r="D607" s="22"/>
+      <c r="E607" s="22"/>
+      <c r="F607" s="22"/>
+      <c r="G607" s="22"/>
+      <c r="H607" s="22"/>
+    </row>
+    <row r="608" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A608" s="8">
+        <v>44070</v>
+      </c>
+      <c r="B608" s="28"/>
+      <c r="C608" s="22"/>
+      <c r="D608" s="22"/>
+      <c r="E608" s="22"/>
+      <c r="F608" s="22"/>
+      <c r="G608" s="22"/>
+      <c r="H608" s="22"/>
+    </row>
+    <row r="609" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A609" s="8">
+        <v>44071</v>
+      </c>
+      <c r="B609" s="28"/>
+      <c r="C609" s="22"/>
+      <c r="D609" s="22"/>
+      <c r="E609" s="22"/>
+      <c r="F609" s="22"/>
+      <c r="G609" s="22"/>
+      <c r="H609" s="22"/>
+    </row>
+    <row r="610" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A610" s="8">
+        <v>44072</v>
+      </c>
+      <c r="B610" s="28"/>
+      <c r="C610" s="22"/>
+      <c r="D610" s="22"/>
+      <c r="E610" s="22"/>
+      <c r="F610" s="22"/>
+      <c r="G610" s="22"/>
+      <c r="H610" s="22"/>
+    </row>
+    <row r="611" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A611" s="8">
+        <v>44073</v>
+      </c>
+      <c r="B611" s="28"/>
+      <c r="C611" s="22"/>
+      <c r="D611" s="22"/>
+      <c r="E611" s="22"/>
+      <c r="F611" s="22"/>
+      <c r="G611" s="22"/>
+      <c r="H611" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -13650,8 +13754,8 @@
   <dimension ref="A1:R604"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A587" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A609" sqref="A609"/>
+      <pane ySplit="3" topLeftCell="A590" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B609" sqref="B609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28609,10 +28713,16 @@
       <c r="A599" s="8">
         <v>44061</v>
       </c>
+      <c r="B599" s="4">
+        <v>7.6964800000000002</v>
+      </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A600" s="8">
         <v>44062</v>
+      </c>
+      <c r="B600" s="4">
+        <v>7.6989400000000003</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-22-2020 03-16-39
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1063" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{931D7990-0B81-4AF5-8476-BAE6B9D8E53D}"/>
+  <xr:revisionPtr revIDLastSave="1087" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A8A0C5AB-86D9-4445-A6A9-DB9BD259AEDA}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="0" windowWidth="14904" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -1638,8 +1638,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H604" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H604" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H611" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H611" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1973,8 +1973,8 @@
   <dimension ref="A1:R611"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A593" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A614" sqref="A614"/>
+      <pane ySplit="3" topLeftCell="A596" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B614" sqref="B614"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3947,8 +3947,12 @@
         <f t="shared" ref="L45" si="1">+K45&amp;", "&amp;J45</f>
         <v>Junio, 2020</v>
       </c>
-      <c r="M45" s="27"/>
-      <c r="N45" s="2"/>
+      <c r="M45" s="27">
+        <v>0</v>
+      </c>
+      <c r="N45" s="2">
+        <v>0</v>
+      </c>
       <c r="O45" s="27">
         <v>1</v>
       </c>
@@ -3988,10 +3992,18 @@
         <f t="shared" ref="L46:L47" si="2">+K46&amp;", "&amp;J46</f>
         <v>Julio, 2020</v>
       </c>
-      <c r="M46" s="27"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="27"/>
-      <c r="P46" s="2"/>
+      <c r="M46" s="27">
+        <v>0</v>
+      </c>
+      <c r="N46" s="2">
+        <v>0</v>
+      </c>
+      <c r="O46" s="27">
+        <v>2</v>
+      </c>
+      <c r="P46" s="2">
+        <v>4251</v>
+      </c>
       <c r="Q46" s="27"/>
       <c r="R46" s="27"/>
     </row>
@@ -13568,7 +13580,7 @@
         <v>24.5123</v>
       </c>
       <c r="C599" s="22">
-        <v>120.53</v>
+        <v>119.3</v>
       </c>
       <c r="D599" s="22">
         <v>12.89</v>
@@ -13585,8 +13597,12 @@
       <c r="B600" s="28">
         <v>24.5016</v>
       </c>
-      <c r="C600" s="22"/>
-      <c r="D600" s="22"/>
+      <c r="C600" s="22">
+        <v>118.45</v>
+      </c>
+      <c r="D600" s="22">
+        <v>13.24</v>
+      </c>
       <c r="E600" s="22"/>
       <c r="F600" s="22"/>
       <c r="G600" s="22"/>
@@ -13596,9 +13612,15 @@
       <c r="A601" s="8">
         <v>44063</v>
       </c>
-      <c r="B601" s="28"/>
-      <c r="C601" s="22"/>
-      <c r="D601" s="22"/>
+      <c r="B601" s="28">
+        <v>24.502600000000001</v>
+      </c>
+      <c r="C601" s="22">
+        <v>118.55</v>
+      </c>
+      <c r="D601" s="22">
+        <v>13.01</v>
+      </c>
       <c r="E601" s="22"/>
       <c r="F601" s="22"/>
       <c r="G601" s="22"/>
@@ -13608,9 +13630,15 @@
       <c r="A602" s="8">
         <v>44064</v>
       </c>
-      <c r="B602" s="28"/>
-      <c r="C602" s="22"/>
-      <c r="D602" s="22"/>
+      <c r="B602" s="28">
+        <v>24.514800000000001</v>
+      </c>
+      <c r="C602" s="22">
+        <v>119.6</v>
+      </c>
+      <c r="D602" s="22">
+        <v>12.82</v>
+      </c>
       <c r="E602" s="22"/>
       <c r="F602" s="22"/>
       <c r="G602" s="22"/>
@@ -13652,7 +13680,9 @@
       <c r="A605" s="8">
         <v>44067</v>
       </c>
-      <c r="B605" s="28"/>
+      <c r="B605" s="28">
+        <v>24.522400000000001</v>
+      </c>
       <c r="C605" s="22"/>
       <c r="D605" s="22"/>
       <c r="E605" s="22"/>
@@ -13751,11 +13781,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R604"/>
+  <dimension ref="A1:R611"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A590" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B609" sqref="B609"/>
+      <pane ySplit="3" topLeftCell="A595" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A613" sqref="A613"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28729,20 +28759,70 @@
       <c r="A601" s="8">
         <v>44063</v>
       </c>
+      <c r="B601" s="4">
+        <v>7.69998</v>
+      </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A602" s="8">
         <v>44064</v>
       </c>
+      <c r="B602" s="4">
+        <v>7.7013199999999999</v>
+      </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A603" s="8">
         <v>44065</v>
       </c>
+      <c r="B603" s="4">
+        <v>7.7013199999999999</v>
+      </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A604" s="8">
         <v>44066</v>
+      </c>
+      <c r="B604" s="27">
+        <v>7.7013199999999999</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A605" s="8">
+        <v>44067</v>
+      </c>
+      <c r="B605" s="4">
+        <v>7.6959499999999998</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A606" s="8">
+        <v>44068</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A607" s="8">
+        <v>44069</v>
+      </c>
+    </row>
+    <row r="608" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A608" s="8">
+        <v>44070</v>
+      </c>
+    </row>
+    <row r="609" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A609" s="8">
+        <v>44071</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A610" s="8">
+        <v>44072</v>
+      </c>
+    </row>
+    <row r="611" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A611" s="8">
+        <v>44073</v>
       </c>
     </row>
   </sheetData>
@@ -28760,10 +28840,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-26-2020 03-29-15
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1087" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A8A0C5AB-86D9-4445-A6A9-DB9BD259AEDA}"/>
+  <xr:revisionPtr revIDLastSave="1108" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7D4B3A1F-16F8-4792-9C43-063879651DDC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11484" yWindow="0" windowWidth="11544" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -1601,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H611" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H611" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H618" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H618" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1970,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R611"/>
+  <dimension ref="A1:R618"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A596" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B614" sqref="B614"/>
+      <pane ySplit="3" topLeftCell="A598" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A622" sqref="A622"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13634,10 +13634,10 @@
         <v>24.514800000000001</v>
       </c>
       <c r="C602" s="22">
-        <v>119.6</v>
+        <v>120.1</v>
       </c>
       <c r="D602" s="22">
-        <v>12.82</v>
+        <v>12.83</v>
       </c>
       <c r="E602" s="22"/>
       <c r="F602" s="22"/>
@@ -13683,8 +13683,12 @@
       <c r="B605" s="28">
         <v>24.522400000000001</v>
       </c>
-      <c r="C605" s="22"/>
-      <c r="D605" s="22"/>
+      <c r="C605" s="22">
+        <v>120.25</v>
+      </c>
+      <c r="D605" s="22">
+        <v>12.71</v>
+      </c>
       <c r="E605" s="22"/>
       <c r="F605" s="22"/>
       <c r="G605" s="22"/>
@@ -13694,9 +13698,15 @@
       <c r="A606" s="8">
         <v>44068</v>
       </c>
-      <c r="B606" s="28"/>
-      <c r="C606" s="22"/>
-      <c r="D606" s="22"/>
+      <c r="B606" s="28">
+        <v>24.520700000000001</v>
+      </c>
+      <c r="C606" s="22">
+        <v>124.18</v>
+      </c>
+      <c r="D606" s="22">
+        <v>12.75</v>
+      </c>
       <c r="E606" s="22"/>
       <c r="F606" s="22"/>
       <c r="G606" s="22"/>
@@ -13706,7 +13716,9 @@
       <c r="A607" s="8">
         <v>44069</v>
       </c>
-      <c r="B607" s="28"/>
+      <c r="B607" s="28">
+        <v>24.520499999999998</v>
+      </c>
       <c r="C607" s="22"/>
       <c r="D607" s="22"/>
       <c r="E607" s="22"/>
@@ -13757,10 +13769,102 @@
       <c r="B611" s="28"/>
       <c r="C611" s="22"/>
       <c r="D611" s="22"/>
-      <c r="E611" s="22"/>
-      <c r="F611" s="22"/>
-      <c r="G611" s="22"/>
-      <c r="H611" s="22"/>
+      <c r="E611" s="22">
+        <v>81.3</v>
+      </c>
+      <c r="F611" s="22">
+        <v>74.98</v>
+      </c>
+      <c r="G611" s="22">
+        <v>65.22</v>
+      </c>
+      <c r="H611" s="22">
+        <v>45.19</v>
+      </c>
+    </row>
+    <row r="612" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A612" s="8">
+        <v>44074</v>
+      </c>
+      <c r="B612" s="28"/>
+      <c r="C612" s="22"/>
+      <c r="D612" s="22"/>
+      <c r="E612" s="22"/>
+      <c r="F612" s="22"/>
+      <c r="G612" s="22"/>
+      <c r="H612" s="22"/>
+    </row>
+    <row r="613" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A613" s="8">
+        <v>44075</v>
+      </c>
+      <c r="B613" s="28"/>
+      <c r="C613" s="22"/>
+      <c r="D613" s="22"/>
+      <c r="E613" s="22"/>
+      <c r="F613" s="22"/>
+      <c r="G613" s="22"/>
+      <c r="H613" s="22"/>
+    </row>
+    <row r="614" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A614" s="8">
+        <v>44076</v>
+      </c>
+      <c r="B614" s="28"/>
+      <c r="C614" s="22"/>
+      <c r="D614" s="22"/>
+      <c r="E614" s="22"/>
+      <c r="F614" s="22"/>
+      <c r="G614" s="22"/>
+      <c r="H614" s="22"/>
+    </row>
+    <row r="615" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A615" s="8">
+        <v>44077</v>
+      </c>
+      <c r="B615" s="28"/>
+      <c r="C615" s="22"/>
+      <c r="D615" s="22"/>
+      <c r="E615" s="22"/>
+      <c r="F615" s="22"/>
+      <c r="G615" s="22"/>
+      <c r="H615" s="22"/>
+    </row>
+    <row r="616" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A616" s="8">
+        <v>44078</v>
+      </c>
+      <c r="B616" s="28"/>
+      <c r="C616" s="22"/>
+      <c r="D616" s="22"/>
+      <c r="E616" s="22"/>
+      <c r="F616" s="22"/>
+      <c r="G616" s="22"/>
+      <c r="H616" s="22"/>
+    </row>
+    <row r="617" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A617" s="8">
+        <v>44079</v>
+      </c>
+      <c r="B617" s="28"/>
+      <c r="C617" s="22"/>
+      <c r="D617" s="22"/>
+      <c r="E617" s="22"/>
+      <c r="F617" s="22"/>
+      <c r="G617" s="22"/>
+      <c r="H617" s="22"/>
+    </row>
+    <row r="618" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A618" s="8">
+        <v>44080</v>
+      </c>
+      <c r="B618" s="28"/>
+      <c r="C618" s="22"/>
+      <c r="D618" s="22"/>
+      <c r="E618" s="22"/>
+      <c r="F618" s="22"/>
+      <c r="G618" s="22"/>
+      <c r="H618" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -13784,8 +13888,8 @@
   <dimension ref="A1:R611"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A595" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A613" sqref="A613"/>
+      <pane ySplit="3" topLeftCell="A599" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A618" sqref="A618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16020,10 +16124,10 @@
       <c r="M46" s="27"/>
       <c r="N46" s="27"/>
       <c r="O46" s="22">
-        <v>2413.9850000000001</v>
+        <v>4167.2861300000004</v>
       </c>
       <c r="P46" s="22">
-        <v>103.02</v>
+        <v>158.065</v>
       </c>
       <c r="Q46" s="27"/>
       <c r="R46" s="27"/>
@@ -16066,8 +16170,12 @@
       </c>
       <c r="M47" s="27"/>
       <c r="N47" s="2"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="22"/>
+      <c r="O47" s="22">
+        <v>2553.4050000000002</v>
+      </c>
+      <c r="P47" s="22">
+        <v>84.5</v>
+      </c>
       <c r="Q47" s="27"/>
       <c r="R47" s="27"/>
     </row>
@@ -28799,10 +28907,16 @@
       <c r="A606" s="8">
         <v>44068</v>
       </c>
+      <c r="B606" s="4">
+        <v>7.6982299999999997</v>
+      </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A607" s="8">
         <v>44069</v>
+      </c>
+      <c r="B607" s="4">
+        <v>7.7026199999999996</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.3">
@@ -28840,7 +28954,7 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F27" sqref="F27"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-29-2020 00-42-21
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1108" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7D4B3A1F-16F8-4792-9C43-063879651DDC}"/>
+  <xr:revisionPtr revIDLastSave="1128" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FEA8842-4D17-40AE-BCA9-D5BF469EDE1E}"/>
   <bookViews>
-    <workbookView xWindow="11484" yWindow="0" windowWidth="11544" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HONDURAS" sheetId="2" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2455" uniqueCount="133">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1638,8 +1638,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H611" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H611" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H618" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H618" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1655,8 +1655,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R47" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R47" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R49" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R49" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="6"/>
@@ -1973,8 +1973,8 @@
   <dimension ref="A1:R618"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A598" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A622" sqref="A622"/>
+      <pane ySplit="3" topLeftCell="A600" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A625" sqref="A625"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13702,10 +13702,10 @@
         <v>24.520700000000001</v>
       </c>
       <c r="C606" s="22">
-        <v>124.18</v>
+        <v>123.2</v>
       </c>
       <c r="D606" s="22">
-        <v>12.75</v>
+        <v>12.76</v>
       </c>
       <c r="E606" s="22"/>
       <c r="F606" s="22"/>
@@ -13719,8 +13719,12 @@
       <c r="B607" s="28">
         <v>24.520499999999998</v>
       </c>
-      <c r="C607" s="22"/>
-      <c r="D607" s="22"/>
+      <c r="C607" s="22">
+        <v>122.8</v>
+      </c>
+      <c r="D607" s="22">
+        <v>12.58</v>
+      </c>
       <c r="E607" s="22"/>
       <c r="F607" s="22"/>
       <c r="G607" s="22"/>
@@ -13730,9 +13734,15 @@
       <c r="A608" s="8">
         <v>44070</v>
       </c>
-      <c r="B608" s="28"/>
-      <c r="C608" s="22"/>
-      <c r="D608" s="22"/>
+      <c r="B608" s="28">
+        <v>24.519600000000001</v>
+      </c>
+      <c r="C608" s="22">
+        <v>122.95</v>
+      </c>
+      <c r="D608" s="22">
+        <v>12.77</v>
+      </c>
       <c r="E608" s="22"/>
       <c r="F608" s="22"/>
       <c r="G608" s="22"/>
@@ -13742,9 +13752,15 @@
       <c r="A609" s="8">
         <v>44071</v>
       </c>
-      <c r="B609" s="28"/>
-      <c r="C609" s="22"/>
-      <c r="D609" s="22"/>
+      <c r="B609" s="28">
+        <v>24.516200000000001</v>
+      </c>
+      <c r="C609" s="22">
+        <v>126.38</v>
+      </c>
+      <c r="D609" s="22">
+        <v>12.62</v>
+      </c>
       <c r="E609" s="22"/>
       <c r="F609" s="22"/>
       <c r="G609" s="22"/>
@@ -13786,7 +13802,9 @@
       <c r="A612" s="8">
         <v>44074</v>
       </c>
-      <c r="B612" s="28"/>
+      <c r="B612" s="28">
+        <v>24.513000000000002</v>
+      </c>
       <c r="C612" s="22"/>
       <c r="D612" s="22"/>
       <c r="E612" s="22"/>
@@ -13885,11 +13903,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R611"/>
+  <dimension ref="A1:R618"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A599" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A618" sqref="A618"/>
+      <pane ySplit="3" topLeftCell="A601" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A623" sqref="A623"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16205,17 +16223,24 @@
         <v>15.15</v>
       </c>
       <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
+      <c r="J48" s="9">
+        <v>2020</v>
+      </c>
+      <c r="K48" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L48" s="9" t="str">
+        <f t="shared" ref="L48:L49" si="3">+K48&amp;", "&amp;J48</f>
+        <v>Septiembre, 2020</v>
+      </c>
       <c r="M48" s="27"/>
-      <c r="N48" s="27"/>
-      <c r="O48" s="27"/>
-      <c r="P48" s="27"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="22"/>
+      <c r="P48" s="22"/>
       <c r="Q48" s="27"/>
       <c r="R48" s="27"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>43511</v>
       </c>
@@ -16240,8 +16265,21 @@
       <c r="H49" s="27">
         <v>15.15</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J49" s="9">
+        <v>2020</v>
+      </c>
+      <c r="K49" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L49" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>Octubre, 2020</v>
+      </c>
+      <c r="N49" s="2"/>
+      <c r="O49" s="22"/>
+      <c r="P49" s="22"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>43512</v>
       </c>
@@ -16267,7 +16305,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>43513</v>
       </c>
@@ -16293,7 +16331,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>43514</v>
       </c>
@@ -16319,7 +16357,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>43515</v>
       </c>
@@ -16345,7 +16383,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>43516</v>
       </c>
@@ -16371,7 +16409,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>43517</v>
       </c>
@@ -16397,7 +16435,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>43518</v>
       </c>
@@ -16423,7 +16461,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>43519</v>
       </c>
@@ -16449,7 +16487,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>43520</v>
       </c>
@@ -16475,7 +16513,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>43521</v>
       </c>
@@ -16501,7 +16539,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <v>43522</v>
       </c>
@@ -16527,7 +16565,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
         <v>43523</v>
       </c>
@@ -16553,7 +16591,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <v>43524</v>
       </c>
@@ -16579,7 +16617,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
         <v>43525</v>
       </c>
@@ -16605,7 +16643,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <v>43526</v>
       </c>
@@ -28923,20 +28961,70 @@
       <c r="A608" s="8">
         <v>44070</v>
       </c>
-    </row>
-    <row r="609" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B608" s="4">
+        <v>7.7102899999999996</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A609" s="8">
         <v>44071</v>
       </c>
-    </row>
-    <row r="610" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B609" s="4">
+        <v>7.7250800000000002</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A610" s="8">
         <v>44072</v>
       </c>
-    </row>
-    <row r="611" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B610" s="27">
+        <v>7.7250800000000002</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A611" s="8">
         <v>44073</v>
+      </c>
+      <c r="B611" s="27">
+        <v>7.7250800000000002</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A612" s="8">
+        <v>44074</v>
+      </c>
+      <c r="B612" s="4">
+        <v>7.7299100000000003</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A613" s="8">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A614" s="8">
+        <v>44076</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A615" s="8">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="616" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A616" s="8">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="617" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A617" s="8">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A618" s="8">
+        <v>44080</v>
       </c>
     </row>
   </sheetData>
@@ -28954,10 +29042,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-02-2020 01-29-15
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1128" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FEA8842-4D17-40AE-BCA9-D5BF469EDE1E}"/>
+  <xr:revisionPtr revIDLastSave="1166" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F3F012C9-7AEF-4668-BD5B-B50EED92389D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2455" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="133">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1203,22 +1203,6 @@
   <dxfs count="29">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1344,6 +1328,22 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1601,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H618" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H618" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H625" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H625" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1618,8 +1618,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R47" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R47" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_HN" displayName="Indicadores_mes_HN" ref="J3:R49" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R49" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="14"/>
@@ -1638,8 +1638,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H618" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H618" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H625" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H625" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1655,18 +1655,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R49" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R49" totalsRowShown="0" headerRowDxfId="6" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R49" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="3">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{B7D1225A-C849-430C-8F2C-569D3B5E64AD}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="4" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="3" dataCellStyle="Millares [0]"/>
-    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="2" dataCellStyle="Millares [0]"/>
+    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="2" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="1" dataCellStyle="Millares [0]"/>
+    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="0" dataCellStyle="Millares [0]"/>
     <tableColumn id="8" xr3:uid="{552CA574-1C46-4E0F-8C54-8DBCDA6B12C1}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{C793523A-103E-4CA7-94B8-3E3D9A633FDB}" name="Ingresos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1675,7 +1675,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="8">
   <autoFilter ref="A1:U36" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -1698,7 +1698,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1970,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R618"/>
+  <dimension ref="A1:R625"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A600" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A625" sqref="A625"/>
+      <pane ySplit="3" topLeftCell="A609" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A631" sqref="A631"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4005,7 +4005,9 @@
         <v>4251</v>
       </c>
       <c r="Q46" s="27"/>
-      <c r="R46" s="27"/>
+      <c r="R46" s="27">
+        <v>515.79999999999995</v>
+      </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
@@ -4060,17 +4062,24 @@
       <c r="G48" s="22"/>
       <c r="H48" s="22"/>
       <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
+      <c r="J48" s="9">
+        <v>2020</v>
+      </c>
+      <c r="K48" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L48" s="9" t="str">
+        <f t="shared" ref="L48:L49" si="3">+K48&amp;", "&amp;J48</f>
+        <v>Septiembre, 2020</v>
+      </c>
       <c r="M48" s="27"/>
-      <c r="N48" s="27"/>
+      <c r="N48" s="2"/>
       <c r="O48" s="27"/>
-      <c r="P48" s="27"/>
+      <c r="P48" s="2"/>
       <c r="Q48" s="27"/>
       <c r="R48" s="27"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>43511</v>
       </c>
@@ -4095,8 +4104,20 @@
       <c r="H49" s="22">
         <v>64.989999999999995</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J49" s="9">
+        <v>2020</v>
+      </c>
+      <c r="K49" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L49" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>Octubre, 2020</v>
+      </c>
+      <c r="N49" s="2"/>
+      <c r="P49" s="2"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>43512</v>
       </c>
@@ -4108,7 +4129,7 @@
       <c r="G50" s="22"/>
       <c r="H50" s="22"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>43513</v>
       </c>
@@ -4120,7 +4141,7 @@
       <c r="G51" s="22"/>
       <c r="H51" s="22"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>43514</v>
       </c>
@@ -4136,7 +4157,7 @@
       <c r="G52" s="22"/>
       <c r="H52" s="22"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>43515</v>
       </c>
@@ -4154,7 +4175,7 @@
       <c r="G53" s="22"/>
       <c r="H53" s="22"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>43516</v>
       </c>
@@ -4172,7 +4193,7 @@
       <c r="G54" s="22"/>
       <c r="H54" s="22"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>43517</v>
       </c>
@@ -4190,7 +4211,7 @@
       <c r="G55" s="22"/>
       <c r="H55" s="22"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>43518</v>
       </c>
@@ -4216,7 +4237,7 @@
         <v>65.400000000000006</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>43519</v>
       </c>
@@ -4228,7 +4249,7 @@
       <c r="G57" s="22"/>
       <c r="H57" s="22"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>43520</v>
       </c>
@@ -4240,7 +4261,7 @@
       <c r="G58" s="22"/>
       <c r="H58" s="22"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>43521</v>
       </c>
@@ -4258,7 +4279,7 @@
       <c r="G59" s="22"/>
       <c r="H59" s="22"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <v>43522</v>
       </c>
@@ -4276,7 +4297,7 @@
       <c r="G60" s="22"/>
       <c r="H60" s="22"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
         <v>43523</v>
       </c>
@@ -4294,7 +4315,7 @@
       <c r="G61" s="22"/>
       <c r="H61" s="22"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <v>43524</v>
       </c>
@@ -4312,7 +4333,7 @@
       <c r="G62" s="22"/>
       <c r="H62" s="22"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
         <v>43525</v>
       </c>
@@ -4338,7 +4359,7 @@
         <v>65.400000000000006</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <v>43526</v>
       </c>
@@ -13756,10 +13777,10 @@
         <v>24.516200000000001</v>
       </c>
       <c r="C609" s="22">
-        <v>126.38</v>
+        <v>127.1</v>
       </c>
       <c r="D609" s="22">
-        <v>12.62</v>
+        <v>12.6</v>
       </c>
       <c r="E609" s="22"/>
       <c r="F609" s="22"/>
@@ -13805,8 +13826,12 @@
       <c r="B612" s="28">
         <v>24.513000000000002</v>
       </c>
-      <c r="C612" s="22"/>
-      <c r="D612" s="22"/>
+      <c r="C612" s="22">
+        <v>129.80000000000001</v>
+      </c>
+      <c r="D612" s="22">
+        <v>12.66</v>
+      </c>
       <c r="E612" s="22"/>
       <c r="F612" s="22"/>
       <c r="G612" s="22"/>
@@ -13816,9 +13841,15 @@
       <c r="A613" s="8">
         <v>44075</v>
       </c>
-      <c r="B613" s="28"/>
-      <c r="C613" s="22"/>
-      <c r="D613" s="22"/>
+      <c r="B613" s="28">
+        <v>24.5092</v>
+      </c>
+      <c r="C613" s="22">
+        <v>130.65</v>
+      </c>
+      <c r="D613" s="22">
+        <v>12.59</v>
+      </c>
       <c r="E613" s="22"/>
       <c r="F613" s="22"/>
       <c r="G613" s="22"/>
@@ -13828,7 +13859,9 @@
       <c r="A614" s="8">
         <v>44076</v>
       </c>
-      <c r="B614" s="28"/>
+      <c r="B614" s="28">
+        <v>24.5046</v>
+      </c>
       <c r="C614" s="22"/>
       <c r="D614" s="22"/>
       <c r="E614" s="22"/>
@@ -13879,10 +13912,102 @@
       <c r="B618" s="28"/>
       <c r="C618" s="22"/>
       <c r="D618" s="22"/>
-      <c r="E618" s="22"/>
-      <c r="F618" s="22"/>
-      <c r="G618" s="22"/>
-      <c r="H618" s="22"/>
+      <c r="E618" s="22">
+        <v>81.87</v>
+      </c>
+      <c r="F618" s="22">
+        <v>75.59</v>
+      </c>
+      <c r="G618" s="22">
+        <v>65.06</v>
+      </c>
+      <c r="H618" s="22">
+        <v>45.19</v>
+      </c>
+    </row>
+    <row r="619" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A619" s="8">
+        <v>44081</v>
+      </c>
+      <c r="B619" s="28"/>
+      <c r="C619" s="22"/>
+      <c r="D619" s="22"/>
+      <c r="E619" s="22"/>
+      <c r="F619" s="22"/>
+      <c r="G619" s="22"/>
+      <c r="H619" s="22"/>
+    </row>
+    <row r="620" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A620" s="8">
+        <v>44082</v>
+      </c>
+      <c r="B620" s="28"/>
+      <c r="C620" s="22"/>
+      <c r="D620" s="22"/>
+      <c r="E620" s="22"/>
+      <c r="F620" s="22"/>
+      <c r="G620" s="22"/>
+      <c r="H620" s="22"/>
+    </row>
+    <row r="621" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A621" s="8">
+        <v>44083</v>
+      </c>
+      <c r="B621" s="28"/>
+      <c r="C621" s="22"/>
+      <c r="D621" s="22"/>
+      <c r="E621" s="22"/>
+      <c r="F621" s="22"/>
+      <c r="G621" s="22"/>
+      <c r="H621" s="22"/>
+    </row>
+    <row r="622" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A622" s="8">
+        <v>44084</v>
+      </c>
+      <c r="B622" s="28"/>
+      <c r="C622" s="22"/>
+      <c r="D622" s="22"/>
+      <c r="E622" s="22"/>
+      <c r="F622" s="22"/>
+      <c r="G622" s="22"/>
+      <c r="H622" s="22"/>
+    </row>
+    <row r="623" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A623" s="8">
+        <v>44085</v>
+      </c>
+      <c r="B623" s="28"/>
+      <c r="C623" s="22"/>
+      <c r="D623" s="22"/>
+      <c r="E623" s="22"/>
+      <c r="F623" s="22"/>
+      <c r="G623" s="22"/>
+      <c r="H623" s="22"/>
+    </row>
+    <row r="624" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A624" s="8">
+        <v>44086</v>
+      </c>
+      <c r="B624" s="28"/>
+      <c r="C624" s="22"/>
+      <c r="D624" s="22"/>
+      <c r="E624" s="22"/>
+      <c r="F624" s="22"/>
+      <c r="G624" s="22"/>
+      <c r="H624" s="22"/>
+    </row>
+    <row r="625" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A625" s="8">
+        <v>44087</v>
+      </c>
+      <c r="B625" s="28"/>
+      <c r="C625" s="22"/>
+      <c r="D625" s="22"/>
+      <c r="E625" s="22"/>
+      <c r="F625" s="22"/>
+      <c r="G625" s="22"/>
+      <c r="H625" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -13903,11 +14028,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R618"/>
+  <dimension ref="A1:R625"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A601" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A623" sqref="A623"/>
+      <pane ySplit="3" topLeftCell="A609" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A631" sqref="A631"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15755,7 +15880,9 @@
       <c r="P38" s="22">
         <v>388.65</v>
       </c>
-      <c r="Q38" s="27"/>
+      <c r="Q38" s="27">
+        <v>2</v>
+      </c>
       <c r="R38" s="27">
         <v>818.6</v>
       </c>
@@ -16002,7 +16129,7 @@
       </c>
       <c r="Q43" s="27"/>
       <c r="R43" s="27">
-        <v>690.6</v>
+        <v>690.5</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
@@ -16051,7 +16178,7 @@
       </c>
       <c r="Q44" s="27"/>
       <c r="R44" s="27">
-        <v>836.6</v>
+        <v>835.8</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
@@ -16100,7 +16227,7 @@
       </c>
       <c r="Q45" s="27"/>
       <c r="R45" s="27">
-        <v>963</v>
+        <v>961.8</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
@@ -16148,7 +16275,9 @@
         <v>158.065</v>
       </c>
       <c r="Q46" s="27"/>
-      <c r="R46" s="27"/>
+      <c r="R46" s="27">
+        <v>1076.7</v>
+      </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
@@ -28837,7 +28966,7 @@
         <v>7.6997200000000001</v>
       </c>
     </row>
-    <row r="593" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="593" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A593" s="8">
         <v>44055</v>
       </c>
@@ -28845,7 +28974,7 @@
         <v>7.70296</v>
       </c>
     </row>
-    <row r="594" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="594" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A594" s="8">
         <v>44056</v>
       </c>
@@ -28853,7 +28982,7 @@
         <v>7.7010500000000004</v>
       </c>
     </row>
-    <row r="595" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="595" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A595" s="8">
         <v>44057</v>
       </c>
@@ -28861,7 +28990,7 @@
         <v>7.7010500000000004</v>
       </c>
     </row>
-    <row r="596" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="596" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A596" s="8">
         <v>44058</v>
       </c>
@@ -28869,7 +28998,7 @@
         <v>7.7010500000000004</v>
       </c>
     </row>
-    <row r="597" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="597" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A597" s="8">
         <v>44059</v>
       </c>
@@ -28877,7 +29006,7 @@
         <v>7.7010500000000004</v>
       </c>
     </row>
-    <row r="598" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A598" s="8">
         <v>44060</v>
       </c>
@@ -28885,7 +29014,7 @@
         <v>7.70024</v>
       </c>
     </row>
-    <row r="599" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="599" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A599" s="8">
         <v>44061</v>
       </c>
@@ -28893,7 +29022,7 @@
         <v>7.6964800000000002</v>
       </c>
     </row>
-    <row r="600" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="600" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A600" s="8">
         <v>44062</v>
       </c>
@@ -28901,7 +29030,7 @@
         <v>7.6989400000000003</v>
       </c>
     </row>
-    <row r="601" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="601" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A601" s="8">
         <v>44063</v>
       </c>
@@ -28909,7 +29038,7 @@
         <v>7.69998</v>
       </c>
     </row>
-    <row r="602" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="602" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A602" s="8">
         <v>44064</v>
       </c>
@@ -28917,7 +29046,7 @@
         <v>7.7013199999999999</v>
       </c>
     </row>
-    <row r="603" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="603" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A603" s="8">
         <v>44065</v>
       </c>
@@ -28925,7 +29054,7 @@
         <v>7.7013199999999999</v>
       </c>
     </row>
-    <row r="604" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="604" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A604" s="8">
         <v>44066</v>
       </c>
@@ -28933,15 +29062,24 @@
         <v>7.7013199999999999</v>
       </c>
     </row>
-    <row r="605" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="605" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A605" s="8">
         <v>44067</v>
       </c>
       <c r="B605" s="4">
         <v>7.6959499999999998</v>
       </c>
-    </row>
-    <row r="606" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E605" s="4">
+        <v>20.98</v>
+      </c>
+      <c r="F605" s="4">
+        <v>20.18</v>
+      </c>
+      <c r="G605" s="4">
+        <v>16.59</v>
+      </c>
+    </row>
+    <row r="606" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A606" s="8">
         <v>44068</v>
       </c>
@@ -28949,7 +29087,7 @@
         <v>7.6982299999999997</v>
       </c>
     </row>
-    <row r="607" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="607" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A607" s="8">
         <v>44069</v>
       </c>
@@ -28957,7 +29095,7 @@
         <v>7.7026199999999996</v>
       </c>
     </row>
-    <row r="608" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="608" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A608" s="8">
         <v>44070</v>
       </c>
@@ -28965,7 +29103,7 @@
         <v>7.7102899999999996</v>
       </c>
     </row>
-    <row r="609" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="609" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A609" s="8">
         <v>44071</v>
       </c>
@@ -28973,7 +29111,7 @@
         <v>7.7250800000000002</v>
       </c>
     </row>
-    <row r="610" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="610" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A610" s="8">
         <v>44072</v>
       </c>
@@ -28981,7 +29119,7 @@
         <v>7.7250800000000002</v>
       </c>
     </row>
-    <row r="611" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="611" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A611" s="8">
         <v>44073</v>
       </c>
@@ -28989,42 +29127,89 @@
         <v>7.7250800000000002</v>
       </c>
     </row>
-    <row r="612" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="612" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A612" s="8">
         <v>44074</v>
       </c>
       <c r="B612" s="4">
         <v>7.7299100000000003</v>
       </c>
-    </row>
-    <row r="613" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E612" s="4">
+        <v>21.4</v>
+      </c>
+      <c r="F612" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="G612" s="4">
+        <v>16.420000000000002</v>
+      </c>
+    </row>
+    <row r="613" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A613" s="8">
         <v>44075</v>
       </c>
-    </row>
-    <row r="614" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B613" s="27">
+        <v>7.7296100000000001</v>
+      </c>
+    </row>
+    <row r="614" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A614" s="8">
         <v>44076</v>
       </c>
     </row>
-    <row r="615" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="615" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A615" s="8">
         <v>44077</v>
       </c>
     </row>
-    <row r="616" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="616" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A616" s="8">
         <v>44078</v>
       </c>
     </row>
-    <row r="617" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="617" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A617" s="8">
         <v>44079</v>
       </c>
     </row>
-    <row r="618" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="618" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A618" s="8">
         <v>44080</v>
+      </c>
+    </row>
+    <row r="619" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A619" s="8">
+        <v>44081</v>
+      </c>
+    </row>
+    <row r="620" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A620" s="8">
+        <v>44082</v>
+      </c>
+    </row>
+    <row r="621" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A621" s="8">
+        <v>44083</v>
+      </c>
+    </row>
+    <row r="622" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A622" s="8">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="623" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A623" s="8">
+        <v>44085</v>
+      </c>
+    </row>
+    <row r="624" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A624" s="8">
+        <v>44086</v>
+      </c>
+    </row>
+    <row r="625" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A625" s="8">
+        <v>44087</v>
       </c>
     </row>
   </sheetData>
@@ -29042,10 +29227,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31744,22 +31929,22 @@
     <hyperlink ref="J6:J8" r:id="rId34" display="https://www.mem.gob.gt/" xr:uid="{A84CC70A-0414-4A2E-BEC8-5680985BE81A}"/>
     <hyperlink ref="H5" r:id="rId35" xr:uid="{D6CB5105-27CA-4EBD-8FAF-6AD03BA57E8E}"/>
     <hyperlink ref="H6:H8" r:id="rId36" display="https://www.mem.gob.gt/contacto/escribenos/" xr:uid="{2E1D2851-EF7B-4D6D-88ED-9BA745AF8A9B}"/>
-    <hyperlink ref="F9" r:id="rId37" xr:uid="{EBD6F2F9-A288-4A48-AD1C-B027F0B1FDCC}"/>
-    <hyperlink ref="F10" r:id="rId38" xr:uid="{5388C766-549D-4DB9-B8A2-EF392AA68BF7}"/>
-    <hyperlink ref="K9" r:id="rId39" xr:uid="{C9FF6777-B7D0-49C1-AFC0-42C7B34A16CC}"/>
-    <hyperlink ref="J9" r:id="rId40" xr:uid="{D3E3CC2A-5411-4646-85D7-6917F62C49C4}"/>
-    <hyperlink ref="H9" r:id="rId41" xr:uid="{B0996637-B8DB-4605-AAE3-1BD61E4675C6}"/>
-    <hyperlink ref="K10" r:id="rId42" xr:uid="{729A966F-2F4A-4CE1-986B-C3B4D21BE0E6}"/>
-    <hyperlink ref="J10" r:id="rId43" xr:uid="{B180DAC5-027A-49A2-8EE3-C47F162824D8}"/>
-    <hyperlink ref="H10" r:id="rId44" xr:uid="{4180A254-40D1-4B19-B9ED-BC98556E01E0}"/>
-    <hyperlink ref="F11" r:id="rId45" xr:uid="{AD0FFFD7-B5EA-4CC6-A2D7-FC711CD9E273}"/>
-    <hyperlink ref="J11" r:id="rId46" xr:uid="{8D3835B9-F568-4D8F-9CD9-8D260D5A6E1A}"/>
-    <hyperlink ref="F12" r:id="rId47" xr:uid="{5BF57AB9-6786-45D4-9B41-00A80ED5A879}"/>
-    <hyperlink ref="J12" r:id="rId48" xr:uid="{610A88D3-7410-471E-8CBA-E264F4E6D8F1}"/>
-    <hyperlink ref="H12" r:id="rId49" xr:uid="{C39C3BB3-728F-42C9-9F79-687468489142}"/>
-    <hyperlink ref="F21:F23" r:id="rId50" display="https://www.bch.hn/estadisticassv.php" xr:uid="{F479A45E-5F7A-41F4-8FCD-0A3A67241764}"/>
-    <hyperlink ref="F5" r:id="rId51" xr:uid="{EB6C19CD-A8BD-482E-B1F2-F7AE05904A57}"/>
-    <hyperlink ref="F6:F8" r:id="rId52" display="https://www.mem.gob.gt/hidrocarburos/precios-combustible-nacionales/" xr:uid="{630442E1-9898-4043-AFD9-BEF9DF0EFD23}"/>
+    <hyperlink ref="F10" r:id="rId37" xr:uid="{5388C766-549D-4DB9-B8A2-EF392AA68BF7}"/>
+    <hyperlink ref="K9" r:id="rId38" xr:uid="{C9FF6777-B7D0-49C1-AFC0-42C7B34A16CC}"/>
+    <hyperlink ref="J9" r:id="rId39" xr:uid="{D3E3CC2A-5411-4646-85D7-6917F62C49C4}"/>
+    <hyperlink ref="H9" r:id="rId40" xr:uid="{B0996637-B8DB-4605-AAE3-1BD61E4675C6}"/>
+    <hyperlink ref="K10" r:id="rId41" xr:uid="{729A966F-2F4A-4CE1-986B-C3B4D21BE0E6}"/>
+    <hyperlink ref="J10" r:id="rId42" xr:uid="{B180DAC5-027A-49A2-8EE3-C47F162824D8}"/>
+    <hyperlink ref="H10" r:id="rId43" xr:uid="{4180A254-40D1-4B19-B9ED-BC98556E01E0}"/>
+    <hyperlink ref="F11" r:id="rId44" xr:uid="{AD0FFFD7-B5EA-4CC6-A2D7-FC711CD9E273}"/>
+    <hyperlink ref="J11" r:id="rId45" xr:uid="{8D3835B9-F568-4D8F-9CD9-8D260D5A6E1A}"/>
+    <hyperlink ref="F12" r:id="rId46" xr:uid="{5BF57AB9-6786-45D4-9B41-00A80ED5A879}"/>
+    <hyperlink ref="J12" r:id="rId47" xr:uid="{610A88D3-7410-471E-8CBA-E264F4E6D8F1}"/>
+    <hyperlink ref="H12" r:id="rId48" xr:uid="{C39C3BB3-728F-42C9-9F79-687468489142}"/>
+    <hyperlink ref="F21:F23" r:id="rId49" display="https://www.bch.hn/estadisticassv.php" xr:uid="{F479A45E-5F7A-41F4-8FCD-0A3A67241764}"/>
+    <hyperlink ref="F5" r:id="rId50" xr:uid="{EB6C19CD-A8BD-482E-B1F2-F7AE05904A57}"/>
+    <hyperlink ref="F6:F8" r:id="rId51" display="https://www.mem.gob.gt/hidrocarburos/precios-combustible-nacionales/" xr:uid="{630442E1-9898-4043-AFD9-BEF9DF0EFD23}"/>
+    <hyperlink ref="F9" r:id="rId52" xr:uid="{EBD6F2F9-A288-4A48-AD1C-B027F0B1FDCC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-05-2020 05-38-17
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1166" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F3F012C9-7AEF-4668-BD5B-B50EED92389D}"/>
+  <xr:revisionPtr revIDLastSave="1189" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BAB924BD-2A6A-4A4E-8FD5-637A8619EC18}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1203,6 +1203,22 @@
   <dxfs count="29">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1328,22 +1344,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1655,18 +1655,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R49" totalsRowShown="0" headerRowDxfId="6" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2883321-A619-4C20-9FAB-4D6F6A60E278}" name="Indicadores_mes_GT" displayName="Indicadores_mes_GT" ref="J3:R49" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R49" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{5AFC3F5A-A075-406F-9360-8992BBE17F43}" name="Año" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{A2961B12-CF36-4F32-9CD0-BA9FDC49E1CD}" name="Mes" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{89C984C2-971D-43A3-9AEE-9C102BDC39EF}" name="Fecha" dataDxfId="5">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{B7D1225A-C849-430C-8F2C-569D3B5E64AD}" name="Número de Operaciones"/>
-    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="2" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="1" dataCellStyle="Millares [0]"/>
-    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="0" dataCellStyle="Millares [0]"/>
+    <tableColumn id="5" xr3:uid="{C99E4801-B4E9-4759-9CB5-3E08D881B72D}" name="Monto Inversión (millones de QUETZALES)" dataDxfId="4" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{46724685-CFCF-4D96-A3EA-0E3C2537B5E5}" name="Montos Negociados Operaciones de Reporto (millones de QUETZALES)" dataDxfId="3" dataCellStyle="Millares [0]"/>
+    <tableColumn id="7" xr3:uid="{C5073926-6E73-4688-8DB0-37A308B9381B}" name="Montos Negociados Operaciones de Reporto (millones de USD)" dataDxfId="2" dataCellStyle="Millares [0]"/>
     <tableColumn id="8" xr3:uid="{552CA574-1C46-4E0F-8C54-8DBCDA6B12C1}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{C793523A-103E-4CA7-94B8-3E3D9A633FDB}" name="Ingresos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1675,7 +1675,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U36" headerRowDxfId="1">
   <autoFilter ref="A1:U36" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -1698,7 +1698,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1972,9 +1972,9 @@
   </sheetPr>
   <dimension ref="A1:R625"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A609" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A631" sqref="A631"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4037,10 +4037,18 @@
         <f t="shared" si="2"/>
         <v>Agosto, 2020</v>
       </c>
-      <c r="M47" s="27"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="27"/>
-      <c r="P47" s="2"/>
+      <c r="M47" s="27">
+        <v>0</v>
+      </c>
+      <c r="N47" s="2">
+        <v>0</v>
+      </c>
+      <c r="O47" s="27">
+        <v>1</v>
+      </c>
+      <c r="P47" s="2">
+        <v>3900</v>
+      </c>
       <c r="Q47" s="27"/>
       <c r="R47" s="27"/>
     </row>
@@ -13830,7 +13838,7 @@
         <v>129.80000000000001</v>
       </c>
       <c r="D612" s="22">
-        <v>12.66</v>
+        <v>12.65</v>
       </c>
       <c r="E612" s="22"/>
       <c r="F612" s="22"/>
@@ -13845,10 +13853,10 @@
         <v>24.5092</v>
       </c>
       <c r="C613" s="22">
-        <v>130.65</v>
+        <v>131.9</v>
       </c>
       <c r="D613" s="22">
-        <v>12.59</v>
+        <v>12.66</v>
       </c>
       <c r="E613" s="22"/>
       <c r="F613" s="22"/>
@@ -13862,8 +13870,12 @@
       <c r="B614" s="28">
         <v>24.5046</v>
       </c>
-      <c r="C614" s="22"/>
-      <c r="D614" s="22"/>
+      <c r="C614" s="22">
+        <v>131.5</v>
+      </c>
+      <c r="D614" s="22">
+        <v>12.6</v>
+      </c>
       <c r="E614" s="22"/>
       <c r="F614" s="22"/>
       <c r="G614" s="22"/>
@@ -13873,9 +13885,15 @@
       <c r="A615" s="8">
         <v>44077</v>
       </c>
-      <c r="B615" s="28"/>
-      <c r="C615" s="22"/>
-      <c r="D615" s="22"/>
+      <c r="B615" s="28">
+        <v>24.5032</v>
+      </c>
+      <c r="C615" s="22">
+        <v>131.6</v>
+      </c>
+      <c r="D615" s="22">
+        <v>12.41</v>
+      </c>
       <c r="E615" s="22"/>
       <c r="F615" s="22"/>
       <c r="G615" s="22"/>
@@ -13885,9 +13903,15 @@
       <c r="A616" s="8">
         <v>44078</v>
       </c>
-      <c r="B616" s="28"/>
-      <c r="C616" s="22"/>
-      <c r="D616" s="22"/>
+      <c r="B616" s="28">
+        <v>24.502500000000001</v>
+      </c>
+      <c r="C616" s="22">
+        <v>134.69999999999999</v>
+      </c>
+      <c r="D616" s="22">
+        <v>12.09</v>
+      </c>
       <c r="E616" s="22"/>
       <c r="F616" s="22"/>
       <c r="G616" s="22"/>
@@ -13929,7 +13953,9 @@
       <c r="A619" s="8">
         <v>44081</v>
       </c>
-      <c r="B619" s="28"/>
+      <c r="B619" s="28">
+        <v>24.502300000000002</v>
+      </c>
       <c r="C619" s="22"/>
       <c r="D619" s="22"/>
       <c r="E619" s="22"/>
@@ -14031,8 +14057,8 @@
   <dimension ref="A1:R625"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A609" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A631" sqref="A631"/>
+      <pane ySplit="3" topLeftCell="A613" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A635" sqref="A635"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28957,6 +28983,18 @@
       <c r="B591" s="4">
         <v>7.7002499999999996</v>
       </c>
+      <c r="E591" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="F591" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="G591" s="4">
+        <v>16.78</v>
+      </c>
+      <c r="H591" s="4">
+        <v>11.56</v>
+      </c>
     </row>
     <row r="592" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A592" s="8">
@@ -28965,104 +29003,152 @@
       <c r="B592" s="4">
         <v>7.6997200000000001</v>
       </c>
-    </row>
-    <row r="593" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H592" s="4">
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="593" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A593" s="8">
         <v>44055</v>
       </c>
       <c r="B593" s="4">
         <v>7.70296</v>
       </c>
-    </row>
-    <row r="594" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H593" s="4">
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="594" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A594" s="8">
         <v>44056</v>
       </c>
       <c r="B594" s="4">
         <v>7.7010500000000004</v>
       </c>
-    </row>
-    <row r="595" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H594" s="4">
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="595" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A595" s="8">
         <v>44057</v>
       </c>
       <c r="B595" s="27">
         <v>7.7010500000000004</v>
       </c>
-    </row>
-    <row r="596" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H595" s="4">
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="596" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A596" s="8">
         <v>44058</v>
       </c>
       <c r="B596" s="27">
         <v>7.7010500000000004</v>
       </c>
-    </row>
-    <row r="597" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H596" s="4">
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="597" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A597" s="8">
         <v>44059</v>
       </c>
       <c r="B597" s="27">
         <v>7.7010500000000004</v>
       </c>
-    </row>
-    <row r="598" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H597" s="4">
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="598" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A598" s="8">
         <v>44060</v>
       </c>
       <c r="B598" s="4">
         <v>7.70024</v>
       </c>
-    </row>
-    <row r="599" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E598" s="4">
+        <v>20.98</v>
+      </c>
+      <c r="F598" s="4">
+        <v>20.18</v>
+      </c>
+      <c r="G598" s="4">
+        <v>16.59</v>
+      </c>
+      <c r="H598" s="4">
+        <v>11.88</v>
+      </c>
+    </row>
+    <row r="599" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A599" s="8">
         <v>44061</v>
       </c>
       <c r="B599" s="4">
         <v>7.6964800000000002</v>
       </c>
-    </row>
-    <row r="600" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H599" s="4">
+        <v>11.88</v>
+      </c>
+    </row>
+    <row r="600" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A600" s="8">
         <v>44062</v>
       </c>
       <c r="B600" s="4">
         <v>7.6989400000000003</v>
       </c>
-    </row>
-    <row r="601" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H600" s="4">
+        <v>11.88</v>
+      </c>
+    </row>
+    <row r="601" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A601" s="8">
         <v>44063</v>
       </c>
       <c r="B601" s="4">
         <v>7.69998</v>
       </c>
-    </row>
-    <row r="602" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H601" s="4">
+        <v>11.88</v>
+      </c>
+    </row>
+    <row r="602" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A602" s="8">
         <v>44064</v>
       </c>
       <c r="B602" s="4">
         <v>7.7013199999999999</v>
       </c>
-    </row>
-    <row r="603" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H602" s="4">
+        <v>11.88</v>
+      </c>
+    </row>
+    <row r="603" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A603" s="8">
         <v>44065</v>
       </c>
       <c r="B603" s="4">
         <v>7.7013199999999999</v>
       </c>
-    </row>
-    <row r="604" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H603" s="4">
+        <v>11.88</v>
+      </c>
+    </row>
+    <row r="604" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A604" s="8">
         <v>44066</v>
       </c>
       <c r="B604" s="27">
         <v>7.7013199999999999</v>
       </c>
-    </row>
-    <row r="605" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H604" s="4">
+        <v>11.88</v>
+      </c>
+    </row>
+    <row r="605" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A605" s="8">
         <v>44067</v>
       </c>
@@ -29078,56 +29164,77 @@
       <c r="G605" s="4">
         <v>16.59</v>
       </c>
-    </row>
-    <row r="606" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H605" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="606" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A606" s="8">
         <v>44068</v>
       </c>
       <c r="B606" s="4">
         <v>7.6982299999999997</v>
       </c>
-    </row>
-    <row r="607" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H606" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="607" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A607" s="8">
         <v>44069</v>
       </c>
       <c r="B607" s="4">
         <v>7.7026199999999996</v>
       </c>
-    </row>
-    <row r="608" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H607" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="608" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A608" s="8">
         <v>44070</v>
       </c>
       <c r="B608" s="4">
         <v>7.7102899999999996</v>
       </c>
-    </row>
-    <row r="609" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H608" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="609" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A609" s="8">
         <v>44071</v>
       </c>
       <c r="B609" s="4">
         <v>7.7250800000000002</v>
       </c>
-    </row>
-    <row r="610" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H609" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="610" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A610" s="8">
         <v>44072</v>
       </c>
       <c r="B610" s="27">
         <v>7.7250800000000002</v>
       </c>
-    </row>
-    <row r="611" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H610" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="611" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A611" s="8">
         <v>44073</v>
       </c>
       <c r="B611" s="27">
         <v>7.7250800000000002</v>
       </c>
-    </row>
-    <row r="612" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H611" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="612" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A612" s="8">
         <v>44074</v>
       </c>
@@ -29143,66 +29250,105 @@
       <c r="G612" s="4">
         <v>16.420000000000002</v>
       </c>
-    </row>
-    <row r="613" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H612" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="613" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A613" s="8">
         <v>44075</v>
       </c>
       <c r="B613" s="27">
         <v>7.7296100000000001</v>
       </c>
-    </row>
-    <row r="614" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H613" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="614" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A614" s="8">
         <v>44076</v>
       </c>
-    </row>
-    <row r="615" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B614" s="4">
+        <v>7.7267200000000003</v>
+      </c>
+      <c r="H614" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="615" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A615" s="8">
         <v>44077</v>
       </c>
-    </row>
-    <row r="616" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B615" s="4">
+        <v>7.7293799999999999</v>
+      </c>
+      <c r="H615" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="616" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A616" s="8">
         <v>44078</v>
       </c>
-    </row>
-    <row r="617" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B616" s="4">
+        <v>7.7348999999999997</v>
+      </c>
+      <c r="H616" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="617" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A617" s="8">
         <v>44079</v>
       </c>
-    </row>
-    <row r="618" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B617" s="27">
+        <v>7.7348999999999997</v>
+      </c>
+      <c r="H617" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="618" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A618" s="8">
         <v>44080</v>
       </c>
-    </row>
-    <row r="619" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B618" s="27">
+        <v>7.7348999999999997</v>
+      </c>
+      <c r="H618" s="4">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="619" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A619" s="8">
         <v>44081</v>
       </c>
-    </row>
-    <row r="620" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B619" s="4">
+        <v>7.7318199999999999</v>
+      </c>
+    </row>
+    <row r="620" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A620" s="8">
         <v>44082</v>
       </c>
     </row>
-    <row r="621" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="621" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A621" s="8">
         <v>44083</v>
       </c>
     </row>
-    <row r="622" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="622" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A622" s="8">
         <v>44084</v>
       </c>
     </row>
-    <row r="623" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="623" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A623" s="8">
         <v>44085</v>
       </c>
     </row>
-    <row r="624" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="624" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A624" s="8">
         <v>44086</v>
       </c>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-08-2020 23-57-10
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1189" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BAB924BD-2A6A-4A4E-8FD5-637A8619EC18}"/>
+  <xr:revisionPtr revIDLastSave="1200" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{593AEF57-806A-47B3-B2DF-7879F66E4CD8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1972,9 +1972,9 @@
   </sheetPr>
   <dimension ref="A1:R625"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R53" sqref="R53"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A612" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B629" sqref="B629"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13838,7 +13838,7 @@
         <v>129.80000000000001</v>
       </c>
       <c r="D612" s="22">
-        <v>12.65</v>
+        <v>12.66</v>
       </c>
       <c r="E612" s="22"/>
       <c r="F612" s="22"/>
@@ -13856,7 +13856,7 @@
         <v>131.9</v>
       </c>
       <c r="D613" s="22">
-        <v>12.66</v>
+        <v>12.6</v>
       </c>
       <c r="E613" s="22"/>
       <c r="F613" s="22"/>
@@ -13874,7 +13874,7 @@
         <v>131.5</v>
       </c>
       <c r="D614" s="22">
-        <v>12.6</v>
+        <v>12.44</v>
       </c>
       <c r="E614" s="22"/>
       <c r="F614" s="22"/>
@@ -13892,7 +13892,7 @@
         <v>131.6</v>
       </c>
       <c r="D615" s="22">
-        <v>12.41</v>
+        <v>12.07</v>
       </c>
       <c r="E615" s="22"/>
       <c r="F615" s="22"/>
@@ -13907,10 +13907,10 @@
         <v>24.502500000000001</v>
       </c>
       <c r="C616" s="22">
-        <v>134.69999999999999</v>
+        <v>134.80000000000001</v>
       </c>
       <c r="D616" s="22">
-        <v>12.09</v>
+        <v>11.93</v>
       </c>
       <c r="E616" s="22"/>
       <c r="F616" s="22"/>
@@ -13967,9 +13967,15 @@
       <c r="A620" s="8">
         <v>44082</v>
       </c>
-      <c r="B620" s="28"/>
-      <c r="C620" s="22"/>
-      <c r="D620" s="22"/>
+      <c r="B620" s="28">
+        <v>24.5</v>
+      </c>
+      <c r="C620" s="22">
+        <v>131.58000000000001</v>
+      </c>
+      <c r="D620" s="22">
+        <v>12.07</v>
+      </c>
       <c r="E620" s="22"/>
       <c r="F620" s="22"/>
       <c r="G620" s="22"/>
@@ -13979,7 +13985,9 @@
       <c r="A621" s="8">
         <v>44083</v>
       </c>
-      <c r="B621" s="28"/>
+      <c r="B621" s="28">
+        <v>24.496400000000001</v>
+      </c>
       <c r="C621" s="22"/>
       <c r="D621" s="22"/>
       <c r="E621" s="22"/>
@@ -14057,8 +14065,8 @@
   <dimension ref="A1:R625"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A613" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A635" sqref="A635"/>
+      <pane ySplit="3" topLeftCell="A614" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A627" sqref="A627"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29332,10 +29340,16 @@
       <c r="A620" s="8">
         <v>44082</v>
       </c>
+      <c r="B620" s="4">
+        <v>7.7393200000000002</v>
+      </c>
     </row>
     <row r="621" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A621" s="8">
         <v>44083</v>
+      </c>
+      <c r="B621" s="4">
+        <v>7.7413100000000004</v>
       </c>
     </row>
     <row r="622" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-18-2020 00-47-00
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1241" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{11DCD94C-A7A9-40B4-80C3-A3A3E3CFCC50}"/>
+  <xr:revisionPtr revIDLastSave="1256" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E3EEC834-9E8F-4E90-AA29-4FF335816F0D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1973,8 +1973,8 @@
   <dimension ref="A1:R639"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A627" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A643" sqref="A643"/>
+      <pane ySplit="3" topLeftCell="A630" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A646" sqref="A646"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14081,14 +14081,12 @@
       <c r="A627" s="8">
         <v>44089</v>
       </c>
-      <c r="B627" s="28">
-        <v>24.482299999999999</v>
-      </c>
+      <c r="B627" s="28"/>
       <c r="C627" s="22">
-        <v>121.65</v>
+        <v>122.2</v>
       </c>
       <c r="D627" s="22">
-        <v>12.09</v>
+        <v>12.08</v>
       </c>
       <c r="E627" s="22"/>
       <c r="F627" s="22"/>
@@ -14099,9 +14097,15 @@
       <c r="A628" s="8">
         <v>44090</v>
       </c>
-      <c r="B628" s="28"/>
-      <c r="C628" s="22"/>
-      <c r="D628" s="22"/>
+      <c r="B628" s="28">
+        <v>24.482299999999999</v>
+      </c>
+      <c r="C628" s="22">
+        <v>120.55</v>
+      </c>
+      <c r="D628" s="22">
+        <v>12.35</v>
+      </c>
       <c r="E628" s="22"/>
       <c r="F628" s="22"/>
       <c r="G628" s="22"/>
@@ -14111,9 +14115,15 @@
       <c r="A629" s="8">
         <v>44091</v>
       </c>
-      <c r="B629" s="28"/>
-      <c r="C629" s="22"/>
-      <c r="D629" s="22"/>
+      <c r="B629" s="28">
+        <v>24.476400000000002</v>
+      </c>
+      <c r="C629" s="22">
+        <v>118.1</v>
+      </c>
+      <c r="D629" s="22">
+        <v>12.55</v>
+      </c>
       <c r="E629" s="22"/>
       <c r="F629" s="22"/>
       <c r="G629" s="22"/>
@@ -14123,7 +14133,9 @@
       <c r="A630" s="8">
         <v>44092</v>
       </c>
-      <c r="B630" s="28"/>
+      <c r="B630" s="28">
+        <v>24.475899999999999</v>
+      </c>
       <c r="C630" s="22"/>
       <c r="D630" s="22"/>
       <c r="E630" s="22"/>
@@ -14261,8 +14273,8 @@
   <dimension ref="A1:R639"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A635" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A646" sqref="A646"/>
+      <pane ySplit="3" topLeftCell="A633" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A644" sqref="A644"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29642,20 +29654,32 @@
       <c r="A629" s="8">
         <v>44091</v>
       </c>
+      <c r="B629" s="4">
+        <v>7.7565</v>
+      </c>
     </row>
     <row r="630" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A630" s="8">
         <v>44092</v>
       </c>
+      <c r="B630" s="4">
+        <v>7.7568700000000002</v>
+      </c>
     </row>
     <row r="631" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A631" s="8">
         <v>44093</v>
       </c>
+      <c r="B631" s="27">
+        <v>7.7568700000000002</v>
+      </c>
     </row>
     <row r="632" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A632" s="8">
         <v>44094</v>
+      </c>
+      <c r="B632" s="27">
+        <v>7.7568700000000002</v>
       </c>
     </row>
     <row r="633" spans="1:8" x14ac:dyDescent="0.25">
@@ -29708,7 +29732,7 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F27" sqref="F27"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-23-2020 01-05-39
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1256" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E3EEC834-9E8F-4E90-AA29-4FF335816F0D}"/>
+  <xr:revisionPtr revIDLastSave="1275" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{26AD4DE4-CAF1-4241-9A07-A6AE397ADDEC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1601,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H639" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H639" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H646" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H646" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1970,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R639"/>
+  <dimension ref="A1:R646"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A630" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A646" sqref="A646"/>
+      <pane ySplit="3" topLeftCell="A640" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A653" sqref="A653"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,7 +3961,7 @@
       </c>
       <c r="Q45" s="27"/>
       <c r="R45" s="27">
-        <v>491.8</v>
+        <v>491.9</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -14054,10 +14054,18 @@
       <c r="B625" s="28"/>
       <c r="C625" s="22"/>
       <c r="D625" s="22"/>
-      <c r="E625" s="22"/>
-      <c r="F625" s="22"/>
-      <c r="G625" s="22"/>
-      <c r="H625" s="22"/>
+      <c r="E625" s="22">
+        <v>82.4</v>
+      </c>
+      <c r="F625" s="22">
+        <v>76</v>
+      </c>
+      <c r="G625" s="22">
+        <v>64.69</v>
+      </c>
+      <c r="H625" s="22">
+        <v>44.97</v>
+      </c>
     </row>
     <row r="626" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A626" s="8">
@@ -14162,10 +14170,18 @@
       <c r="B632" s="28"/>
       <c r="C632" s="22"/>
       <c r="D632" s="22"/>
-      <c r="E632" s="22"/>
-      <c r="F632" s="22"/>
-      <c r="G632" s="22"/>
-      <c r="H632" s="22"/>
+      <c r="E632" s="22">
+        <v>82.36</v>
+      </c>
+      <c r="F632" s="22">
+        <v>75.739999999999995</v>
+      </c>
+      <c r="G632" s="22">
+        <v>64.040000000000006</v>
+      </c>
+      <c r="H632" s="22">
+        <v>44.36</v>
+      </c>
     </row>
     <row r="633" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A633" s="8">
@@ -14246,10 +14262,102 @@
       <c r="B639" s="28"/>
       <c r="C639" s="22"/>
       <c r="D639" s="22"/>
-      <c r="E639" s="22"/>
-      <c r="F639" s="22"/>
-      <c r="G639" s="22"/>
-      <c r="H639" s="22"/>
+      <c r="E639" s="22">
+        <v>82.25</v>
+      </c>
+      <c r="F639" s="22">
+        <v>75.55</v>
+      </c>
+      <c r="G639" s="22">
+        <v>63.17</v>
+      </c>
+      <c r="H639" s="22">
+        <v>43.6</v>
+      </c>
+    </row>
+    <row r="640" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A640" s="8">
+        <v>44102</v>
+      </c>
+      <c r="B640" s="28"/>
+      <c r="C640" s="22"/>
+      <c r="D640" s="22"/>
+      <c r="E640" s="22"/>
+      <c r="F640" s="22"/>
+      <c r="G640" s="22"/>
+      <c r="H640" s="22"/>
+    </row>
+    <row r="641" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A641" s="8">
+        <v>44103</v>
+      </c>
+      <c r="B641" s="28"/>
+      <c r="C641" s="22"/>
+      <c r="D641" s="22"/>
+      <c r="E641" s="22"/>
+      <c r="F641" s="22"/>
+      <c r="G641" s="22"/>
+      <c r="H641" s="22"/>
+    </row>
+    <row r="642" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A642" s="8">
+        <v>44104</v>
+      </c>
+      <c r="B642" s="28"/>
+      <c r="C642" s="22"/>
+      <c r="D642" s="22"/>
+      <c r="E642" s="22"/>
+      <c r="F642" s="22"/>
+      <c r="G642" s="22"/>
+      <c r="H642" s="22"/>
+    </row>
+    <row r="643" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A643" s="8">
+        <v>44105</v>
+      </c>
+      <c r="B643" s="28"/>
+      <c r="C643" s="22"/>
+      <c r="D643" s="22"/>
+      <c r="E643" s="22"/>
+      <c r="F643" s="22"/>
+      <c r="G643" s="22"/>
+      <c r="H643" s="22"/>
+    </row>
+    <row r="644" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A644" s="8">
+        <v>44106</v>
+      </c>
+      <c r="B644" s="28"/>
+      <c r="C644" s="22"/>
+      <c r="D644" s="22"/>
+      <c r="E644" s="22"/>
+      <c r="F644" s="22"/>
+      <c r="G644" s="22"/>
+      <c r="H644" s="22"/>
+    </row>
+    <row r="645" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A645" s="8">
+        <v>44107</v>
+      </c>
+      <c r="B645" s="28"/>
+      <c r="C645" s="22"/>
+      <c r="D645" s="22"/>
+      <c r="E645" s="22"/>
+      <c r="F645" s="22"/>
+      <c r="G645" s="22"/>
+      <c r="H645" s="22"/>
+    </row>
+    <row r="646" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A646" s="8">
+        <v>44108</v>
+      </c>
+      <c r="B646" s="28"/>
+      <c r="C646" s="22"/>
+      <c r="D646" s="22"/>
+      <c r="E646" s="22"/>
+      <c r="F646" s="22"/>
+      <c r="G646" s="22"/>
+      <c r="H646" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -14274,7 +14382,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A633" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A644" sqref="A644"/>
+      <selection pane="bottomLeft" activeCell="B644" sqref="B644"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-26-2020 01-17-54
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1275" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{26AD4DE4-CAF1-4241-9A07-A6AE397ADDEC}"/>
+  <xr:revisionPtr revIDLastSave="1309" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{399B3D4B-1C75-435A-B700-F8B393EC6EB7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1638,8 +1638,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H639" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H639" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H646" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H646" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1973,7 +1973,7 @@
   <dimension ref="A1:R646"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A640" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A637" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A653" sqref="A653"/>
     </sheetView>
   </sheetViews>
@@ -14130,7 +14130,7 @@
         <v>118.1</v>
       </c>
       <c r="D629" s="22">
-        <v>12.55</v>
+        <v>12.62</v>
       </c>
       <c r="E629" s="22"/>
       <c r="F629" s="22"/>
@@ -14144,8 +14144,12 @@
       <c r="B630" s="28">
         <v>24.475899999999999</v>
       </c>
-      <c r="C630" s="22"/>
-      <c r="D630" s="22"/>
+      <c r="C630" s="22">
+        <v>113.6</v>
+      </c>
+      <c r="D630" s="22">
+        <v>12.77</v>
+      </c>
       <c r="E630" s="22"/>
       <c r="F630" s="22"/>
       <c r="G630" s="22"/>
@@ -14187,9 +14191,15 @@
       <c r="A633" s="8">
         <v>44095</v>
       </c>
-      <c r="B633" s="28"/>
-      <c r="C633" s="22"/>
-      <c r="D633" s="22"/>
+      <c r="B633" s="28">
+        <v>24.4758</v>
+      </c>
+      <c r="C633" s="22">
+        <v>112</v>
+      </c>
+      <c r="D633" s="22">
+        <v>12.55</v>
+      </c>
       <c r="E633" s="22"/>
       <c r="F633" s="22"/>
       <c r="G633" s="22"/>
@@ -14199,9 +14209,15 @@
       <c r="A634" s="8">
         <v>44096</v>
       </c>
-      <c r="B634" s="28"/>
-      <c r="C634" s="22"/>
-      <c r="D634" s="22"/>
+      <c r="B634" s="28">
+        <v>24.4757</v>
+      </c>
+      <c r="C634" s="22">
+        <v>110.65</v>
+      </c>
+      <c r="D634" s="22">
+        <v>12.89</v>
+      </c>
       <c r="E634" s="22"/>
       <c r="F634" s="22"/>
       <c r="G634" s="22"/>
@@ -14211,9 +14227,15 @@
       <c r="A635" s="8">
         <v>44097</v>
       </c>
-      <c r="B635" s="28"/>
-      <c r="C635" s="22"/>
-      <c r="D635" s="22"/>
+      <c r="B635" s="28">
+        <v>24.472200000000001</v>
+      </c>
+      <c r="C635" s="22">
+        <v>110.5</v>
+      </c>
+      <c r="D635" s="22">
+        <v>12.82</v>
+      </c>
       <c r="E635" s="22"/>
       <c r="F635" s="22"/>
       <c r="G635" s="22"/>
@@ -14223,9 +14245,15 @@
       <c r="A636" s="8">
         <v>44098</v>
       </c>
-      <c r="B636" s="28"/>
-      <c r="C636" s="22"/>
-      <c r="D636" s="22"/>
+      <c r="B636" s="28">
+        <v>24.468399999999999</v>
+      </c>
+      <c r="C636" s="22">
+        <v>111.15</v>
+      </c>
+      <c r="D636" s="22">
+        <v>12.84</v>
+      </c>
       <c r="E636" s="22"/>
       <c r="F636" s="22"/>
       <c r="G636" s="22"/>
@@ -14235,9 +14263,15 @@
       <c r="A637" s="8">
         <v>44099</v>
       </c>
-      <c r="B637" s="28"/>
-      <c r="C637" s="22"/>
-      <c r="D637" s="22"/>
+      <c r="B637" s="28">
+        <v>24.464099999999998</v>
+      </c>
+      <c r="C637" s="22">
+        <v>114.25</v>
+      </c>
+      <c r="D637" s="22">
+        <v>13.03</v>
+      </c>
       <c r="E637" s="22"/>
       <c r="F637" s="22"/>
       <c r="G637" s="22"/>
@@ -14279,7 +14313,9 @@
       <c r="A640" s="8">
         <v>44102</v>
       </c>
-      <c r="B640" s="28"/>
+      <c r="B640" s="28">
+        <v>24.459199999999999</v>
+      </c>
       <c r="C640" s="22"/>
       <c r="D640" s="22"/>
       <c r="E640" s="22"/>
@@ -14378,11 +14414,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R639"/>
+  <dimension ref="A1:R646"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A633" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B644" sqref="B644"/>
+      <pane ySplit="3" topLeftCell="A640" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A651" sqref="A651"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29741,6 +29777,18 @@
       <c r="B626" s="4">
         <v>7.7592699999999999</v>
       </c>
+      <c r="E626" s="4">
+        <v>21.02</v>
+      </c>
+      <c r="F626" s="4">
+        <v>20.21</v>
+      </c>
+      <c r="G626" s="4">
+        <v>15.55</v>
+      </c>
+      <c r="H626" s="4">
+        <v>11.45</v>
+      </c>
     </row>
     <row r="627" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A627" s="8">
@@ -29749,6 +29797,9 @@
       <c r="B627" s="27">
         <v>7.7592699999999999</v>
       </c>
+      <c r="H627" s="4">
+        <v>11.45</v>
+      </c>
     </row>
     <row r="628" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A628" s="8">
@@ -29757,6 +29808,9 @@
       <c r="B628" s="4">
         <v>7.7530299999999999</v>
       </c>
+      <c r="H628" s="4">
+        <v>11.45</v>
+      </c>
     </row>
     <row r="629" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A629" s="8">
@@ -29765,6 +29819,9 @@
       <c r="B629" s="4">
         <v>7.7565</v>
       </c>
+      <c r="H629" s="4">
+        <v>11.45</v>
+      </c>
     </row>
     <row r="630" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A630" s="8">
@@ -29773,6 +29830,9 @@
       <c r="B630" s="4">
         <v>7.7568700000000002</v>
       </c>
+      <c r="H630" s="4">
+        <v>11.45</v>
+      </c>
     </row>
     <row r="631" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A631" s="8">
@@ -29781,6 +29841,9 @@
       <c r="B631" s="27">
         <v>7.7568700000000002</v>
       </c>
+      <c r="H631" s="4">
+        <v>11.45</v>
+      </c>
     </row>
     <row r="632" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A632" s="8">
@@ -29789,40 +29852,132 @@
       <c r="B632" s="27">
         <v>7.7568700000000002</v>
       </c>
+      <c r="H632" s="4">
+        <v>11.45</v>
+      </c>
     </row>
     <row r="633" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A633" s="8">
         <v>44095</v>
       </c>
+      <c r="B633" s="4">
+        <v>7.7660999999999998</v>
+      </c>
+      <c r="E633" s="4">
+        <v>20.89</v>
+      </c>
+      <c r="F633" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="G633" s="4">
+        <v>15.06</v>
+      </c>
+      <c r="H633" s="4">
+        <v>11.6</v>
+      </c>
     </row>
     <row r="634" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A634" s="8">
         <v>44096</v>
       </c>
+      <c r="B634" s="4">
+        <v>7.7588800000000004</v>
+      </c>
+      <c r="H634" s="4">
+        <v>11.6</v>
+      </c>
     </row>
     <row r="635" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A635" s="8">
         <v>44097</v>
       </c>
+      <c r="B635" s="4">
+        <v>7.7667700000000002</v>
+      </c>
+      <c r="H635" s="4">
+        <v>11.6</v>
+      </c>
     </row>
     <row r="636" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A636" s="8">
         <v>44098</v>
       </c>
+      <c r="B636" s="4">
+        <v>7.7862999999999998</v>
+      </c>
+      <c r="H636" s="4">
+        <v>11.6</v>
+      </c>
     </row>
     <row r="637" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A637" s="8">
         <v>44099</v>
       </c>
+      <c r="B637" s="4">
+        <v>7.7845899999999997</v>
+      </c>
+      <c r="H637" s="4">
+        <v>11.6</v>
+      </c>
     </row>
     <row r="638" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A638" s="8">
         <v>44100</v>
       </c>
+      <c r="B638" s="4">
+        <v>7.7845899999999997</v>
+      </c>
+      <c r="H638" s="4">
+        <v>11.6</v>
+      </c>
     </row>
     <row r="639" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A639" s="8">
         <v>44101</v>
+      </c>
+      <c r="B639" s="4">
+        <v>7.7845899999999997</v>
+      </c>
+      <c r="H639" s="4">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="640" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A640" s="8">
+        <v>44102</v>
+      </c>
+      <c r="B640" s="4">
+        <v>7.7823000000000002</v>
+      </c>
+    </row>
+    <row r="641" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A641" s="8">
+        <v>44103</v>
+      </c>
+    </row>
+    <row r="642" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A642" s="8">
+        <v>44104</v>
+      </c>
+    </row>
+    <row r="643" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A643" s="8">
+        <v>44105</v>
+      </c>
+    </row>
+    <row r="644" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A644" s="8">
+        <v>44106</v>
+      </c>
+    </row>
+    <row r="645" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A645" s="8">
+        <v>44107</v>
+      </c>
+    </row>
+    <row r="646" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A646" s="8">
+        <v>44108</v>
       </c>
     </row>
   </sheetData>
@@ -29840,7 +29995,7 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F27" sqref="F27"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-30-2020 01-35-30
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1309" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{399B3D4B-1C75-435A-B700-F8B393EC6EB7}"/>
+  <xr:revisionPtr revIDLastSave="1338" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EC0F0055-98F2-4EB2-866C-9E5AE8F2CCF4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1601,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H646" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H646" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H653" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H653" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1638,8 +1638,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H646" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H646" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H653" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H653" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1970,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R646"/>
+  <dimension ref="A1:R653"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A637" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A653" sqref="A653"/>
+      <pane ySplit="3" topLeftCell="A641" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A655" sqref="A655"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14267,10 +14267,10 @@
         <v>24.464099999999998</v>
       </c>
       <c r="C637" s="22">
-        <v>114.25</v>
+        <v>113.65</v>
       </c>
       <c r="D637" s="22">
-        <v>13.03</v>
+        <v>13</v>
       </c>
       <c r="E637" s="22"/>
       <c r="F637" s="22"/>
@@ -14316,8 +14316,12 @@
       <c r="B640" s="28">
         <v>24.459199999999999</v>
       </c>
-      <c r="C640" s="22"/>
-      <c r="D640" s="22"/>
+      <c r="C640" s="22">
+        <v>109.55</v>
+      </c>
+      <c r="D640" s="22">
+        <v>12.59</v>
+      </c>
       <c r="E640" s="22"/>
       <c r="F640" s="22"/>
       <c r="G640" s="22"/>
@@ -14327,9 +14331,15 @@
       <c r="A641" s="8">
         <v>44103</v>
       </c>
-      <c r="B641" s="28"/>
-      <c r="C641" s="22"/>
-      <c r="D641" s="22"/>
+      <c r="B641" s="28">
+        <v>24.454499999999999</v>
+      </c>
+      <c r="C641" s="22">
+        <v>109.58</v>
+      </c>
+      <c r="D641" s="22">
+        <v>13.43</v>
+      </c>
       <c r="E641" s="22"/>
       <c r="F641" s="22"/>
       <c r="G641" s="22"/>
@@ -14339,7 +14349,9 @@
       <c r="A642" s="8">
         <v>44104</v>
       </c>
-      <c r="B642" s="28"/>
+      <c r="B642" s="28">
+        <v>24.4482</v>
+      </c>
       <c r="C642" s="22"/>
       <c r="D642" s="22"/>
       <c r="E642" s="22"/>
@@ -14390,10 +14402,102 @@
       <c r="B646" s="28"/>
       <c r="C646" s="22"/>
       <c r="D646" s="22"/>
-      <c r="E646" s="22"/>
-      <c r="F646" s="22"/>
-      <c r="G646" s="22"/>
-      <c r="H646" s="22"/>
+      <c r="E646" s="22">
+        <v>81.98</v>
+      </c>
+      <c r="F646" s="22">
+        <v>75.09</v>
+      </c>
+      <c r="G646" s="22">
+        <v>62.34</v>
+      </c>
+      <c r="H646" s="22">
+        <v>42.73</v>
+      </c>
+    </row>
+    <row r="647" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A647" s="8">
+        <v>44109</v>
+      </c>
+      <c r="B647" s="28"/>
+      <c r="C647" s="22"/>
+      <c r="D647" s="22"/>
+      <c r="E647" s="22"/>
+      <c r="F647" s="22"/>
+      <c r="G647" s="22"/>
+      <c r="H647" s="22"/>
+    </row>
+    <row r="648" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A648" s="8">
+        <v>44110</v>
+      </c>
+      <c r="B648" s="28"/>
+      <c r="C648" s="22"/>
+      <c r="D648" s="22"/>
+      <c r="E648" s="22"/>
+      <c r="F648" s="22"/>
+      <c r="G648" s="22"/>
+      <c r="H648" s="22"/>
+    </row>
+    <row r="649" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A649" s="8">
+        <v>44111</v>
+      </c>
+      <c r="B649" s="28"/>
+      <c r="C649" s="22"/>
+      <c r="D649" s="22"/>
+      <c r="E649" s="22"/>
+      <c r="F649" s="22"/>
+      <c r="G649" s="22"/>
+      <c r="H649" s="22"/>
+    </row>
+    <row r="650" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A650" s="8">
+        <v>44112</v>
+      </c>
+      <c r="B650" s="28"/>
+      <c r="C650" s="22"/>
+      <c r="D650" s="22"/>
+      <c r="E650" s="22"/>
+      <c r="F650" s="22"/>
+      <c r="G650" s="22"/>
+      <c r="H650" s="22"/>
+    </row>
+    <row r="651" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A651" s="8">
+        <v>44113</v>
+      </c>
+      <c r="B651" s="28"/>
+      <c r="C651" s="22"/>
+      <c r="D651" s="22"/>
+      <c r="E651" s="22"/>
+      <c r="F651" s="22"/>
+      <c r="G651" s="22"/>
+      <c r="H651" s="22"/>
+    </row>
+    <row r="652" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A652" s="8">
+        <v>44114</v>
+      </c>
+      <c r="B652" s="28"/>
+      <c r="C652" s="22"/>
+      <c r="D652" s="22"/>
+      <c r="E652" s="22"/>
+      <c r="F652" s="22"/>
+      <c r="G652" s="22"/>
+      <c r="H652" s="22"/>
+    </row>
+    <row r="653" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A653" s="8">
+        <v>44115</v>
+      </c>
+      <c r="B653" s="28"/>
+      <c r="C653" s="22"/>
+      <c r="D653" s="22"/>
+      <c r="E653" s="22"/>
+      <c r="F653" s="22"/>
+      <c r="G653" s="22"/>
+      <c r="H653" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -14414,11 +14518,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R646"/>
+  <dimension ref="A1:R653"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A640" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A651" sqref="A651"/>
+      <pane ySplit="3" topLeftCell="A635" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E657" sqref="E657"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29949,35 +30053,89 @@
       <c r="B640" s="4">
         <v>7.7823000000000002</v>
       </c>
-    </row>
-    <row r="641" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E640" s="4">
+        <v>20.87</v>
+      </c>
+      <c r="F640" s="4">
+        <v>20.09</v>
+      </c>
+      <c r="G640" s="4">
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A641" s="8">
         <v>44103</v>
       </c>
-    </row>
-    <row r="642" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B641" s="27">
+        <v>7.7854299999999999</v>
+      </c>
+    </row>
+    <row r="642" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A642" s="8">
         <v>44104</v>
       </c>
-    </row>
-    <row r="643" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B642" s="27">
+        <v>7.7860199999999997</v>
+      </c>
+    </row>
+    <row r="643" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A643" s="8">
         <v>44105</v>
       </c>
-    </row>
-    <row r="644" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B643" s="27"/>
+    </row>
+    <row r="644" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A644" s="8">
         <v>44106</v>
       </c>
-    </row>
-    <row r="645" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B644" s="27"/>
+    </row>
+    <row r="645" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A645" s="8">
         <v>44107</v>
       </c>
-    </row>
-    <row r="646" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B645" s="27"/>
+    </row>
+    <row r="646" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A646" s="8">
         <v>44108</v>
+      </c>
+      <c r="B646" s="27"/>
+    </row>
+    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A647" s="8">
+        <v>44109</v>
+      </c>
+    </row>
+    <row r="648" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A648" s="8">
+        <v>44110</v>
+      </c>
+    </row>
+    <row r="649" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A649" s="8">
+        <v>44111</v>
+      </c>
+    </row>
+    <row r="650" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A650" s="8">
+        <v>44112</v>
+      </c>
+    </row>
+    <row r="651" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A651" s="8">
+        <v>44113</v>
+      </c>
+    </row>
+    <row r="652" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A652" s="8">
+        <v>44114</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A653" s="8">
+        <v>44115</v>
       </c>
     </row>
   </sheetData>
@@ -29995,10 +30153,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-03-2020 01-47-01
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1338" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EC0F0055-98F2-4EB2-866C-9E5AE8F2CCF4}"/>
+  <xr:revisionPtr revIDLastSave="1357" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B5D4970E-105D-4209-9495-BDB9B312C381}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1973,8 +1973,8 @@
   <dimension ref="A1:R653"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A641" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A655" sqref="A655"/>
+      <pane ySplit="3" topLeftCell="A646" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A662" sqref="A662"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14335,10 +14335,10 @@
         <v>24.454499999999999</v>
       </c>
       <c r="C641" s="22">
-        <v>109.58</v>
+        <v>109.55</v>
       </c>
       <c r="D641" s="22">
-        <v>13.43</v>
+        <v>12.99</v>
       </c>
       <c r="E641" s="22"/>
       <c r="F641" s="22"/>
@@ -14352,8 +14352,12 @@
       <c r="B642" s="28">
         <v>24.4482</v>
       </c>
-      <c r="C642" s="22"/>
-      <c r="D642" s="22"/>
+      <c r="C642" s="22">
+        <v>110.95</v>
+      </c>
+      <c r="D642" s="22">
+        <v>13.07</v>
+      </c>
       <c r="E642" s="22"/>
       <c r="F642" s="22"/>
       <c r="G642" s="22"/>
@@ -14363,9 +14367,15 @@
       <c r="A643" s="8">
         <v>44105</v>
       </c>
-      <c r="B643" s="28"/>
-      <c r="C643" s="22"/>
-      <c r="D643" s="22"/>
+      <c r="B643" s="28">
+        <v>24.4438</v>
+      </c>
+      <c r="C643" s="22">
+        <v>107.05</v>
+      </c>
+      <c r="D643" s="22">
+        <v>13.58</v>
+      </c>
       <c r="E643" s="22"/>
       <c r="F643" s="22"/>
       <c r="G643" s="22"/>
@@ -14375,9 +14385,15 @@
       <c r="A644" s="8">
         <v>44106</v>
       </c>
-      <c r="B644" s="28"/>
-      <c r="C644" s="22"/>
-      <c r="D644" s="22"/>
+      <c r="B644" s="28">
+        <v>24.441500000000001</v>
+      </c>
+      <c r="C644" s="22">
+        <v>109.45</v>
+      </c>
+      <c r="D644" s="22">
+        <v>13.57</v>
+      </c>
       <c r="E644" s="22"/>
       <c r="F644" s="22"/>
       <c r="G644" s="22"/>
@@ -14419,7 +14435,9 @@
       <c r="A647" s="8">
         <v>44109</v>
       </c>
-      <c r="B647" s="28"/>
+      <c r="B647" s="28">
+        <v>24.44</v>
+      </c>
       <c r="C647" s="22"/>
       <c r="D647" s="22"/>
       <c r="E647" s="22"/>
@@ -14521,8 +14539,8 @@
   <dimension ref="A1:R653"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A635" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E657" sqref="E657"/>
+      <pane ySplit="3" topLeftCell="A648" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A659" sqref="A659"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30062,78 +30080,110 @@
       <c r="G640" s="4">
         <v>14.99</v>
       </c>
-    </row>
-    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H640" s="4">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="641" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A641" s="8">
         <v>44103</v>
       </c>
       <c r="B641" s="27">
         <v>7.7854299999999999</v>
       </c>
-    </row>
-    <row r="642" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H641" s="4">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="642" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A642" s="8">
         <v>44104</v>
       </c>
       <c r="B642" s="27">
         <v>7.7860199999999997</v>
       </c>
-    </row>
-    <row r="643" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H642" s="4">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="643" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A643" s="8">
         <v>44105</v>
       </c>
-      <c r="B643" s="27"/>
-    </row>
-    <row r="644" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B643" s="27">
+        <v>7.7837500000000004</v>
+      </c>
+      <c r="H643" s="4">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="644" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A644" s="8">
         <v>44106</v>
       </c>
-      <c r="B644" s="27"/>
-    </row>
-    <row r="645" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B644" s="27">
+        <v>7.7822199999999997</v>
+      </c>
+      <c r="H644" s="4">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="645" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A645" s="8">
         <v>44107</v>
       </c>
-      <c r="B645" s="27"/>
-    </row>
-    <row r="646" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B645" s="27">
+        <v>7.7822199999999997</v>
+      </c>
+      <c r="H645" s="4">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="646" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A646" s="8">
         <v>44108</v>
       </c>
-      <c r="B646" s="27"/>
-    </row>
-    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B646" s="27">
+        <v>7.7822199999999997</v>
+      </c>
+      <c r="H646" s="4">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="647" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A647" s="8">
         <v>44109</v>
       </c>
-    </row>
-    <row r="648" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B647" s="4">
+        <v>7.7771800000000004</v>
+      </c>
+    </row>
+    <row r="648" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A648" s="8">
         <v>44110</v>
       </c>
     </row>
-    <row r="649" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A649" s="8">
         <v>44111</v>
       </c>
     </row>
-    <row r="650" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A650" s="8">
         <v>44112</v>
       </c>
     </row>
-    <row r="651" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="651" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A651" s="8">
         <v>44113</v>
       </c>
     </row>
-    <row r="652" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A652" s="8">
         <v>44114</v>
       </c>
     </row>
-    <row r="653" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A653" s="8">
         <v>44115</v>
       </c>
@@ -30153,10 +30203,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-06-2020 23-01-30
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1357" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B5D4970E-105D-4209-9495-BDB9B312C381}"/>
+  <xr:revisionPtr revIDLastSave="1393" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B92E8B83-3BA4-4EDD-A2C3-53064D2D596F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1601,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H653" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H653" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H660" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H660" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1638,8 +1638,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H653" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H653" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H660" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H660" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1970,11 +1970,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R653"/>
+  <dimension ref="A1:R661"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A646" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A662" sqref="A662"/>
+      <pane ySplit="3" topLeftCell="A647" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A668" sqref="A668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="Q46" s="27"/>
       <c r="R46" s="27">
-        <v>515.79999999999995</v>
+        <v>516.6</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -4050,7 +4050,9 @@
         <v>3900</v>
       </c>
       <c r="Q47" s="27"/>
-      <c r="R47" s="27"/>
+      <c r="R47" s="27">
+        <v>519.4</v>
+      </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
@@ -14389,10 +14391,10 @@
         <v>24.441500000000001</v>
       </c>
       <c r="C644" s="22">
-        <v>109.45</v>
+        <v>108.95</v>
       </c>
       <c r="D644" s="22">
-        <v>13.57</v>
+        <v>13.55</v>
       </c>
       <c r="E644" s="22"/>
       <c r="F644" s="22"/>
@@ -14438,8 +14440,12 @@
       <c r="B647" s="28">
         <v>24.44</v>
       </c>
-      <c r="C647" s="22"/>
-      <c r="D647" s="22"/>
+      <c r="C647" s="22">
+        <v>107.2</v>
+      </c>
+      <c r="D647" s="22">
+        <v>13.61</v>
+      </c>
       <c r="E647" s="22"/>
       <c r="F647" s="22"/>
       <c r="G647" s="22"/>
@@ -14449,9 +14455,15 @@
       <c r="A648" s="8">
         <v>44110</v>
       </c>
-      <c r="B648" s="28"/>
-      <c r="C648" s="22"/>
-      <c r="D648" s="22"/>
+      <c r="B648" s="28">
+        <v>24.4373</v>
+      </c>
+      <c r="C648" s="22">
+        <v>107.73</v>
+      </c>
+      <c r="D648" s="22">
+        <v>13.86</v>
+      </c>
       <c r="E648" s="22"/>
       <c r="F648" s="22"/>
       <c r="G648" s="22"/>
@@ -14461,7 +14473,9 @@
       <c r="A649" s="8">
         <v>44111</v>
       </c>
-      <c r="B649" s="28"/>
+      <c r="B649" s="28">
+        <v>24.43</v>
+      </c>
       <c r="C649" s="22"/>
       <c r="D649" s="22"/>
       <c r="E649" s="22"/>
@@ -14512,10 +14526,112 @@
       <c r="B653" s="28"/>
       <c r="C653" s="22"/>
       <c r="D653" s="22"/>
-      <c r="E653" s="22"/>
-      <c r="F653" s="22"/>
-      <c r="G653" s="22"/>
-      <c r="H653" s="22"/>
+      <c r="E653" s="22">
+        <v>81.64</v>
+      </c>
+      <c r="F653" s="22">
+        <v>74.75</v>
+      </c>
+      <c r="G653" s="22">
+        <v>61.54</v>
+      </c>
+      <c r="H653" s="22">
+        <v>41.98</v>
+      </c>
+    </row>
+    <row r="654" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A654" s="8">
+        <v>44116</v>
+      </c>
+      <c r="B654" s="28"/>
+      <c r="C654" s="22"/>
+      <c r="D654" s="22"/>
+      <c r="E654" s="22"/>
+      <c r="F654" s="22"/>
+      <c r="G654" s="22"/>
+      <c r="H654" s="22"/>
+    </row>
+    <row r="655" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A655" s="8">
+        <v>44117</v>
+      </c>
+      <c r="B655" s="28"/>
+      <c r="C655" s="22"/>
+      <c r="D655" s="22"/>
+      <c r="E655" s="22"/>
+      <c r="F655" s="22"/>
+      <c r="G655" s="22"/>
+      <c r="H655" s="22"/>
+    </row>
+    <row r="656" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A656" s="8">
+        <v>44118</v>
+      </c>
+      <c r="B656" s="28"/>
+      <c r="C656" s="22"/>
+      <c r="D656" s="22"/>
+      <c r="E656" s="22"/>
+      <c r="F656" s="22"/>
+      <c r="G656" s="22"/>
+      <c r="H656" s="22"/>
+    </row>
+    <row r="657" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A657" s="8">
+        <v>44119</v>
+      </c>
+      <c r="B657" s="28"/>
+      <c r="C657" s="22"/>
+      <c r="D657" s="22"/>
+      <c r="E657" s="22"/>
+      <c r="F657" s="22"/>
+      <c r="G657" s="22"/>
+      <c r="H657" s="22"/>
+    </row>
+    <row r="658" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A658" s="8">
+        <v>44120</v>
+      </c>
+      <c r="B658" s="28"/>
+      <c r="C658" s="22"/>
+      <c r="D658" s="22"/>
+      <c r="E658" s="22"/>
+      <c r="F658" s="22"/>
+      <c r="G658" s="22"/>
+      <c r="H658" s="22"/>
+    </row>
+    <row r="659" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A659" s="8">
+        <v>44121</v>
+      </c>
+      <c r="B659" s="28"/>
+      <c r="C659" s="22"/>
+      <c r="D659" s="22"/>
+      <c r="E659" s="22"/>
+      <c r="F659" s="22"/>
+      <c r="G659" s="22"/>
+      <c r="H659" s="22"/>
+    </row>
+    <row r="660" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A660" s="8">
+        <v>44122</v>
+      </c>
+      <c r="B660" s="28"/>
+      <c r="C660" s="22"/>
+      <c r="D660" s="22"/>
+      <c r="E660" s="22"/>
+      <c r="F660" s="22"/>
+      <c r="G660" s="22"/>
+      <c r="H660" s="22"/>
+    </row>
+    <row r="661" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A661" s="8"/>
+      <c r="B661" s="28"/>
+      <c r="C661" s="22"/>
+      <c r="D661" s="22"/>
+      <c r="E661" s="22"/>
+      <c r="F661" s="22"/>
+      <c r="G661" s="22"/>
+      <c r="H661" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -14536,11 +14652,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R653"/>
+  <dimension ref="A1:R661"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A648" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A659" sqref="A659"/>
+      <pane ySplit="3" topLeftCell="A653" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A667" sqref="A667"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16784,7 +16900,7 @@
       </c>
       <c r="Q46" s="27"/>
       <c r="R46" s="27">
-        <v>1076.7</v>
+        <v>1077.7</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -16832,7 +16948,9 @@
         <v>144.75</v>
       </c>
       <c r="Q47" s="27"/>
-      <c r="R47" s="27"/>
+      <c r="R47" s="27">
+        <v>1049</v>
+      </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
@@ -30157,36 +30275,120 @@
       <c r="B647" s="4">
         <v>7.7771800000000004</v>
       </c>
+      <c r="E647" s="4">
+        <v>21.41</v>
+      </c>
+      <c r="F647" s="4">
+        <v>20.61</v>
+      </c>
+      <c r="G647" s="4">
+        <v>15.01</v>
+      </c>
+      <c r="H647" s="4">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="648" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A648" s="8">
         <v>44110</v>
       </c>
+      <c r="B648" s="4">
+        <v>7.7784800000000001</v>
+      </c>
+      <c r="H648" s="4">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="649" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A649" s="8">
         <v>44111</v>
       </c>
+      <c r="B649" s="4">
+        <v>7.7768600000000001</v>
+      </c>
+      <c r="H649" s="4">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="650" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A650" s="8">
         <v>44112</v>
       </c>
+      <c r="H650" s="4">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="651" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A651" s="8">
         <v>44113</v>
       </c>
+      <c r="H651" s="4">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="652" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A652" s="8">
         <v>44114</v>
       </c>
+      <c r="H652" s="4">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="653" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A653" s="8">
         <v>44115</v>
       </c>
+      <c r="H653" s="4">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="654" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A654" s="8">
+        <v>44116</v>
+      </c>
+      <c r="H654" s="27">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="655" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A655" s="8">
+        <v>44117</v>
+      </c>
+      <c r="H655" s="27"/>
+    </row>
+    <row r="656" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A656" s="8">
+        <v>44118</v>
+      </c>
+      <c r="H656" s="27"/>
+    </row>
+    <row r="657" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A657" s="8">
+        <v>44119</v>
+      </c>
+      <c r="H657" s="27"/>
+    </row>
+    <row r="658" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A658" s="8">
+        <v>44120</v>
+      </c>
+      <c r="H658" s="27"/>
+    </row>
+    <row r="659" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A659" s="8">
+        <v>44121</v>
+      </c>
+      <c r="H659" s="27"/>
+    </row>
+    <row r="660" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A660" s="8">
+        <v>44122</v>
+      </c>
+      <c r="H660" s="27"/>
+    </row>
+    <row r="661" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A661" s="8"/>
+      <c r="H661" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="32" type="noConversion"/>
@@ -30203,10 +30405,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-10-2020 02-13-13
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1393" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B92E8B83-3BA4-4EDD-A2C3-53064D2D596F}"/>
+  <xr:revisionPtr revIDLastSave="1418" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{65BE6FC8-EB0B-44CE-AFD2-D71B64469835}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1973,8 +1973,8 @@
   <dimension ref="A1:R661"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A647" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A668" sqref="A668"/>
+      <pane ySplit="3" topLeftCell="A648" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A662" sqref="A662"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1989,7 +1989,7 @@
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" customWidth="1"/>
     <col min="14" max="14" width="20.140625" customWidth="1"/>
     <col min="15" max="15" width="11.85546875" customWidth="1"/>
@@ -4082,10 +4082,18 @@
         <f t="shared" ref="L48:L49" si="3">+K48&amp;", "&amp;J48</f>
         <v>Septiembre, 2020</v>
       </c>
-      <c r="M48" s="27"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="27"/>
-      <c r="P48" s="2"/>
+      <c r="M48" s="27">
+        <v>0</v>
+      </c>
+      <c r="N48" s="2">
+        <v>0</v>
+      </c>
+      <c r="O48" s="27">
+        <v>1</v>
+      </c>
+      <c r="P48" s="2">
+        <v>5000</v>
+      </c>
       <c r="Q48" s="27"/>
       <c r="R48" s="27"/>
     </row>
@@ -14459,10 +14467,10 @@
         <v>24.4373</v>
       </c>
       <c r="C648" s="22">
-        <v>107.73</v>
+        <v>107.65</v>
       </c>
       <c r="D648" s="22">
-        <v>13.86</v>
+        <v>13.88</v>
       </c>
       <c r="E648" s="22"/>
       <c r="F648" s="22"/>
@@ -14476,8 +14484,12 @@
       <c r="B649" s="28">
         <v>24.43</v>
       </c>
-      <c r="C649" s="22"/>
-      <c r="D649" s="22"/>
+      <c r="C649" s="22">
+        <v>109.6</v>
+      </c>
+      <c r="D649" s="22">
+        <v>14.14</v>
+      </c>
       <c r="E649" s="22"/>
       <c r="F649" s="22"/>
       <c r="G649" s="22"/>
@@ -14487,9 +14499,15 @@
       <c r="A650" s="8">
         <v>44112</v>
       </c>
-      <c r="B650" s="28"/>
-      <c r="C650" s="22"/>
-      <c r="D650" s="22"/>
+      <c r="B650" s="28">
+        <v>24.428699999999999</v>
+      </c>
+      <c r="C650" s="22">
+        <v>110.25</v>
+      </c>
+      <c r="D650" s="22">
+        <v>14.17</v>
+      </c>
       <c r="E650" s="22"/>
       <c r="F650" s="22"/>
       <c r="G650" s="22"/>
@@ -14499,9 +14517,15 @@
       <c r="A651" s="8">
         <v>44113</v>
       </c>
-      <c r="B651" s="28"/>
-      <c r="C651" s="22"/>
-      <c r="D651" s="22"/>
+      <c r="B651" s="28">
+        <v>24.428799999999999</v>
+      </c>
+      <c r="C651" s="22">
+        <v>111.13</v>
+      </c>
+      <c r="D651" s="22">
+        <v>14.23</v>
+      </c>
       <c r="E651" s="22"/>
       <c r="F651" s="22"/>
       <c r="G651" s="22"/>
@@ -14543,7 +14567,9 @@
       <c r="A654" s="8">
         <v>44116</v>
       </c>
-      <c r="B654" s="28"/>
+      <c r="B654" s="28">
+        <v>24.4331</v>
+      </c>
       <c r="C654" s="22"/>
       <c r="D654" s="22"/>
       <c r="E654" s="22"/>
@@ -14655,8 +14681,8 @@
   <dimension ref="A1:R661"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A653" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A667" sqref="A667"/>
+      <pane ySplit="3" topLeftCell="A654" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A662" sqref="A662"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16991,10 +17017,10 @@
       <c r="M48" s="27"/>
       <c r="N48" s="2"/>
       <c r="O48" s="22">
-        <v>1013.63</v>
+        <v>3006.3180600000001</v>
       </c>
       <c r="P48" s="22">
-        <v>81.635000000000005</v>
+        <v>176.67</v>
       </c>
       <c r="Q48" s="27"/>
       <c r="R48" s="27"/>
@@ -17035,8 +17061,12 @@
         <v>Octubre, 2020</v>
       </c>
       <c r="N49" s="2"/>
-      <c r="O49" s="22"/>
-      <c r="P49" s="22"/>
+      <c r="O49" s="22">
+        <v>627.53</v>
+      </c>
+      <c r="P49" s="22">
+        <v>16.495000000000001</v>
+      </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
@@ -30314,6 +30344,9 @@
       <c r="A650" s="8">
         <v>44112</v>
       </c>
+      <c r="B650" s="4">
+        <v>7.7770299999999999</v>
+      </c>
       <c r="H650" s="4">
         <v>11.5</v>
       </c>
@@ -30322,6 +30355,9 @@
       <c r="A651" s="8">
         <v>44113</v>
       </c>
+      <c r="B651" s="4">
+        <v>7.7751400000000004</v>
+      </c>
       <c r="H651" s="4">
         <v>11.5</v>
       </c>
@@ -30330,6 +30366,9 @@
       <c r="A652" s="8">
         <v>44114</v>
       </c>
+      <c r="B652" s="27">
+        <v>7.7751400000000004</v>
+      </c>
       <c r="H652" s="4">
         <v>11.5</v>
       </c>
@@ -30338,6 +30377,9 @@
       <c r="A653" s="8">
         <v>44115</v>
       </c>
+      <c r="B653" s="27">
+        <v>7.7751400000000004</v>
+      </c>
       <c r="H653" s="4">
         <v>11.5</v>
       </c>
@@ -30346,6 +30388,9 @@
       <c r="A654" s="8">
         <v>44116</v>
       </c>
+      <c r="B654" s="27">
+        <v>7.7751400000000004</v>
+      </c>
       <c r="H654" s="27">
         <v>11.5</v>
       </c>
@@ -30353,6 +30398,9 @@
     <row r="655" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A655" s="8">
         <v>44117</v>
+      </c>
+      <c r="B655" s="4">
+        <v>7.78165</v>
       </c>
       <c r="H655" s="27"/>
     </row>
@@ -30405,10 +30453,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-14-2020 02-27-59
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1418" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{65BE6FC8-EB0B-44CE-AFD2-D71B64469835}"/>
+  <xr:revisionPtr revIDLastSave="1442" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{96EF8C84-DB23-4F89-8BEF-053E329536B2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1600,9 +1600,58 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>662</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>45999</xdr:colOff>
+      <xdr:row>700</xdr:row>
+      <xdr:rowOff>75286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F6078D0-8549-4EC5-827A-2239464F47B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7924800" y="127444500"/>
+          <a:ext cx="13009524" cy="7314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H660" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H660" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H667" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H667" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1638,8 +1687,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H660" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H660" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H667" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H667" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1970,11 +2019,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R661"/>
+  <dimension ref="A1:R667"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A648" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A662" sqref="A662"/>
+      <pane ySplit="3" topLeftCell="A657" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A673" sqref="A673"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14521,7 +14570,7 @@
         <v>24.428799999999999</v>
       </c>
       <c r="C651" s="22">
-        <v>111.13</v>
+        <v>111.55</v>
       </c>
       <c r="D651" s="22">
         <v>14.23</v>
@@ -14570,8 +14619,12 @@
       <c r="B654" s="28">
         <v>24.4331</v>
       </c>
-      <c r="C654" s="22"/>
-      <c r="D654" s="22"/>
+      <c r="C654" s="22">
+        <v>109.15</v>
+      </c>
+      <c r="D654" s="22">
+        <v>13.84</v>
+      </c>
       <c r="E654" s="22"/>
       <c r="F654" s="22"/>
       <c r="G654" s="22"/>
@@ -14581,9 +14634,15 @@
       <c r="A655" s="8">
         <v>44117</v>
       </c>
-      <c r="B655" s="28"/>
-      <c r="C655" s="22"/>
-      <c r="D655" s="22"/>
+      <c r="B655" s="28">
+        <v>24.428599999999999</v>
+      </c>
+      <c r="C655" s="22">
+        <v>110.03</v>
+      </c>
+      <c r="D655" s="22">
+        <v>14.02</v>
+      </c>
       <c r="E655" s="22"/>
       <c r="F655" s="22"/>
       <c r="G655" s="22"/>
@@ -14593,7 +14652,9 @@
       <c r="A656" s="8">
         <v>44118</v>
       </c>
-      <c r="B656" s="28"/>
+      <c r="B656" s="28">
+        <v>24.428699999999999</v>
+      </c>
       <c r="C656" s="22"/>
       <c r="D656" s="22"/>
       <c r="E656" s="22"/>
@@ -14644,13 +14705,23 @@
       <c r="B660" s="28"/>
       <c r="C660" s="22"/>
       <c r="D660" s="22"/>
-      <c r="E660" s="22"/>
-      <c r="F660" s="22"/>
-      <c r="G660" s="22"/>
-      <c r="H660" s="22"/>
+      <c r="E660" s="22">
+        <v>81.72</v>
+      </c>
+      <c r="F660" s="22">
+        <v>74.83</v>
+      </c>
+      <c r="G660" s="22">
+        <v>61.47</v>
+      </c>
+      <c r="H660" s="22">
+        <v>41.9</v>
+      </c>
     </row>
     <row r="661" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A661" s="8"/>
+      <c r="A661" s="8">
+        <v>44123</v>
+      </c>
       <c r="B661" s="28"/>
       <c r="C661" s="22"/>
       <c r="D661" s="22"/>
@@ -14658,6 +14729,78 @@
       <c r="F661" s="22"/>
       <c r="G661" s="22"/>
       <c r="H661" s="22"/>
+    </row>
+    <row r="662" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A662" s="8">
+        <v>44124</v>
+      </c>
+      <c r="B662" s="28"/>
+      <c r="C662" s="22"/>
+      <c r="D662" s="22"/>
+      <c r="E662" s="22"/>
+      <c r="F662" s="22"/>
+      <c r="G662" s="22"/>
+      <c r="H662" s="22"/>
+    </row>
+    <row r="663" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A663" s="8">
+        <v>44125</v>
+      </c>
+      <c r="B663" s="28"/>
+      <c r="C663" s="22"/>
+      <c r="D663" s="22"/>
+      <c r="E663" s="22"/>
+      <c r="F663" s="22"/>
+      <c r="G663" s="22"/>
+      <c r="H663" s="22"/>
+    </row>
+    <row r="664" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A664" s="8">
+        <v>44126</v>
+      </c>
+      <c r="B664" s="28"/>
+      <c r="C664" s="22"/>
+      <c r="D664" s="22"/>
+      <c r="E664" s="22"/>
+      <c r="F664" s="22"/>
+      <c r="G664" s="22"/>
+      <c r="H664" s="22"/>
+    </row>
+    <row r="665" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A665" s="8">
+        <v>44127</v>
+      </c>
+      <c r="B665" s="28"/>
+      <c r="C665" s="22"/>
+      <c r="D665" s="22"/>
+      <c r="E665" s="22"/>
+      <c r="F665" s="22"/>
+      <c r="G665" s="22"/>
+      <c r="H665" s="22"/>
+    </row>
+    <row r="666" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A666" s="8">
+        <v>44128</v>
+      </c>
+      <c r="B666" s="28"/>
+      <c r="C666" s="22"/>
+      <c r="D666" s="22"/>
+      <c r="E666" s="22"/>
+      <c r="F666" s="22"/>
+      <c r="G666" s="22"/>
+      <c r="H666" s="22"/>
+    </row>
+    <row r="667" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A667" s="8">
+        <v>44129</v>
+      </c>
+      <c r="B667" s="28"/>
+      <c r="C667" s="22"/>
+      <c r="D667" s="22"/>
+      <c r="E667" s="22"/>
+      <c r="F667" s="22"/>
+      <c r="G667" s="22"/>
+      <c r="H667" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -14678,11 +14821,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R661"/>
+  <dimension ref="A1:R667"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A654" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A662" sqref="A662"/>
+      <pane ySplit="3" topLeftCell="A659" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A669" sqref="A669"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30391,6 +30534,15 @@
       <c r="B654" s="27">
         <v>7.7751400000000004</v>
       </c>
+      <c r="E654" s="4">
+        <v>21.41</v>
+      </c>
+      <c r="F654" s="4">
+        <v>20.61</v>
+      </c>
+      <c r="G654" s="4">
+        <v>15.03</v>
+      </c>
       <c r="H654" s="27">
         <v>11.5</v>
       </c>
@@ -30408,6 +30560,9 @@
       <c r="A656" s="8">
         <v>44118</v>
       </c>
+      <c r="B656" s="4">
+        <v>7.7769599999999999</v>
+      </c>
       <c r="H656" s="27"/>
     </row>
     <row r="657" spans="1:8" x14ac:dyDescent="0.25">
@@ -30435,15 +30590,48 @@
       <c r="H660" s="27"/>
     </row>
     <row r="661" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A661" s="8"/>
+      <c r="A661" s="8">
+        <v>44123</v>
+      </c>
       <c r="H661" s="27"/>
+    </row>
+    <row r="662" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A662" s="8">
+        <v>44124</v>
+      </c>
+    </row>
+    <row r="663" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A663" s="8">
+        <v>44125</v>
+      </c>
+    </row>
+    <row r="664" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A664" s="8">
+        <v>44126</v>
+      </c>
+    </row>
+    <row r="665" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A665" s="8">
+        <v>44127</v>
+      </c>
+    </row>
+    <row r="666" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A666" s="8">
+        <v>44128</v>
+      </c>
+    </row>
+    <row r="667" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A667" s="8">
+        <v>44129</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -30453,10 +30641,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-17-2020 01-27-35
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1442" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{96EF8C84-DB23-4F89-8BEF-053E329536B2}"/>
+  <xr:revisionPtr revIDLastSave="1463" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C5BB1DF9-CAF3-40DB-AFB4-F73D75BE9748}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="134">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -472,6 +472,9 @@
   </si>
   <si>
     <t>https://www.ine.gob.hn/V3/</t>
+  </si>
+  <si>
+    <t>https://mem.gob.gt/precios-petroleo-combustibles/</t>
   </si>
 </sst>
 </file>
@@ -1600,55 +1603,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>662</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>45999</xdr:colOff>
-      <xdr:row>700</xdr:row>
-      <xdr:rowOff>75286</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F6078D0-8549-4EC5-827A-2239464F47B3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7924800" y="127444500"/>
-          <a:ext cx="13009524" cy="7314286"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H667" totalsRowShown="0" headerRowDxfId="25">
   <autoFilter ref="A3:H667" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
@@ -2022,8 +1976,8 @@
   <dimension ref="A1:R667"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A657" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A673" sqref="A673"/>
+      <pane ySplit="3" topLeftCell="A658" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A674" sqref="A674"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14638,10 +14592,10 @@
         <v>24.428599999999999</v>
       </c>
       <c r="C655" s="22">
-        <v>110.03</v>
+        <v>110.1</v>
       </c>
       <c r="D655" s="22">
-        <v>14.02</v>
+        <v>14.01</v>
       </c>
       <c r="E655" s="22"/>
       <c r="F655" s="22"/>
@@ -14655,8 +14609,12 @@
       <c r="B656" s="28">
         <v>24.428699999999999</v>
       </c>
-      <c r="C656" s="22"/>
-      <c r="D656" s="22"/>
+      <c r="C656" s="22">
+        <v>109.6</v>
+      </c>
+      <c r="D656" s="22">
+        <v>14.2</v>
+      </c>
       <c r="E656" s="22"/>
       <c r="F656" s="22"/>
       <c r="G656" s="22"/>
@@ -14666,9 +14624,15 @@
       <c r="A657" s="8">
         <v>44119</v>
       </c>
-      <c r="B657" s="28"/>
-      <c r="C657" s="22"/>
-      <c r="D657" s="22"/>
+      <c r="B657" s="28">
+        <v>24.4221</v>
+      </c>
+      <c r="C657" s="22">
+        <v>109.5</v>
+      </c>
+      <c r="D657" s="22">
+        <v>14.18</v>
+      </c>
       <c r="E657" s="22"/>
       <c r="F657" s="22"/>
       <c r="G657" s="22"/>
@@ -14678,9 +14642,15 @@
       <c r="A658" s="8">
         <v>44120</v>
       </c>
-      <c r="B658" s="28"/>
-      <c r="C658" s="22"/>
-      <c r="D658" s="22"/>
+      <c r="B658" s="28">
+        <v>24.4117</v>
+      </c>
+      <c r="C658" s="22">
+        <v>106.9</v>
+      </c>
+      <c r="D658" s="22">
+        <v>14.45</v>
+      </c>
       <c r="E658" s="22"/>
       <c r="F658" s="22"/>
       <c r="G658" s="22"/>
@@ -14722,7 +14692,9 @@
       <c r="A661" s="8">
         <v>44123</v>
       </c>
-      <c r="B661" s="28"/>
+      <c r="B661" s="28">
+        <v>24.403400000000001</v>
+      </c>
       <c r="C661" s="22"/>
       <c r="D661" s="22"/>
       <c r="E661" s="22"/>
@@ -14824,8 +14796,8 @@
   <dimension ref="A1:R667"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A659" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A669" sqref="A669"/>
+      <pane ySplit="3" topLeftCell="A660" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A671" sqref="A671"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30569,36 +30541,54 @@
       <c r="A657" s="8">
         <v>44119</v>
       </c>
+      <c r="B657" s="4">
+        <v>7.7794999999999996</v>
+      </c>
       <c r="H657" s="27"/>
     </row>
     <row r="658" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A658" s="8">
         <v>44120</v>
       </c>
+      <c r="B658" s="4">
+        <v>7.7823099999999998</v>
+      </c>
       <c r="H658" s="27"/>
     </row>
     <row r="659" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A659" s="8">
         <v>44121</v>
       </c>
+      <c r="B659" s="27">
+        <v>7.7823099999999998</v>
+      </c>
       <c r="H659" s="27"/>
     </row>
     <row r="660" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A660" s="8">
         <v>44122</v>
       </c>
+      <c r="B660" s="27">
+        <v>7.7823099999999998</v>
+      </c>
       <c r="H660" s="27"/>
     </row>
     <row r="661" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A661" s="8">
         <v>44123</v>
       </c>
+      <c r="B661" s="4">
+        <v>7.78355</v>
+      </c>
       <c r="H661" s="27"/>
     </row>
     <row r="662" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A662" s="8">
         <v>44124</v>
       </c>
+      <c r="B662" s="27">
+        <v>7.78355</v>
+      </c>
     </row>
     <row r="663" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A663" s="8">
@@ -30628,10 +30618,9 @@
   </sheetData>
   <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
   <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -30644,7 +30633,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -30992,7 +30981,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>90</v>
@@ -31047,7 +31036,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>91</v>
@@ -31102,7 +31091,7 @@
         <v>36</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>92</v>
@@ -33357,14 +33346,15 @@
     <hyperlink ref="H12" r:id="rId48" xr:uid="{C39C3BB3-728F-42C9-9F79-687468489142}"/>
     <hyperlink ref="F21:F23" r:id="rId49" display="https://www.bch.hn/estadisticassv.php" xr:uid="{F479A45E-5F7A-41F4-8FCD-0A3A67241764}"/>
     <hyperlink ref="F5" r:id="rId50" xr:uid="{EB6C19CD-A8BD-482E-B1F2-F7AE05904A57}"/>
-    <hyperlink ref="F6:F8" r:id="rId51" display="https://www.mem.gob.gt/hidrocarburos/precios-combustible-nacionales/" xr:uid="{630442E1-9898-4043-AFD9-BEF9DF0EFD23}"/>
-    <hyperlink ref="F9" r:id="rId52" xr:uid="{EBD6F2F9-A288-4A48-AD1C-B027F0B1FDCC}"/>
+    <hyperlink ref="F9" r:id="rId51" xr:uid="{EBD6F2F9-A288-4A48-AD1C-B027F0B1FDCC}"/>
+    <hyperlink ref="F6" r:id="rId52" xr:uid="{68FFD4E7-0A3D-4EB3-A5FE-AD91A128FC22}"/>
+    <hyperlink ref="F7:F8" r:id="rId53" display="https://mem.gob.gt/precios-petroleo-combustibles/" xr:uid="{F419304C-0E16-4626-AF11-25645A6D96E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId53"/>
+  <legacyDrawing r:id="rId54"/>
   <tableParts count="1">
-    <tablePart r:id="rId54"/>
+    <tablePart r:id="rId55"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 10-21-2020 01-42-42
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1463" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C5BB1DF9-CAF3-40DB-AFB4-F73D75BE9748}"/>
+  <xr:revisionPtr revIDLastSave="1480" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{45EB601B-457C-40A1-AA73-B141F8D72A84}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1604,8 +1604,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H667" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H667" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H674" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H674" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1641,8 +1641,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H667" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H667" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H674" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H674" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1973,11 +1973,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R667"/>
+  <dimension ref="A1:R674"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A658" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A674" sqref="A674"/>
+      <pane ySplit="3" topLeftCell="A662" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A678" sqref="A678"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14646,10 +14646,10 @@
         <v>24.4117</v>
       </c>
       <c r="C658" s="22">
-        <v>106.9</v>
+        <v>107.25</v>
       </c>
       <c r="D658" s="22">
-        <v>14.45</v>
+        <v>14.43</v>
       </c>
       <c r="E658" s="22"/>
       <c r="F658" s="22"/>
@@ -14695,8 +14695,12 @@
       <c r="B661" s="28">
         <v>24.403400000000001</v>
       </c>
-      <c r="C661" s="22"/>
-      <c r="D661" s="22"/>
+      <c r="C661" s="22">
+        <v>106.05</v>
+      </c>
+      <c r="D661" s="22">
+        <v>14.72</v>
+      </c>
       <c r="E661" s="22"/>
       <c r="F661" s="22"/>
       <c r="G661" s="22"/>
@@ -14706,9 +14710,15 @@
       <c r="A662" s="8">
         <v>44124</v>
       </c>
-      <c r="B662" s="28"/>
-      <c r="C662" s="22"/>
-      <c r="D662" s="22"/>
+      <c r="B662" s="28">
+        <v>24.3933</v>
+      </c>
+      <c r="C662" s="22">
+        <v>104.78</v>
+      </c>
+      <c r="D662" s="22">
+        <v>14.52</v>
+      </c>
       <c r="E662" s="22"/>
       <c r="F662" s="22"/>
       <c r="G662" s="22"/>
@@ -14718,7 +14728,9 @@
       <c r="A663" s="8">
         <v>44125</v>
       </c>
-      <c r="B663" s="28"/>
+      <c r="B663" s="28">
+        <v>24.380700000000001</v>
+      </c>
       <c r="C663" s="22"/>
       <c r="D663" s="22"/>
       <c r="E663" s="22"/>
@@ -14769,10 +14781,102 @@
       <c r="B667" s="28"/>
       <c r="C667" s="22"/>
       <c r="D667" s="22"/>
-      <c r="E667" s="22"/>
-      <c r="F667" s="22"/>
-      <c r="G667" s="22"/>
-      <c r="H667" s="22"/>
+      <c r="E667" s="22">
+        <v>81.98</v>
+      </c>
+      <c r="F667" s="22">
+        <v>75.25</v>
+      </c>
+      <c r="G667" s="22">
+        <v>61.88</v>
+      </c>
+      <c r="H667" s="22">
+        <v>42.39</v>
+      </c>
+    </row>
+    <row r="668" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A668" s="8">
+        <v>44130</v>
+      </c>
+      <c r="B668" s="28"/>
+      <c r="C668" s="22"/>
+      <c r="D668" s="22"/>
+      <c r="E668" s="22"/>
+      <c r="F668" s="22"/>
+      <c r="G668" s="22"/>
+      <c r="H668" s="22"/>
+    </row>
+    <row r="669" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A669" s="8">
+        <v>44131</v>
+      </c>
+      <c r="B669" s="28"/>
+      <c r="C669" s="22"/>
+      <c r="D669" s="22"/>
+      <c r="E669" s="22"/>
+      <c r="F669" s="22"/>
+      <c r="G669" s="22"/>
+      <c r="H669" s="22"/>
+    </row>
+    <row r="670" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A670" s="8">
+        <v>44132</v>
+      </c>
+      <c r="B670" s="28"/>
+      <c r="C670" s="22"/>
+      <c r="D670" s="22"/>
+      <c r="E670" s="22"/>
+      <c r="F670" s="22"/>
+      <c r="G670" s="22"/>
+      <c r="H670" s="22"/>
+    </row>
+    <row r="671" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A671" s="8">
+        <v>44133</v>
+      </c>
+      <c r="B671" s="28"/>
+      <c r="C671" s="22"/>
+      <c r="D671" s="22"/>
+      <c r="E671" s="22"/>
+      <c r="F671" s="22"/>
+      <c r="G671" s="22"/>
+      <c r="H671" s="22"/>
+    </row>
+    <row r="672" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A672" s="8">
+        <v>44134</v>
+      </c>
+      <c r="B672" s="28"/>
+      <c r="C672" s="22"/>
+      <c r="D672" s="22"/>
+      <c r="E672" s="22"/>
+      <c r="F672" s="22"/>
+      <c r="G672" s="22"/>
+      <c r="H672" s="22"/>
+    </row>
+    <row r="673" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A673" s="8">
+        <v>44135</v>
+      </c>
+      <c r="B673" s="28"/>
+      <c r="C673" s="22"/>
+      <c r="D673" s="22"/>
+      <c r="E673" s="22"/>
+      <c r="F673" s="22"/>
+      <c r="G673" s="22"/>
+      <c r="H673" s="22"/>
+    </row>
+    <row r="674" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A674" s="8">
+        <v>44136</v>
+      </c>
+      <c r="B674" s="28"/>
+      <c r="C674" s="22"/>
+      <c r="D674" s="22"/>
+      <c r="E674" s="22"/>
+      <c r="F674" s="22"/>
+      <c r="G674" s="22"/>
+      <c r="H674" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -14793,11 +14897,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R667"/>
+  <dimension ref="A1:R674"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A660" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A671" sqref="A671"/>
+      <pane ySplit="3" topLeftCell="A667" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A678" sqref="A678"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30594,6 +30698,9 @@
       <c r="A663" s="8">
         <v>44125</v>
       </c>
+      <c r="B663" s="4">
+        <v>7.7778999999999998</v>
+      </c>
     </row>
     <row r="664" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A664" s="8">
@@ -30613,6 +30720,41 @@
     <row r="667" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A667" s="8">
         <v>44129</v>
+      </c>
+    </row>
+    <row r="668" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A668" s="8">
+        <v>44130</v>
+      </c>
+    </row>
+    <row r="669" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A669" s="8">
+        <v>44131</v>
+      </c>
+    </row>
+    <row r="670" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A670" s="8">
+        <v>44132</v>
+      </c>
+    </row>
+    <row r="671" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A671" s="8">
+        <v>44133</v>
+      </c>
+    </row>
+    <row r="672" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A672" s="8">
+        <v>44134</v>
+      </c>
+    </row>
+    <row r="673" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A673" s="8">
+        <v>44135</v>
+      </c>
+    </row>
+    <row r="674" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A674" s="8">
+        <v>44136</v>
       </c>
     </row>
   </sheetData>
@@ -30633,7 +30775,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-24-2020 01-54-45
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1480" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{45EB601B-457C-40A1-AA73-B141F8D72A84}"/>
+  <xr:revisionPtr revIDLastSave="1511" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E8D1031-96B8-49A0-B16B-5B2B1CD6F5E3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,9 +354,6 @@
     <t>Precios de combustibles (galones). Combustible Kerosene</t>
   </si>
   <si>
-    <t>http://www.banguat.gob.gt/variables/seleccion.ASP?grupo=8</t>
-  </si>
-  <si>
     <t>.xls</t>
   </si>
   <si>
@@ -475,6 +472,9 @@
   </si>
   <si>
     <t>https://mem.gob.gt/precios-petroleo-combustibles/</t>
+  </si>
+  <si>
+    <t>https://app1.banguat.gob.gt/ords/f?p=215:8:8626733943480::::P8_GRUPO:8</t>
   </si>
 </sst>
 </file>
@@ -1976,8 +1976,8 @@
   <dimension ref="A1:R674"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A662" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A678" sqref="A678"/>
+      <pane ySplit="3" topLeftCell="A667" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B674" sqref="B674"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14714,10 +14714,10 @@
         <v>24.3933</v>
       </c>
       <c r="C662" s="22">
-        <v>104.78</v>
+        <v>104.9</v>
       </c>
       <c r="D662" s="22">
-        <v>14.52</v>
+        <v>14.54</v>
       </c>
       <c r="E662" s="22"/>
       <c r="F662" s="22"/>
@@ -14731,8 +14731,12 @@
       <c r="B663" s="28">
         <v>24.380700000000001</v>
       </c>
-      <c r="C663" s="22"/>
-      <c r="D663" s="22"/>
+      <c r="C663" s="22">
+        <v>104.15</v>
+      </c>
+      <c r="D663" s="22">
+        <v>14.5</v>
+      </c>
       <c r="E663" s="22"/>
       <c r="F663" s="22"/>
       <c r="G663" s="22"/>
@@ -14742,9 +14746,15 @@
       <c r="A664" s="8">
         <v>44126</v>
       </c>
-      <c r="B664" s="28"/>
-      <c r="C664" s="22"/>
-      <c r="D664" s="22"/>
+      <c r="B664" s="28">
+        <v>24.367999999999999</v>
+      </c>
+      <c r="C664" s="22">
+        <v>106.7</v>
+      </c>
+      <c r="D664" s="22">
+        <v>14.78</v>
+      </c>
       <c r="E664" s="22"/>
       <c r="F664" s="22"/>
       <c r="G664" s="22"/>
@@ -14754,9 +14764,15 @@
       <c r="A665" s="8">
         <v>44127</v>
       </c>
-      <c r="B665" s="28"/>
-      <c r="C665" s="22"/>
-      <c r="D665" s="22"/>
+      <c r="B665" s="28">
+        <v>24.361699999999999</v>
+      </c>
+      <c r="C665" s="22">
+        <v>105.38</v>
+      </c>
+      <c r="D665" s="22">
+        <v>14.73</v>
+      </c>
       <c r="E665" s="22"/>
       <c r="F665" s="22"/>
       <c r="G665" s="22"/>
@@ -14798,7 +14814,9 @@
       <c r="A668" s="8">
         <v>44130</v>
       </c>
-      <c r="B668" s="28"/>
+      <c r="B668" s="28">
+        <v>24.3522</v>
+      </c>
       <c r="C668" s="22"/>
       <c r="D668" s="22"/>
       <c r="E668" s="22"/>
@@ -14900,8 +14918,8 @@
   <dimension ref="A1:R674"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A667" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A678" sqref="A678"/>
+      <pane ySplit="3" topLeftCell="A670" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B674" sqref="B674"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30684,6 +30702,15 @@
       <c r="B661" s="4">
         <v>7.78355</v>
       </c>
+      <c r="E661" s="4">
+        <v>21.31</v>
+      </c>
+      <c r="F661" s="4">
+        <v>20.51</v>
+      </c>
+      <c r="G661" s="4">
+        <v>15</v>
+      </c>
       <c r="H661" s="27"/>
     </row>
     <row r="662" spans="1:8" x14ac:dyDescent="0.25">
@@ -30706,25 +30733,40 @@
       <c r="A664" s="8">
         <v>44126</v>
       </c>
+      <c r="B664" s="4">
+        <v>7.7804599999999997</v>
+      </c>
     </row>
     <row r="665" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A665" s="8">
         <v>44127</v>
       </c>
+      <c r="B665" s="4">
+        <v>7.7803500000000003</v>
+      </c>
     </row>
     <row r="666" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A666" s="8">
         <v>44128</v>
       </c>
+      <c r="B666" s="27">
+        <v>7.7803500000000003</v>
+      </c>
     </row>
     <row r="667" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A667" s="8">
         <v>44129</v>
       </c>
+      <c r="B667" s="27">
+        <v>7.7803500000000003</v>
+      </c>
     </row>
     <row r="668" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A668" s="8">
         <v>44130</v>
+      </c>
+      <c r="B668" s="27">
+        <v>7.7798299999999996</v>
       </c>
     </row>
     <row r="669" spans="1:8" x14ac:dyDescent="0.25">
@@ -31123,7 +31165,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>90</v>
@@ -31178,7 +31220,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>91</v>
@@ -31233,7 +31275,7 @@
         <v>36</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>92</v>
@@ -31288,7 +31330,7 @@
         <v>38</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>38</v>
@@ -31326,7 +31368,7 @@
         <v>76</v>
       </c>
       <c r="T9" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U9" s="19"/>
     </row>
@@ -31347,7 +31389,7 @@
         <v>39</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>39</v>
@@ -31385,7 +31427,7 @@
         <v>76</v>
       </c>
       <c r="T10" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U10" s="19"/>
     </row>
@@ -31394,7 +31436,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" s="16">
         <v>7</v>
@@ -31406,21 +31448,21 @@
         <v>19</v>
       </c>
       <c r="F11" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>97</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K11" s="17"/>
       <c r="L11" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
@@ -31451,7 +31493,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="16">
         <v>7</v>
@@ -31460,22 +31502,22 @@
         <v>66</v>
       </c>
       <c r="E12" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="G12" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="H12" s="17" t="s">
         <v>103</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>104</v>
       </c>
       <c r="I12" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K12" s="17"/>
       <c r="L12" s="16"/>
@@ -31508,7 +31550,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="16">
         <v>7</v>
@@ -31517,22 +31559,22 @@
         <v>66</v>
       </c>
       <c r="E13" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="G13" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="H13" s="17" t="s">
         <v>109</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>110</v>
       </c>
       <c r="I13" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K13" s="17"/>
       <c r="L13" s="16"/>
@@ -31548,7 +31590,7 @@
         <v>43963</v>
       </c>
       <c r="R13" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S13" s="14" t="s">
         <v>76</v>
@@ -31563,7 +31605,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" s="16">
         <v>7</v>
@@ -31572,20 +31614,20 @@
         <v>66</v>
       </c>
       <c r="E14" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="G14" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>116</v>
       </c>
       <c r="H14" s="17"/>
       <c r="I14" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K14" s="17"/>
       <c r="L14" s="16"/>
@@ -31601,7 +31643,7 @@
         <v>43963</v>
       </c>
       <c r="R14" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S14" s="14" t="s">
         <v>76</v>
@@ -31618,7 +31660,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" s="16">
         <v>7</v>
@@ -31627,20 +31669,20 @@
         <v>66</v>
       </c>
       <c r="E15" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="G15" s="16" t="s">
         <v>119</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>120</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K15" s="17"/>
       <c r="L15" s="16"/>
@@ -31656,7 +31698,7 @@
         <v>43963</v>
       </c>
       <c r="R15" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S15" s="14" t="s">
         <v>76</v>
@@ -31673,7 +31715,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C16" s="16">
         <v>7</v>
@@ -31685,7 +31727,7 @@
         <v>9</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>86</v>
@@ -31695,7 +31737,7 @@
         <v>71</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K16" s="17"/>
       <c r="L16" s="16"/>
@@ -31711,13 +31753,13 @@
         <v>43968</v>
       </c>
       <c r="R16" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S16" s="14" t="s">
         <v>76</v>
       </c>
       <c r="T16" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U16" s="19" t="s">
         <v>82</v>
@@ -31728,7 +31770,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" s="16">
         <v>7</v>
@@ -31740,7 +31782,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>90</v>
@@ -31750,7 +31792,7 @@
         <v>71</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K17" s="17"/>
       <c r="L17" s="16"/>
@@ -31766,13 +31808,13 @@
         <v>43968</v>
       </c>
       <c r="R17" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S17" s="14" t="s">
         <v>76</v>
       </c>
       <c r="T17" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U17" s="19" t="s">
         <v>82</v>
@@ -31783,7 +31825,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18" s="16">
         <v>7</v>
@@ -31795,7 +31837,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>91</v>
@@ -31805,7 +31847,7 @@
         <v>71</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K18" s="17"/>
       <c r="L18" s="16"/>
@@ -31821,13 +31863,13 @@
         <v>43968</v>
       </c>
       <c r="R18" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S18" s="14" t="s">
         <v>76</v>
       </c>
       <c r="T18" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U18" s="19" t="s">
         <v>82</v>
@@ -31838,7 +31880,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="16">
         <v>7</v>
@@ -31850,7 +31892,7 @@
         <v>12</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>92</v>
@@ -31860,7 +31902,7 @@
         <v>71</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K19" s="17"/>
       <c r="L19" s="16"/>
@@ -31876,13 +31918,13 @@
         <v>43968</v>
       </c>
       <c r="R19" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S19" s="14" t="s">
         <v>76</v>
       </c>
       <c r="T19" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U19" s="19" t="s">
         <v>82</v>
@@ -31893,7 +31935,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" s="16">
         <v>7</v>
@@ -31905,19 +31947,19 @@
         <v>15</v>
       </c>
       <c r="F20" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="G20" s="16" t="s">
-        <v>126</v>
-      </c>
       <c r="H20" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K20" s="17"/>
       <c r="L20" s="16"/>
@@ -31933,7 +31975,7 @@
         <v>43963</v>
       </c>
       <c r="R20" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S20" s="14" t="s">
         <v>76</v>
@@ -31948,7 +31990,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C21" s="16">
         <v>7</v>
@@ -31960,19 +32002,19 @@
         <v>16</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I21" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K21" s="17"/>
       <c r="L21" s="16"/>
@@ -31988,7 +32030,7 @@
         <v>43963</v>
       </c>
       <c r="R21" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S21" s="14" t="s">
         <v>76</v>
@@ -32003,7 +32045,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" s="16">
         <v>7</v>
@@ -32015,19 +32057,19 @@
         <v>17</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I22" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K22" s="17"/>
       <c r="L22" s="16"/>
@@ -32043,7 +32085,7 @@
         <v>43963</v>
       </c>
       <c r="R22" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S22" s="14" t="s">
         <v>76</v>
@@ -32058,7 +32100,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="16">
         <v>7</v>
@@ -32070,19 +32112,19 @@
         <v>18</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I23" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K23" s="17"/>
       <c r="L23" s="16"/>
@@ -32098,7 +32140,7 @@
         <v>43963</v>
       </c>
       <c r="R23" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S23" s="14" t="s">
         <v>76</v>
@@ -32113,7 +32155,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C24" s="16">
         <v>7</v>
@@ -32125,19 +32167,19 @@
         <v>19</v>
       </c>
       <c r="F24" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>130</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>131</v>
       </c>
       <c r="I24" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K24" s="17"/>
       <c r="L24" s="16"/>
@@ -32153,7 +32195,7 @@
         <v>43963</v>
       </c>
       <c r="R24" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S24" s="14" t="s">
         <v>76</v>
@@ -32168,7 +32210,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C25" s="16">
         <v>7</v>
@@ -32177,22 +32219,22 @@
         <v>66</v>
       </c>
       <c r="E25" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="G25" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="H25" s="17" t="s">
         <v>103</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>104</v>
       </c>
       <c r="I25" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K25" s="17"/>
       <c r="L25" s="16"/>
@@ -32208,7 +32250,7 @@
         <v>43963</v>
       </c>
       <c r="R25" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S25" s="14" t="s">
         <v>76</v>
@@ -33474,23 +33516,23 @@
     <hyperlink ref="J6:J8" r:id="rId34" display="https://www.mem.gob.gt/" xr:uid="{A84CC70A-0414-4A2E-BEC8-5680985BE81A}"/>
     <hyperlink ref="H5" r:id="rId35" xr:uid="{D6CB5105-27CA-4EBD-8FAF-6AD03BA57E8E}"/>
     <hyperlink ref="H6:H8" r:id="rId36" display="https://www.mem.gob.gt/contacto/escribenos/" xr:uid="{2E1D2851-EF7B-4D6D-88ED-9BA745AF8A9B}"/>
-    <hyperlink ref="F10" r:id="rId37" xr:uid="{5388C766-549D-4DB9-B8A2-EF392AA68BF7}"/>
-    <hyperlink ref="K9" r:id="rId38" xr:uid="{C9FF6777-B7D0-49C1-AFC0-42C7B34A16CC}"/>
-    <hyperlink ref="J9" r:id="rId39" xr:uid="{D3E3CC2A-5411-4646-85D7-6917F62C49C4}"/>
-    <hyperlink ref="H9" r:id="rId40" xr:uid="{B0996637-B8DB-4605-AAE3-1BD61E4675C6}"/>
-    <hyperlink ref="K10" r:id="rId41" xr:uid="{729A966F-2F4A-4CE1-986B-C3B4D21BE0E6}"/>
-    <hyperlink ref="J10" r:id="rId42" xr:uid="{B180DAC5-027A-49A2-8EE3-C47F162824D8}"/>
-    <hyperlink ref="H10" r:id="rId43" xr:uid="{4180A254-40D1-4B19-B9ED-BC98556E01E0}"/>
-    <hyperlink ref="F11" r:id="rId44" xr:uid="{AD0FFFD7-B5EA-4CC6-A2D7-FC711CD9E273}"/>
-    <hyperlink ref="J11" r:id="rId45" xr:uid="{8D3835B9-F568-4D8F-9CD9-8D260D5A6E1A}"/>
-    <hyperlink ref="F12" r:id="rId46" xr:uid="{5BF57AB9-6786-45D4-9B41-00A80ED5A879}"/>
-    <hyperlink ref="J12" r:id="rId47" xr:uid="{610A88D3-7410-471E-8CBA-E264F4E6D8F1}"/>
-    <hyperlink ref="H12" r:id="rId48" xr:uid="{C39C3BB3-728F-42C9-9F79-687468489142}"/>
-    <hyperlink ref="F21:F23" r:id="rId49" display="https://www.bch.hn/estadisticassv.php" xr:uid="{F479A45E-5F7A-41F4-8FCD-0A3A67241764}"/>
-    <hyperlink ref="F5" r:id="rId50" xr:uid="{EB6C19CD-A8BD-482E-B1F2-F7AE05904A57}"/>
-    <hyperlink ref="F9" r:id="rId51" xr:uid="{EBD6F2F9-A288-4A48-AD1C-B027F0B1FDCC}"/>
-    <hyperlink ref="F6" r:id="rId52" xr:uid="{68FFD4E7-0A3D-4EB3-A5FE-AD91A128FC22}"/>
-    <hyperlink ref="F7:F8" r:id="rId53" display="https://mem.gob.gt/precios-petroleo-combustibles/" xr:uid="{F419304C-0E16-4626-AF11-25645A6D96E7}"/>
+    <hyperlink ref="K9" r:id="rId37" xr:uid="{C9FF6777-B7D0-49C1-AFC0-42C7B34A16CC}"/>
+    <hyperlink ref="J9" r:id="rId38" xr:uid="{D3E3CC2A-5411-4646-85D7-6917F62C49C4}"/>
+    <hyperlink ref="H9" r:id="rId39" xr:uid="{B0996637-B8DB-4605-AAE3-1BD61E4675C6}"/>
+    <hyperlink ref="K10" r:id="rId40" xr:uid="{729A966F-2F4A-4CE1-986B-C3B4D21BE0E6}"/>
+    <hyperlink ref="J10" r:id="rId41" xr:uid="{B180DAC5-027A-49A2-8EE3-C47F162824D8}"/>
+    <hyperlink ref="H10" r:id="rId42" xr:uid="{4180A254-40D1-4B19-B9ED-BC98556E01E0}"/>
+    <hyperlink ref="F11" r:id="rId43" xr:uid="{AD0FFFD7-B5EA-4CC6-A2D7-FC711CD9E273}"/>
+    <hyperlink ref="J11" r:id="rId44" xr:uid="{8D3835B9-F568-4D8F-9CD9-8D260D5A6E1A}"/>
+    <hyperlink ref="F12" r:id="rId45" xr:uid="{5BF57AB9-6786-45D4-9B41-00A80ED5A879}"/>
+    <hyperlink ref="J12" r:id="rId46" xr:uid="{610A88D3-7410-471E-8CBA-E264F4E6D8F1}"/>
+    <hyperlink ref="H12" r:id="rId47" xr:uid="{C39C3BB3-728F-42C9-9F79-687468489142}"/>
+    <hyperlink ref="F21:F23" r:id="rId48" display="https://www.bch.hn/estadisticassv.php" xr:uid="{F479A45E-5F7A-41F4-8FCD-0A3A67241764}"/>
+    <hyperlink ref="F5" r:id="rId49" xr:uid="{EB6C19CD-A8BD-482E-B1F2-F7AE05904A57}"/>
+    <hyperlink ref="F9" r:id="rId50" xr:uid="{EBD6F2F9-A288-4A48-AD1C-B027F0B1FDCC}"/>
+    <hyperlink ref="F6" r:id="rId51" xr:uid="{68FFD4E7-0A3D-4EB3-A5FE-AD91A128FC22}"/>
+    <hyperlink ref="F7:F8" r:id="rId52" display="https://mem.gob.gt/precios-petroleo-combustibles/" xr:uid="{F419304C-0E16-4626-AF11-25645A6D96E7}"/>
+    <hyperlink ref="F10" r:id="rId53" xr:uid="{11A8405E-B255-49D3-A986-892C6FE35B72}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-28-2020 02-11-34
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1511" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E8D1031-96B8-49A0-B16B-5B2B1CD6F5E3}"/>
+  <xr:revisionPtr revIDLastSave="1532" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9BAB9805-5577-4FE4-AF18-AC63BE2D1541}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1604,8 +1604,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H674" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H674" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H681" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H681" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1641,8 +1641,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H674" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H674" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H681" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H681" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1973,11 +1973,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R674"/>
+  <dimension ref="A1:R681"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A667" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B674" sqref="B674"/>
+      <pane ySplit="3" topLeftCell="A672" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A688" sqref="A688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14768,10 +14768,10 @@
         <v>24.361699999999999</v>
       </c>
       <c r="C665" s="22">
-        <v>105.38</v>
+        <v>105.6</v>
       </c>
       <c r="D665" s="22">
-        <v>14.73</v>
+        <v>14.72</v>
       </c>
       <c r="E665" s="22"/>
       <c r="F665" s="22"/>
@@ -14817,8 +14817,12 @@
       <c r="B668" s="28">
         <v>24.3522</v>
       </c>
-      <c r="C668" s="22"/>
-      <c r="D668" s="22"/>
+      <c r="C668" s="22">
+        <v>106.65</v>
+      </c>
+      <c r="D668" s="22">
+        <v>14.77</v>
+      </c>
       <c r="E668" s="22"/>
       <c r="F668" s="22"/>
       <c r="G668" s="22"/>
@@ -14828,9 +14832,15 @@
       <c r="A669" s="8">
         <v>44131</v>
       </c>
-      <c r="B669" s="28"/>
-      <c r="C669" s="22"/>
-      <c r="D669" s="22"/>
+      <c r="B669" s="28">
+        <v>24.343</v>
+      </c>
+      <c r="C669" s="22">
+        <v>106.98</v>
+      </c>
+      <c r="D669" s="22">
+        <v>14.89</v>
+      </c>
       <c r="E669" s="22"/>
       <c r="F669" s="22"/>
       <c r="G669" s="22"/>
@@ -14840,7 +14850,9 @@
       <c r="A670" s="8">
         <v>44132</v>
       </c>
-      <c r="B670" s="28"/>
+      <c r="B670" s="28">
+        <v>24.3277</v>
+      </c>
       <c r="C670" s="22"/>
       <c r="D670" s="22"/>
       <c r="E670" s="22"/>
@@ -14891,10 +14903,102 @@
       <c r="B674" s="28"/>
       <c r="C674" s="22"/>
       <c r="D674" s="22"/>
-      <c r="E674" s="22"/>
-      <c r="F674" s="22"/>
-      <c r="G674" s="22"/>
-      <c r="H674" s="22"/>
+      <c r="E674" s="22">
+        <v>81.42</v>
+      </c>
+      <c r="F674" s="22">
+        <v>74.790000000000006</v>
+      </c>
+      <c r="G674" s="22">
+        <v>61.88</v>
+      </c>
+      <c r="H674" s="22">
+        <v>42.66</v>
+      </c>
+    </row>
+    <row r="675" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A675" s="8">
+        <v>44137</v>
+      </c>
+      <c r="B675" s="28"/>
+      <c r="C675" s="22"/>
+      <c r="D675" s="22"/>
+      <c r="E675" s="22"/>
+      <c r="F675" s="22"/>
+      <c r="G675" s="22"/>
+      <c r="H675" s="22"/>
+    </row>
+    <row r="676" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A676" s="8">
+        <v>44138</v>
+      </c>
+      <c r="B676" s="28"/>
+      <c r="C676" s="22"/>
+      <c r="D676" s="22"/>
+      <c r="E676" s="22"/>
+      <c r="F676" s="22"/>
+      <c r="G676" s="22"/>
+      <c r="H676" s="22"/>
+    </row>
+    <row r="677" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A677" s="8">
+        <v>44139</v>
+      </c>
+      <c r="B677" s="28"/>
+      <c r="C677" s="22"/>
+      <c r="D677" s="22"/>
+      <c r="E677" s="22"/>
+      <c r="F677" s="22"/>
+      <c r="G677" s="22"/>
+      <c r="H677" s="22"/>
+    </row>
+    <row r="678" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A678" s="8">
+        <v>44140</v>
+      </c>
+      <c r="B678" s="28"/>
+      <c r="C678" s="22"/>
+      <c r="D678" s="22"/>
+      <c r="E678" s="22"/>
+      <c r="F678" s="22"/>
+      <c r="G678" s="22"/>
+      <c r="H678" s="22"/>
+    </row>
+    <row r="679" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A679" s="8">
+        <v>44141</v>
+      </c>
+      <c r="B679" s="28"/>
+      <c r="C679" s="22"/>
+      <c r="D679" s="22"/>
+      <c r="E679" s="22"/>
+      <c r="F679" s="22"/>
+      <c r="G679" s="22"/>
+      <c r="H679" s="22"/>
+    </row>
+    <row r="680" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A680" s="8">
+        <v>44142</v>
+      </c>
+      <c r="B680" s="28"/>
+      <c r="C680" s="22"/>
+      <c r="D680" s="22"/>
+      <c r="E680" s="22"/>
+      <c r="F680" s="22"/>
+      <c r="G680" s="22"/>
+      <c r="H680" s="22"/>
+    </row>
+    <row r="681" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A681" s="8">
+        <v>44143</v>
+      </c>
+      <c r="B681" s="28"/>
+      <c r="C681" s="22"/>
+      <c r="D681" s="22"/>
+      <c r="E681" s="22"/>
+      <c r="F681" s="22"/>
+      <c r="G681" s="22"/>
+      <c r="H681" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -14915,11 +15019,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R674"/>
+  <dimension ref="A1:R681"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A670" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B674" sqref="B674"/>
+      <pane ySplit="3" topLeftCell="A677" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A688" sqref="A688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30768,16 +30872,31 @@
       <c r="B668" s="27">
         <v>7.7798299999999996</v>
       </c>
+      <c r="E668" s="4">
+        <v>20.38</v>
+      </c>
+      <c r="F668" s="4">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="G668" s="4">
+        <v>14.99</v>
+      </c>
     </row>
     <row r="669" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A669" s="8">
         <v>44131</v>
       </c>
+      <c r="B669" s="4">
+        <v>7.7804200000000003</v>
+      </c>
     </row>
     <row r="670" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A670" s="8">
         <v>44132</v>
       </c>
+      <c r="B670" s="4">
+        <v>7.7861900000000004</v>
+      </c>
     </row>
     <row r="671" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A671" s="8">
@@ -30797,6 +30916,41 @@
     <row r="674" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A674" s="8">
         <v>44136</v>
+      </c>
+    </row>
+    <row r="675" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A675" s="8">
+        <v>44137</v>
+      </c>
+    </row>
+    <row r="676" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A676" s="8">
+        <v>44138</v>
+      </c>
+    </row>
+    <row r="677" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A677" s="8">
+        <v>44139</v>
+      </c>
+    </row>
+    <row r="678" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A678" s="8">
+        <v>44140</v>
+      </c>
+    </row>
+    <row r="679" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A679" s="8">
+        <v>44141</v>
+      </c>
+    </row>
+    <row r="680" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A680" s="8">
+        <v>44142</v>
+      </c>
+    </row>
+    <row r="681" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A681" s="8">
+        <v>44143</v>
       </c>
     </row>
   </sheetData>
@@ -30814,10 +30968,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-31-2020 02-24-18
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1532" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9BAB9805-5577-4FE4-AF18-AC63BE2D1541}"/>
+  <xr:revisionPtr revIDLastSave="1545" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F929190-B6FA-4790-B967-15E4D65D7E12}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1976,8 +1976,8 @@
   <dimension ref="A1:R681"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A672" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A688" sqref="A688"/>
+      <pane ySplit="3" topLeftCell="A673" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B681" sqref="B681"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14836,10 +14836,10 @@
         <v>24.343</v>
       </c>
       <c r="C669" s="22">
-        <v>106.98</v>
+        <v>106.95</v>
       </c>
       <c r="D669" s="22">
-        <v>14.89</v>
+        <v>14.83</v>
       </c>
       <c r="E669" s="22"/>
       <c r="F669" s="22"/>
@@ -14853,8 +14853,12 @@
       <c r="B670" s="28">
         <v>24.3277</v>
       </c>
-      <c r="C670" s="22"/>
-      <c r="D670" s="22"/>
+      <c r="C670" s="22">
+        <v>105</v>
+      </c>
+      <c r="D670" s="22">
+        <v>14.89</v>
+      </c>
       <c r="E670" s="22"/>
       <c r="F670" s="22"/>
       <c r="G670" s="22"/>
@@ -14864,9 +14868,15 @@
       <c r="A671" s="8">
         <v>44133</v>
       </c>
-      <c r="B671" s="28"/>
-      <c r="C671" s="22"/>
-      <c r="D671" s="22"/>
+      <c r="B671" s="28">
+        <v>24.324999999999999</v>
+      </c>
+      <c r="C671" s="22">
+        <v>104.38</v>
+      </c>
+      <c r="D671" s="22">
+        <v>14.39</v>
+      </c>
       <c r="E671" s="22"/>
       <c r="F671" s="22"/>
       <c r="G671" s="22"/>
@@ -14876,9 +14886,15 @@
       <c r="A672" s="8">
         <v>44134</v>
       </c>
-      <c r="B672" s="28"/>
-      <c r="C672" s="22"/>
-      <c r="D672" s="22"/>
+      <c r="B672" s="28">
+        <v>24.327300000000001</v>
+      </c>
+      <c r="C672" s="22">
+        <v>104.28</v>
+      </c>
+      <c r="D672" s="22">
+        <v>14.41</v>
+      </c>
       <c r="E672" s="22"/>
       <c r="F672" s="22"/>
       <c r="G672" s="22"/>
@@ -14920,7 +14936,9 @@
       <c r="A675" s="8">
         <v>44137</v>
       </c>
-      <c r="B675" s="28"/>
+      <c r="B675" s="28">
+        <v>24.326899999999998</v>
+      </c>
       <c r="C675" s="22"/>
       <c r="D675" s="22"/>
       <c r="E675" s="22"/>
@@ -15022,8 +15040,8 @@
   <dimension ref="A1:R681"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A677" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A688" sqref="A688"/>
+      <pane ySplit="3" topLeftCell="A674" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B681" sqref="B681"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30902,53 +30920,65 @@
       <c r="A671" s="8">
         <v>44133</v>
       </c>
+      <c r="B671" s="4">
+        <v>7.7916499999999997</v>
+      </c>
     </row>
     <row r="672" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A672" s="8">
         <v>44134</v>
       </c>
-    </row>
-    <row r="673" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B672" s="4">
+        <v>7.7959500000000004</v>
+      </c>
+    </row>
+    <row r="673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A673" s="8">
         <v>44135</v>
       </c>
-    </row>
-    <row r="674" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B673" s="27">
+        <v>7.7959500000000004</v>
+      </c>
+    </row>
+    <row r="674" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A674" s="8">
         <v>44136</v>
       </c>
-    </row>
-    <row r="675" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B674" s="27">
+        <v>7.7959500000000004</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A675" s="8">
         <v>44137</v>
       </c>
     </row>
-    <row r="676" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" s="8">
         <v>44138</v>
       </c>
     </row>
-    <row r="677" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A677" s="8">
         <v>44139</v>
       </c>
     </row>
-    <row r="678" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A678" s="8">
         <v>44140</v>
       </c>
     </row>
-    <row r="679" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A679" s="8">
         <v>44141</v>
       </c>
     </row>
-    <row r="680" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A680" s="8">
         <v>44142</v>
       </c>
     </row>
-    <row r="681" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A681" s="8">
         <v>44143</v>
       </c>
@@ -30968,7 +30998,7 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F27" sqref="F27"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-04-2020 02-39-05
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1545" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F929190-B6FA-4790-B967-15E4D65D7E12}"/>
+  <xr:revisionPtr revIDLastSave="1568" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{54160E96-C61E-4BF1-9C58-BE5A800BA027}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1604,8 +1604,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H681" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A3:H681" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_HN" displayName="Indicadores_dia_HN" ref="A3:H688" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A3:H688" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="TCR para el día (L por US$1.00)" dataDxfId="23"/>
@@ -1641,8 +1641,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H681" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:H681" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F6EB074-F734-4887-A912-97D45532A2DC}" name="Indicadores_dia_GT" displayName="Indicadores_dia_GT" ref="A3:H688" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:H688" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3C07F94B-5627-412C-BE11-8F3583459ECF}" name="Fecha" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EE5D7B7B-B3DE-4DF7-892D-A458246C4E6D}" name="TCR para el día (Q por US$1.00)"/>
@@ -1973,11 +1973,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R681"/>
+  <dimension ref="A1:R688"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A673" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B681" sqref="B681"/>
+      <pane ySplit="3" topLeftCell="A679" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A691" sqref="A691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4098,7 +4098,9 @@
         <v>5000</v>
       </c>
       <c r="Q48" s="27"/>
-      <c r="R48" s="27"/>
+      <c r="R48" s="27">
+        <v>536.1</v>
+      </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
@@ -14872,10 +14874,10 @@
         <v>24.324999999999999</v>
       </c>
       <c r="C671" s="22">
-        <v>104.38</v>
+        <v>104.6</v>
       </c>
       <c r="D671" s="22">
-        <v>14.39</v>
+        <v>14.4</v>
       </c>
       <c r="E671" s="22"/>
       <c r="F671" s="22"/>
@@ -14890,10 +14892,10 @@
         <v>24.327300000000001</v>
       </c>
       <c r="C672" s="22">
-        <v>104.28</v>
+        <v>104.4</v>
       </c>
       <c r="D672" s="22">
-        <v>14.41</v>
+        <v>14.36</v>
       </c>
       <c r="E672" s="22"/>
       <c r="F672" s="22"/>
@@ -14939,8 +14941,12 @@
       <c r="B675" s="28">
         <v>24.326899999999998</v>
       </c>
-      <c r="C675" s="22"/>
-      <c r="D675" s="22"/>
+      <c r="C675" s="22">
+        <v>102.8</v>
+      </c>
+      <c r="D675" s="22">
+        <v>14.97</v>
+      </c>
       <c r="E675" s="22"/>
       <c r="F675" s="22"/>
       <c r="G675" s="22"/>
@@ -14950,9 +14956,15 @@
       <c r="A676" s="8">
         <v>44138</v>
       </c>
-      <c r="B676" s="28"/>
-      <c r="C676" s="22"/>
-      <c r="D676" s="22"/>
+      <c r="B676" s="28">
+        <v>24.317599999999999</v>
+      </c>
+      <c r="C676" s="22">
+        <v>103.38</v>
+      </c>
+      <c r="D676" s="22">
+        <v>14.73</v>
+      </c>
       <c r="E676" s="22"/>
       <c r="F676" s="22"/>
       <c r="G676" s="22"/>
@@ -14962,7 +14974,9 @@
       <c r="A677" s="8">
         <v>44139</v>
       </c>
-      <c r="B677" s="28"/>
+      <c r="B677" s="28">
+        <v>24.308299999999999</v>
+      </c>
       <c r="C677" s="22"/>
       <c r="D677" s="22"/>
       <c r="E677" s="22"/>
@@ -15013,10 +15027,102 @@
       <c r="B681" s="28"/>
       <c r="C681" s="22"/>
       <c r="D681" s="22"/>
-      <c r="E681" s="22"/>
-      <c r="F681" s="22"/>
-      <c r="G681" s="22"/>
-      <c r="H681" s="22"/>
+      <c r="E681" s="22">
+        <v>80.58</v>
+      </c>
+      <c r="F681" s="22">
+        <v>74.069999999999993</v>
+      </c>
+      <c r="G681" s="22">
+        <v>61.88</v>
+      </c>
+      <c r="H681" s="22">
+        <v>42.77</v>
+      </c>
+    </row>
+    <row r="682" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A682" s="8">
+        <v>44144</v>
+      </c>
+      <c r="B682" s="28"/>
+      <c r="C682" s="22"/>
+      <c r="D682" s="22"/>
+      <c r="E682" s="22"/>
+      <c r="F682" s="22"/>
+      <c r="G682" s="22"/>
+      <c r="H682" s="22"/>
+    </row>
+    <row r="683" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A683" s="8">
+        <v>44145</v>
+      </c>
+      <c r="B683" s="28"/>
+      <c r="C683" s="22"/>
+      <c r="D683" s="22"/>
+      <c r="E683" s="22"/>
+      <c r="F683" s="22"/>
+      <c r="G683" s="22"/>
+      <c r="H683" s="22"/>
+    </row>
+    <row r="684" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A684" s="8">
+        <v>44146</v>
+      </c>
+      <c r="B684" s="28"/>
+      <c r="C684" s="22"/>
+      <c r="D684" s="22"/>
+      <c r="E684" s="22"/>
+      <c r="F684" s="22"/>
+      <c r="G684" s="22"/>
+      <c r="H684" s="22"/>
+    </row>
+    <row r="685" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A685" s="8">
+        <v>44147</v>
+      </c>
+      <c r="B685" s="28"/>
+      <c r="C685" s="22"/>
+      <c r="D685" s="22"/>
+      <c r="E685" s="22"/>
+      <c r="F685" s="22"/>
+      <c r="G685" s="22"/>
+      <c r="H685" s="22"/>
+    </row>
+    <row r="686" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A686" s="8">
+        <v>44148</v>
+      </c>
+      <c r="B686" s="28"/>
+      <c r="C686" s="22"/>
+      <c r="D686" s="22"/>
+      <c r="E686" s="22"/>
+      <c r="F686" s="22"/>
+      <c r="G686" s="22"/>
+      <c r="H686" s="22"/>
+    </row>
+    <row r="687" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A687" s="8">
+        <v>44149</v>
+      </c>
+      <c r="B687" s="28"/>
+      <c r="C687" s="22"/>
+      <c r="D687" s="22"/>
+      <c r="E687" s="22"/>
+      <c r="F687" s="22"/>
+      <c r="G687" s="22"/>
+      <c r="H687" s="22"/>
+    </row>
+    <row r="688" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A688" s="8">
+        <v>44150</v>
+      </c>
+      <c r="B688" s="28"/>
+      <c r="C688" s="22"/>
+      <c r="D688" s="22"/>
+      <c r="E688" s="22"/>
+      <c r="F688" s="22"/>
+      <c r="G688" s="22"/>
+      <c r="H688" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -15037,11 +15143,11 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R681"/>
+  <dimension ref="A1:R688"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A674" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B681" sqref="B681"/>
+      <pane ySplit="3" topLeftCell="A680" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B690" sqref="B690"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17382,7 +17488,9 @@
         <v>176.67</v>
       </c>
       <c r="Q48" s="27"/>
-      <c r="R48" s="27"/>
+      <c r="R48" s="27">
+        <v>1050.2</v>
+      </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
@@ -30952,16 +31060,25 @@
       <c r="A675" s="8">
         <v>44137</v>
       </c>
+      <c r="B675" s="27">
+        <v>7.7959500000000004</v>
+      </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" s="8">
         <v>44138</v>
       </c>
+      <c r="B676" s="4">
+        <v>7.7885799999999996</v>
+      </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A677" s="8">
         <v>44139</v>
       </c>
+      <c r="B677" s="4">
+        <v>7.7860199999999997</v>
+      </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A678" s="8">
@@ -30981,6 +31098,41 @@
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A681" s="8">
         <v>44143</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A682" s="8">
+        <v>44144</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A683" s="8">
+        <v>44145</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A684" s="8">
+        <v>44146</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A685" s="8">
+        <v>44147</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686" s="8">
+        <v>44148</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687" s="8">
+        <v>44149</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688" s="8">
+        <v>44150</v>
       </c>
     </row>
   </sheetData>
@@ -30998,10 +31150,10 @@
   <dimension ref="A1:Y972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-11-2020 22-35-29
</commit_message>
<xml_diff>
--- a/datacovidgt/ECONOMICOS HN Y GT.xlsx
+++ b/datacovidgt/ECONOMICOS HN Y GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1568" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{54160E96-C61E-4BF1-9C58-BE5A800BA027}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{BB75621D-B0B6-4649-B515-C7FE02111ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1976,7 +1976,7 @@
   <dimension ref="A1:R688"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A679" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A682" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A691" sqref="A691"/>
     </sheetView>
   </sheetViews>

</xml_diff>